<commit_message>
Added Rep2 for Third_Plate
</commit_message>
<xml_diff>
--- a/data/Results_Masterfile.xlsx
+++ b/data/Results_Masterfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOL428\Documents\GitHub\SynBioMLMH\SynbioML\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D89A9F-6F9B-4CD3-99E7-EB2CAABF0002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDD41A5-48CA-4CCC-850E-914DBDD6457B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2739" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="661">
   <si>
     <t>RBS</t>
   </si>
@@ -2548,8 +2548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P269"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O182" sqref="O182"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F189" sqref="F189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2560,7 +2560,7 @@
     <col min="11" max="11" width="9.1796875" customWidth="1"/>
     <col min="12" max="12" width="10.81640625" customWidth="1"/>
     <col min="13" max="14" width="8.81640625" customWidth="1"/>
-    <col min="15" max="15" width="23.36328125" customWidth="1"/>
+    <col min="15" max="15" width="13.36328125" customWidth="1"/>
     <col min="17" max="17" width="9.1796875" customWidth="1"/>
     <col min="18" max="18" width="10.54296875" customWidth="1"/>
     <col min="19" max="1025" width="9.1796875" customWidth="1"/>
@@ -12054,17 +12054,20 @@
       <c r="C180">
         <v>19.20331081932234</v>
       </c>
+      <c r="D180">
+        <v>24.453626711267411</v>
+      </c>
       <c r="I180">
         <f t="shared" ref="I180:I243" si="18">AVERAGE(C180:H180)</f>
-        <v>19.20331081932234</v>
+        <v>21.828468765294875</v>
       </c>
       <c r="J180">
         <f t="shared" ref="J180:J243" si="19">_xlfn.STDEV.P(C180:H180)</f>
-        <v>0</v>
+        <v>2.6251579459725405</v>
       </c>
       <c r="K180" s="6">
         <f t="shared" ref="K180:K243" si="20">J180/I180</f>
-        <v>0</v>
+        <v>0.12026303696328366</v>
       </c>
       <c r="L180" t="s">
         <v>660</v>
@@ -12089,17 +12092,20 @@
       <c r="C181">
         <v>17.610238008659859</v>
       </c>
+      <c r="D181">
+        <v>24.14740489760085</v>
+      </c>
       <c r="I181">
         <f t="shared" si="18"/>
-        <v>17.610238008659859</v>
+        <v>20.878821453130357</v>
       </c>
       <c r="J181">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>3.2685834444704827</v>
       </c>
       <c r="K181" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.15655018899452414</v>
       </c>
       <c r="L181" t="s">
         <v>660</v>
@@ -12124,17 +12130,20 @@
       <c r="C182">
         <v>19.1398619685645</v>
       </c>
+      <c r="D182">
+        <v>23.017435589334902</v>
+      </c>
       <c r="I182">
         <f t="shared" si="18"/>
-        <v>19.1398619685645</v>
+        <v>21.078648778949699</v>
       </c>
       <c r="J182">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.9387868103852011</v>
       </c>
       <c r="K182" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>9.1978704646446807E-2</v>
       </c>
       <c r="L182" t="s">
         <v>660</v>
@@ -12159,17 +12168,20 @@
       <c r="C183">
         <v>17.75236657101177</v>
       </c>
+      <c r="D183">
+        <v>18.515949336571961</v>
+      </c>
       <c r="I183">
         <f t="shared" si="18"/>
-        <v>17.75236657101177</v>
+        <v>18.134157953791863</v>
       </c>
       <c r="J183">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.38179138278009539</v>
       </c>
       <c r="K183" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.1053714418554657E-2</v>
       </c>
       <c r="L183" t="s">
         <v>660</v>
@@ -12194,17 +12206,20 @@
       <c r="C184">
         <v>17.372920501433001</v>
       </c>
+      <c r="D184">
+        <v>16.256351764188611</v>
+      </c>
       <c r="I184">
         <f t="shared" si="18"/>
-        <v>17.372920501433001</v>
+        <v>16.814636132810804</v>
       </c>
       <c r="J184">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.55828436862219455</v>
       </c>
       <c r="K184" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>3.3202286639602077E-2</v>
       </c>
       <c r="L184" t="s">
         <v>660</v>
@@ -12229,17 +12244,20 @@
       <c r="C185">
         <v>16.17888348298991</v>
       </c>
+      <c r="D185">
+        <v>18.339535870145909</v>
+      </c>
       <c r="I185">
         <f t="shared" si="18"/>
-        <v>16.17888348298991</v>
+        <v>17.259209676567909</v>
       </c>
       <c r="J185">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.0803261935779993</v>
       </c>
       <c r="K185" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>6.2594186745683497E-2</v>
       </c>
       <c r="L185" t="s">
         <v>660</v>
@@ -12264,17 +12282,20 @@
       <c r="C186">
         <v>17.71881140290003</v>
       </c>
+      <c r="D186">
+        <v>17.674828192863639</v>
+      </c>
       <c r="I186">
         <f t="shared" si="18"/>
-        <v>17.71881140290003</v>
+        <v>17.696819797881837</v>
       </c>
       <c r="J186">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2.1991605018195415E-2</v>
       </c>
       <c r="K186" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1.2426868369212658E-3</v>
       </c>
       <c r="L186" t="s">
         <v>660</v>
@@ -12299,17 +12320,20 @@
       <c r="C187">
         <v>19.652989292439042</v>
       </c>
+      <c r="D187">
+        <v>20.13079756464824</v>
+      </c>
       <c r="I187">
         <f t="shared" si="18"/>
-        <v>19.652989292439042</v>
+        <v>19.891893428543639</v>
       </c>
       <c r="J187">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.23890413610459937</v>
       </c>
       <c r="K187" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1.2010125479648241E-2</v>
       </c>
       <c r="L187" t="s">
         <v>660</v>
@@ -12334,17 +12358,20 @@
       <c r="C188">
         <v>17.120631805364631</v>
       </c>
+      <c r="D188">
+        <v>16.691212955283071</v>
+      </c>
       <c r="I188">
         <f t="shared" si="18"/>
-        <v>17.120631805364631</v>
+        <v>16.905922380323851</v>
       </c>
       <c r="J188">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.21470942504078039</v>
       </c>
       <c r="K188" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1.2700249073110166E-2</v>
       </c>
       <c r="L188" t="s">
         <v>660</v>
@@ -12369,17 +12396,20 @@
       <c r="C189">
         <v>16.19152959007284</v>
       </c>
+      <c r="D189">
+        <v>16.020762960507231</v>
+      </c>
       <c r="I189">
         <f t="shared" si="18"/>
-        <v>16.19152959007284</v>
+        <v>16.106146275290037</v>
       </c>
       <c r="J189">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>8.5383314782804476E-2</v>
       </c>
       <c r="K189" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.3012876775991469E-3</v>
       </c>
       <c r="L189" t="s">
         <v>660</v>
@@ -12404,17 +12434,20 @@
       <c r="C190">
         <v>16.969707070775691</v>
       </c>
+      <c r="D190">
+        <v>15.01080166188494</v>
+      </c>
       <c r="I190">
         <f t="shared" si="18"/>
-        <v>16.969707070775691</v>
+        <v>15.990254366330316</v>
       </c>
       <c r="J190">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.97945270444537513</v>
       </c>
       <c r="K190" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>6.1253103422028596E-2</v>
       </c>
       <c r="L190" t="s">
         <v>660</v>
@@ -12439,17 +12472,20 @@
       <c r="C191">
         <v>19.347722394075479</v>
       </c>
+      <c r="D191">
+        <v>18.571164605712209</v>
+      </c>
       <c r="I191">
         <f t="shared" si="18"/>
-        <v>19.347722394075479</v>
+        <v>18.959443499893844</v>
       </c>
       <c r="J191">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.38827889418163508</v>
       </c>
       <c r="K191" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.0479445727603192E-2</v>
       </c>
       <c r="L191" t="s">
         <v>660</v>
@@ -12474,17 +12510,20 @@
       <c r="C192">
         <v>34.039694513566737</v>
       </c>
+      <c r="D192">
+        <v>34.920384109409589</v>
+      </c>
       <c r="I192">
         <f t="shared" si="18"/>
-        <v>34.039694513566737</v>
+        <v>34.480039311488163</v>
       </c>
       <c r="J192">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.44034479792142633</v>
       </c>
       <c r="K192" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1.2771006260851649E-2</v>
       </c>
       <c r="L192" t="s">
         <v>660</v>
@@ -12509,17 +12548,20 @@
       <c r="C193">
         <v>15.225148884430441</v>
       </c>
+      <c r="D193">
+        <v>18.42129817654267</v>
+      </c>
       <c r="I193">
         <f t="shared" si="18"/>
-        <v>15.225148884430441</v>
+        <v>16.823223530486555</v>
       </c>
       <c r="J193">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.5980746460561146</v>
       </c>
       <c r="K193" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>9.4992178113791945E-2</v>
       </c>
       <c r="L193" t="s">
         <v>660</v>
@@ -12544,17 +12586,20 @@
       <c r="C194">
         <v>8.9546779243415653</v>
       </c>
+      <c r="D194">
+        <v>15.09112251057871</v>
+      </c>
       <c r="I194">
         <f t="shared" si="18"/>
-        <v>8.9546779243415653</v>
+        <v>12.022900217460137</v>
       </c>
       <c r="J194">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>3.0682222931185765</v>
       </c>
       <c r="K194" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.25519818326885729</v>
       </c>
       <c r="L194" t="s">
         <v>660</v>
@@ -12579,17 +12624,20 @@
       <c r="C195">
         <v>12.04222552272264</v>
       </c>
+      <c r="D195">
+        <v>14.57827132562549</v>
+      </c>
       <c r="I195">
         <f t="shared" si="18"/>
-        <v>12.04222552272264</v>
+        <v>13.310248424174066</v>
       </c>
       <c r="J195">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.2680229014514248</v>
       </c>
       <c r="K195" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>9.5266659271996929E-2</v>
       </c>
       <c r="L195" t="s">
         <v>660</v>
@@ -12614,17 +12662,20 @@
       <c r="C196">
         <v>14.8982025842705</v>
       </c>
+      <c r="D196">
+        <v>15.53046337302092</v>
+      </c>
       <c r="I196">
         <f t="shared" si="18"/>
-        <v>14.8982025842705</v>
+        <v>15.214332978645711</v>
       </c>
       <c r="J196">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.31613039437521007</v>
       </c>
       <c r="K196" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.0778459024061016E-2</v>
       </c>
       <c r="L196" t="s">
         <v>660</v>
@@ -12649,17 +12700,20 @@
       <c r="C197">
         <v>9.8111139227566984</v>
       </c>
+      <c r="D197">
+        <v>10.297011062925691</v>
+      </c>
       <c r="I197">
         <f t="shared" si="18"/>
-        <v>9.8111139227566984</v>
+        <v>10.054062492841194</v>
       </c>
       <c r="J197">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.24294857008449622</v>
       </c>
       <c r="K197" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.4164219215613906E-2</v>
       </c>
       <c r="L197" t="s">
         <v>660</v>
@@ -12684,17 +12738,20 @@
       <c r="C198">
         <v>9.5640862524991537</v>
       </c>
+      <c r="D198">
+        <v>10.7921879787532</v>
+      </c>
       <c r="I198">
         <f t="shared" si="18"/>
-        <v>9.5640862524991537</v>
+        <v>10.178137115626177</v>
       </c>
       <c r="J198">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.61405086312702295</v>
       </c>
       <c r="K198" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>6.0330378354236339E-2</v>
       </c>
       <c r="L198" t="s">
         <v>660</v>
@@ -12719,17 +12776,20 @@
       <c r="C199">
         <v>7.9381651868506324</v>
       </c>
+      <c r="D199">
+        <v>8.4463036475557072</v>
+      </c>
       <c r="I199">
         <f t="shared" si="18"/>
-        <v>7.9381651868506324</v>
+        <v>8.1922344172031707</v>
       </c>
       <c r="J199">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.25406923035253737</v>
       </c>
       <c r="K199" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>3.1013422884849116E-2</v>
       </c>
       <c r="L199" t="s">
         <v>660</v>
@@ -12754,17 +12814,20 @@
       <c r="C200">
         <v>12.80966436996504</v>
       </c>
+      <c r="D200">
+        <v>11.653105644297829</v>
+      </c>
       <c r="I200">
         <f t="shared" si="18"/>
-        <v>12.80966436996504</v>
+        <v>12.231385007131435</v>
       </c>
       <c r="J200">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.57827936283360515</v>
       </c>
       <c r="K200" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>4.7278322323795946E-2</v>
       </c>
       <c r="L200" t="s">
         <v>660</v>
@@ -12789,17 +12852,20 @@
       <c r="C201">
         <v>14.44686016263555</v>
       </c>
+      <c r="D201">
+        <v>9.5546871914631684</v>
+      </c>
       <c r="I201">
         <f t="shared" si="18"/>
-        <v>14.44686016263555</v>
+        <v>12.000773677049359</v>
       </c>
       <c r="J201">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2.4460864855861946</v>
       </c>
       <c r="K201" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.20382739908379108</v>
       </c>
       <c r="L201" t="s">
         <v>660</v>
@@ -12824,17 +12890,20 @@
       <c r="C202">
         <v>14.44908288400034</v>
       </c>
+      <c r="D202">
+        <v>9.2735077546288043</v>
+      </c>
       <c r="I202">
         <f t="shared" si="18"/>
-        <v>14.44908288400034</v>
+        <v>11.861295319314571</v>
       </c>
       <c r="J202">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2.5877875646857751</v>
       </c>
       <c r="K202" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.21817073894719582</v>
       </c>
       <c r="L202" t="s">
         <v>660</v>
@@ -12859,17 +12928,20 @@
       <c r="C203">
         <v>19.522553044213691</v>
       </c>
+      <c r="D203">
+        <v>15.91659144304214</v>
+      </c>
       <c r="I203">
         <f t="shared" si="18"/>
-        <v>19.522553044213691</v>
+        <v>17.719572243627915</v>
       </c>
       <c r="J203">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.8029808005857819</v>
       </c>
       <c r="K203" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.10175080841661664</v>
       </c>
       <c r="L203" t="s">
         <v>660</v>
@@ -12894,17 +12966,20 @@
       <c r="C204">
         <v>14.942633386412631</v>
       </c>
+      <c r="D204">
+        <v>19.473140312346569</v>
+      </c>
       <c r="I204">
         <f t="shared" si="18"/>
-        <v>14.942633386412631</v>
+        <v>17.207886849379598</v>
       </c>
       <c r="J204">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2.2652534629669732</v>
       </c>
       <c r="K204" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.13164042062774506</v>
       </c>
       <c r="L204" t="s">
         <v>660</v>
@@ -12929,17 +13004,20 @@
       <c r="C205">
         <v>6.5696337866293506</v>
       </c>
+      <c r="D205">
+        <v>12.68408732550512</v>
+      </c>
       <c r="I205">
         <f t="shared" si="18"/>
-        <v>6.5696337866293506</v>
+        <v>9.6268605560672356</v>
       </c>
       <c r="J205">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>3.0572267694378841</v>
       </c>
       <c r="K205" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.31757256185777993</v>
       </c>
       <c r="L205" t="s">
         <v>660</v>
@@ -12964,17 +13042,20 @@
       <c r="C206">
         <v>17.437438573542661</v>
       </c>
+      <c r="D206">
+        <v>19.1883242770866</v>
+      </c>
       <c r="I206">
         <f t="shared" si="18"/>
-        <v>17.437438573542661</v>
+        <v>18.312881425314629</v>
       </c>
       <c r="J206">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.8754428517719699</v>
       </c>
       <c r="K206" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>4.7804757287502019E-2</v>
       </c>
       <c r="L206" t="s">
         <v>660</v>
@@ -12999,17 +13080,20 @@
       <c r="C207">
         <v>13.073256482008009</v>
       </c>
+      <c r="D207">
+        <v>9.1470579100474421</v>
+      </c>
       <c r="I207">
         <f t="shared" si="18"/>
-        <v>13.073256482008009</v>
+        <v>11.110157196027725</v>
       </c>
       <c r="J207">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.9630992859802869</v>
       </c>
       <c r="K207" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.17669410534372679</v>
       </c>
       <c r="L207" t="s">
         <v>660</v>
@@ -13034,17 +13118,20 @@
       <c r="C208">
         <v>8.3703605277557802</v>
       </c>
+      <c r="D208">
+        <v>9.3173162797921556</v>
+      </c>
       <c r="I208">
         <f t="shared" si="18"/>
-        <v>8.3703605277557802</v>
+        <v>8.8438384037739688</v>
       </c>
       <c r="J208">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.47347787601818769</v>
       </c>
       <c r="K208" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.3537599218924946E-2</v>
       </c>
       <c r="L208" t="s">
         <v>660</v>
@@ -13069,17 +13156,20 @@
       <c r="C209">
         <v>11.70761630893251</v>
       </c>
+      <c r="D209">
+        <v>8.0191434188848998</v>
+      </c>
       <c r="I209">
         <f t="shared" si="18"/>
-        <v>11.70761630893251</v>
+        <v>9.8633798639087047</v>
       </c>
       <c r="J209">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.8442364450238038</v>
       </c>
       <c r="K209" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.18697814242885313</v>
       </c>
       <c r="L209" t="s">
         <v>660</v>
@@ -13104,17 +13194,20 @@
       <c r="C210">
         <v>8.6285580759081952</v>
       </c>
+      <c r="D210">
+        <v>7.6474175616034641</v>
+      </c>
       <c r="I210">
         <f t="shared" si="18"/>
-        <v>8.6285580759081952</v>
+        <v>8.1379878187558301</v>
       </c>
       <c r="J210">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.49057025715236557</v>
       </c>
       <c r="K210" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>6.0281517750829718E-2</v>
       </c>
       <c r="L210" t="s">
         <v>660</v>
@@ -13139,17 +13232,20 @@
       <c r="C211">
         <v>10.965726308967451</v>
       </c>
+      <c r="D211">
+        <v>6.9313003325357752</v>
+      </c>
       <c r="I211">
         <f t="shared" si="18"/>
-        <v>10.965726308967451</v>
+        <v>8.9485133207516121</v>
       </c>
       <c r="J211">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2.0172129882158423</v>
       </c>
       <c r="K211" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.2254243711676579</v>
       </c>
       <c r="L211" t="s">
         <v>660</v>
@@ -13174,17 +13270,20 @@
       <c r="C212">
         <v>10.37895798517688</v>
       </c>
+      <c r="D212">
+        <v>9.3094906507977733</v>
+      </c>
       <c r="I212">
         <f t="shared" si="18"/>
-        <v>10.37895798517688</v>
+        <v>9.8442243179873259</v>
       </c>
       <c r="J212">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.53473366718955351</v>
       </c>
       <c r="K212" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.4319532948115611E-2</v>
       </c>
       <c r="L212" t="s">
         <v>660</v>
@@ -13209,17 +13308,20 @@
       <c r="C213">
         <v>12.31632351975867</v>
       </c>
+      <c r="D213">
+        <v>5.8002804003794557</v>
+      </c>
       <c r="I213">
         <f t="shared" si="18"/>
-        <v>12.31632351975867</v>
+        <v>9.0583019600690626</v>
       </c>
       <c r="J213">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>3.2580215596896083</v>
       </c>
       <c r="K213" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.35967243905664281</v>
       </c>
       <c r="L213" t="s">
         <v>660</v>
@@ -13244,17 +13346,20 @@
       <c r="C214">
         <v>12.016030847483901</v>
       </c>
+      <c r="D214">
+        <v>5.2805371133292018</v>
+      </c>
       <c r="I214">
         <f t="shared" si="18"/>
-        <v>12.016030847483901</v>
+        <v>8.6482839804065517</v>
       </c>
       <c r="J214">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>3.3677468670773472</v>
       </c>
       <c r="K214" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.38941215097784415</v>
       </c>
       <c r="L214" t="s">
         <v>660</v>
@@ -13279,17 +13384,20 @@
       <c r="C215">
         <v>19.4231503304322</v>
       </c>
+      <c r="D215">
+        <v>16.039160167671579</v>
+      </c>
       <c r="I215">
         <f t="shared" si="18"/>
-        <v>19.4231503304322</v>
+        <v>17.731155249051888</v>
       </c>
       <c r="J215">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.6919950813803106</v>
       </c>
       <c r="K215" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>9.5424976974965256E-2</v>
       </c>
       <c r="L215" t="s">
         <v>660</v>
@@ -13314,17 +13422,20 @@
       <c r="C216">
         <v>26.395147649722691</v>
       </c>
+      <c r="D216">
+        <v>26.0843625985774</v>
+      </c>
       <c r="I216">
         <f t="shared" si="18"/>
-        <v>26.395147649722691</v>
+        <v>26.239755124150044</v>
       </c>
       <c r="J216">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.15539252557264582</v>
       </c>
       <c r="K216" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.9220265142500752E-3</v>
       </c>
       <c r="L216" t="s">
         <v>660</v>
@@ -13349,17 +13460,20 @@
       <c r="C217">
         <v>9.3910912840599234</v>
       </c>
+      <c r="D217">
+        <v>14.674130390916631</v>
+      </c>
       <c r="I217">
         <f t="shared" si="18"/>
-        <v>9.3910912840599234</v>
+        <v>12.032610837488278</v>
       </c>
       <c r="J217">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2.6415195534283509</v>
       </c>
       <c r="K217" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.21953004124412864</v>
       </c>
       <c r="L217" t="s">
         <v>660</v>
@@ -13384,17 +13498,20 @@
       <c r="C218">
         <v>9.4813968060510625</v>
       </c>
+      <c r="D218">
+        <v>10.61968030298668</v>
+      </c>
       <c r="I218">
         <f t="shared" si="18"/>
-        <v>9.4813968060510625</v>
+        <v>10.050538554518871</v>
       </c>
       <c r="J218">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.56914174846780874</v>
       </c>
       <c r="K218" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.6627985195073366E-2</v>
       </c>
       <c r="L218" t="s">
         <v>660</v>
@@ -13419,17 +13536,20 @@
       <c r="C219">
         <v>7.074900757346847</v>
       </c>
+      <c r="D219">
+        <v>10.34063893592457</v>
+      </c>
       <c r="I219">
         <f t="shared" si="18"/>
-        <v>7.074900757346847</v>
+        <v>8.7077698466357081</v>
       </c>
       <c r="J219">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.6328690892888644</v>
       </c>
       <c r="K219" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.18751863198586166</v>
       </c>
       <c r="L219" t="s">
         <v>660</v>
@@ -13454,17 +13574,20 @@
       <c r="C220">
         <v>7.7722592551717469</v>
       </c>
+      <c r="D220">
+        <v>5.7289057209809782</v>
+      </c>
       <c r="I220">
         <f t="shared" si="18"/>
-        <v>7.7722592551717469</v>
+        <v>6.750582488076363</v>
       </c>
       <c r="J220">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.021676767095381</v>
       </c>
       <c r="K220" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.15134646067950155</v>
       </c>
       <c r="L220" t="s">
         <v>660</v>
@@ -13489,17 +13612,20 @@
       <c r="C221">
         <v>4.7455167469007424</v>
       </c>
+      <c r="D221">
+        <v>7.8130307495477336</v>
+      </c>
       <c r="I221">
         <f t="shared" si="18"/>
-        <v>4.7455167469007424</v>
+        <v>6.279273748224238</v>
       </c>
       <c r="J221">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.5337570013234969</v>
       </c>
       <c r="K221" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.24425706902127645</v>
       </c>
       <c r="L221" t="s">
         <v>660</v>
@@ -13524,17 +13650,20 @@
       <c r="C222">
         <v>9.252310501261185</v>
       </c>
+      <c r="D222">
+        <v>10.3452794145442</v>
+      </c>
       <c r="I222">
         <f t="shared" si="18"/>
-        <v>9.252310501261185</v>
+        <v>9.7987949579026932</v>
       </c>
       <c r="J222">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.54648445664150724</v>
       </c>
       <c r="K222" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.5770577809750928E-2</v>
       </c>
       <c r="L222" t="s">
         <v>660</v>
@@ -13559,17 +13688,20 @@
       <c r="C223">
         <v>9.8119613923544389</v>
       </c>
+      <c r="D223">
+        <v>10.27544101250262</v>
+      </c>
       <c r="I223">
         <f t="shared" si="18"/>
-        <v>9.8119613923544389</v>
+        <v>10.043701202428529</v>
       </c>
       <c r="J223">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.23173981007409061</v>
       </c>
       <c r="K223" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3073148573760516E-2</v>
       </c>
       <c r="L223" t="s">
         <v>660</v>
@@ -13594,17 +13726,20 @@
       <c r="C224">
         <v>9.7355120454435546</v>
       </c>
+      <c r="D224">
+        <v>4.9385335066367304</v>
+      </c>
       <c r="I224">
         <f t="shared" si="18"/>
-        <v>9.7355120454435546</v>
+        <v>7.3370227760401425</v>
       </c>
       <c r="J224">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2.398489269403413</v>
       </c>
       <c r="K224" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.32690225212819896</v>
       </c>
       <c r="L224" t="s">
         <v>660</v>
@@ -13629,17 +13764,20 @@
       <c r="C225">
         <v>10.559782435926969</v>
       </c>
+      <c r="D225">
+        <v>8.2930813172369469</v>
+      </c>
       <c r="I225">
         <f t="shared" si="18"/>
-        <v>10.559782435926969</v>
+        <v>9.4264318765819581</v>
       </c>
       <c r="J225">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.1333505593450106</v>
       </c>
       <c r="K225" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.12023113031353765</v>
       </c>
       <c r="L225" t="s">
         <v>660</v>
@@ -13664,17 +13802,20 @@
       <c r="C226">
         <v>11.201062028641291</v>
       </c>
+      <c r="D226">
+        <v>5.6389728802921812</v>
+      </c>
       <c r="I226">
         <f t="shared" si="18"/>
-        <v>11.201062028641291</v>
+        <v>8.4200174544667359</v>
       </c>
       <c r="J226">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2.781044574174556</v>
       </c>
       <c r="K226" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.33028964479156031</v>
       </c>
       <c r="L226" t="s">
         <v>660</v>
@@ -13699,17 +13840,20 @@
       <c r="C227">
         <v>19.105961998307599</v>
       </c>
+      <c r="D227">
+        <v>14.183453856141499</v>
+      </c>
       <c r="I227">
         <f t="shared" si="18"/>
-        <v>19.105961998307599</v>
+        <v>16.644707927224548</v>
       </c>
       <c r="J227">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2.4612540710830446</v>
       </c>
       <c r="K227" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.14787006668091476</v>
       </c>
       <c r="L227" t="s">
         <v>660</v>
@@ -13734,17 +13878,20 @@
       <c r="C228">
         <v>14.489223183503549</v>
       </c>
+      <c r="D228">
+        <v>17.756224693214339</v>
+      </c>
       <c r="I228">
         <f t="shared" si="18"/>
-        <v>14.489223183503549</v>
+        <v>16.122723938358945</v>
       </c>
       <c r="J228">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.6335007548553784</v>
       </c>
       <c r="K228" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.10131667335498921</v>
       </c>
       <c r="L228" t="s">
         <v>660</v>
@@ -13769,17 +13916,20 @@
       <c r="C229">
         <v>7.0631268894668233</v>
       </c>
+      <c r="D229">
+        <v>11.556763088733909</v>
+      </c>
       <c r="I229">
         <f t="shared" si="18"/>
-        <v>7.0631268894668233</v>
+        <v>9.3099449891003658</v>
       </c>
       <c r="J229">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2.2468180996335443</v>
       </c>
       <c r="K229" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.24133527128935889</v>
       </c>
       <c r="L229" t="s">
         <v>660</v>
@@ -13804,17 +13954,20 @@
       <c r="C230">
         <v>5.4832606272799476</v>
       </c>
+      <c r="D230">
+        <v>1.976737914860593</v>
+      </c>
       <c r="I230">
         <f t="shared" si="18"/>
-        <v>5.4832606272799476</v>
+        <v>3.7299992710702705</v>
       </c>
       <c r="J230">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.753261356209677</v>
       </c>
       <c r="K230" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.47004335089497312</v>
       </c>
       <c r="L230" t="s">
         <v>660</v>
@@ -13839,17 +13992,20 @@
       <c r="C231">
         <v>9.1609659005114885</v>
       </c>
+      <c r="D231">
+        <v>6.9249517225862016</v>
+      </c>
       <c r="I231">
         <f t="shared" si="18"/>
-        <v>9.1609659005114885</v>
+        <v>8.0429588115488446</v>
       </c>
       <c r="J231">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.1180070889626477</v>
       </c>
       <c r="K231" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.13900445285848123</v>
       </c>
       <c r="L231" t="s">
         <v>660</v>
@@ -13874,17 +14030,20 @@
       <c r="C232">
         <v>8.146574943674505</v>
       </c>
+      <c r="D232">
+        <v>8.1003136442443573</v>
+      </c>
       <c r="I232">
         <f t="shared" si="18"/>
-        <v>8.146574943674505</v>
+        <v>8.1234442939594302</v>
       </c>
       <c r="J232">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2.3130649715073837E-2</v>
       </c>
       <c r="K232" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.8473943906125779E-3</v>
       </c>
       <c r="L232" t="s">
         <v>660</v>
@@ -13909,17 +14068,20 @@
       <c r="C233">
         <v>20.23617447392796</v>
       </c>
+      <c r="D233">
+        <v>20.15876485798406</v>
+      </c>
       <c r="I233">
         <f t="shared" si="18"/>
-        <v>20.23617447392796</v>
+        <v>20.19746966595601</v>
       </c>
       <c r="J233">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>3.8704807971949862E-2</v>
       </c>
       <c r="K233" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1.9163196485542458E-3</v>
       </c>
       <c r="L233" t="s">
         <v>660</v>
@@ -13944,17 +14106,20 @@
       <c r="C234">
         <v>5.5158107127912368</v>
       </c>
+      <c r="D234">
+        <v>1.7300464501596631</v>
+      </c>
       <c r="I234">
         <f t="shared" si="18"/>
-        <v>5.5158107127912368</v>
+        <v>3.6229285814754499</v>
       </c>
       <c r="J234">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.8928821313157869</v>
       </c>
       <c r="K234" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.52247293556775121</v>
       </c>
       <c r="L234" t="s">
         <v>660</v>
@@ -13979,17 +14144,20 @@
       <c r="C235">
         <v>9.5330155437996886</v>
       </c>
+      <c r="D235">
+        <v>6.6658752359786124</v>
+      </c>
       <c r="I235">
         <f t="shared" si="18"/>
-        <v>9.5330155437996886</v>
+        <v>8.0994453898891514</v>
       </c>
       <c r="J235">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.433570153910533</v>
       </c>
       <c r="K235" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.17699608860874766</v>
       </c>
       <c r="L235" t="s">
         <v>660</v>
@@ -14014,17 +14182,20 @@
       <c r="C236">
         <v>9.9467610660466352</v>
       </c>
+      <c r="D236">
+        <v>5.3987500660167722</v>
+      </c>
       <c r="I236">
         <f t="shared" si="18"/>
-        <v>9.9467610660466352</v>
+        <v>7.6727555660317037</v>
       </c>
       <c r="J236">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2.2740055000149324</v>
       </c>
       <c r="K236" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.2963740315255517</v>
       </c>
       <c r="L236" t="s">
         <v>660</v>
@@ -14049,17 +14220,20 @@
       <c r="C237">
         <v>10.821015969241479</v>
       </c>
+      <c r="D237">
+        <v>9.8035298088473741</v>
+      </c>
       <c r="I237">
         <f t="shared" si="18"/>
-        <v>10.821015969241479</v>
+        <v>10.312272889044426</v>
       </c>
       <c r="J237">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.5087430801970525</v>
       </c>
       <c r="K237" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>4.9333748793394715E-2</v>
       </c>
       <c r="L237" t="s">
         <v>660</v>
@@ -14084,17 +14258,20 @@
       <c r="C238">
         <v>11.535747559879031</v>
       </c>
+      <c r="D238">
+        <v>10.57359027540835</v>
+      </c>
       <c r="I238">
         <f t="shared" si="18"/>
-        <v>11.535747559879031</v>
+        <v>11.05466891764369</v>
       </c>
       <c r="J238">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.48107864223534058</v>
       </c>
       <c r="K238" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>4.3518141141931442E-2</v>
       </c>
       <c r="L238" t="s">
         <v>660</v>
@@ -14119,17 +14296,20 @@
       <c r="C239">
         <v>22.933192341731448</v>
       </c>
+      <c r="D239">
+        <v>18.053515904748231</v>
+      </c>
       <c r="I239">
         <f t="shared" si="18"/>
-        <v>22.933192341731448</v>
+        <v>20.49335412323984</v>
       </c>
       <c r="J239">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2.4398382184916043</v>
       </c>
       <c r="K239" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.1190550948282684</v>
       </c>
       <c r="L239" t="s">
         <v>660</v>
@@ -14154,17 +14334,20 @@
       <c r="C240">
         <v>14.677961186482911</v>
       </c>
+      <c r="D240">
+        <v>16.924663081946729</v>
+      </c>
       <c r="I240">
         <f t="shared" si="18"/>
-        <v>14.677961186482911</v>
+        <v>15.80131213421482</v>
       </c>
       <c r="J240">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.1233509477319092</v>
       </c>
       <c r="K240" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7.1092257287893229E-2</v>
       </c>
       <c r="L240" t="s">
         <v>660</v>
@@ -14189,17 +14372,20 @@
       <c r="C241">
         <v>9.7291181683601557</v>
       </c>
+      <c r="D241">
+        <v>12.714805545128421</v>
+      </c>
       <c r="I241">
         <f t="shared" si="18"/>
-        <v>9.7291181683601557</v>
+        <v>11.221961856744288</v>
       </c>
       <c r="J241">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1.4928436883841349</v>
       </c>
       <c r="K241" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.13302876158743585</v>
       </c>
       <c r="L241" t="s">
         <v>660</v>
@@ -14224,17 +14410,20 @@
       <c r="C242">
         <v>2.577360826054544</v>
       </c>
+      <c r="D242">
+        <v>9.646719401160329</v>
+      </c>
       <c r="I242">
         <f t="shared" si="18"/>
-        <v>2.577360826054544</v>
+        <v>6.1120401136074367</v>
       </c>
       <c r="J242">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>3.5346792875528918</v>
       </c>
       <c r="K242" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.57831415073397807</v>
       </c>
       <c r="L242" t="s">
         <v>660</v>
@@ -14259,17 +14448,20 @@
       <c r="C243">
         <v>5.8232437495763367</v>
       </c>
+      <c r="D243">
+        <v>7.6761450750708926</v>
+      </c>
       <c r="I243">
         <f t="shared" si="18"/>
-        <v>5.8232437495763367</v>
+        <v>6.7496944123236151</v>
       </c>
       <c r="J243">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.92645066274727361</v>
       </c>
       <c r="K243" s="6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.13725816402232327</v>
       </c>
       <c r="L243" t="s">
         <v>660</v>
@@ -14294,17 +14486,20 @@
       <c r="C244">
         <v>7.0199035338844364</v>
       </c>
+      <c r="D244">
+        <v>6.128280702610426</v>
+      </c>
       <c r="I244">
         <f t="shared" ref="I244:I269" si="21">AVERAGE(C244:H244)</f>
-        <v>7.0199035338844364</v>
+        <v>6.5740921182474317</v>
       </c>
       <c r="J244">
         <f t="shared" ref="J244:J269" si="22">_xlfn.STDEV.P(C244:H244)</f>
-        <v>0</v>
+        <v>0.44581141563700522</v>
       </c>
       <c r="K244" s="6">
         <f t="shared" ref="K244:K269" si="23">J244/I244</f>
-        <v>0</v>
+        <v>6.7813381318400631E-2</v>
       </c>
       <c r="L244" t="s">
         <v>660</v>
@@ -14329,17 +14524,20 @@
       <c r="C245">
         <v>4.015647607802852</v>
       </c>
+      <c r="D245">
+        <v>6.0973556318044722</v>
+      </c>
       <c r="I245">
         <f t="shared" si="21"/>
-        <v>4.015647607802852</v>
+        <v>5.0565016198036616</v>
       </c>
       <c r="J245">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1.0408540120008125</v>
       </c>
       <c r="K245" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>0.20584469070954786</v>
       </c>
       <c r="L245" t="s">
         <v>660</v>
@@ -14364,17 +14562,20 @@
       <c r="C246">
         <v>16.296389466504959</v>
       </c>
+      <c r="D246">
+        <v>14.85781537939023</v>
+      </c>
       <c r="I246">
         <f t="shared" si="21"/>
-        <v>16.296389466504959</v>
+        <v>15.577102422947593</v>
       </c>
       <c r="J246">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.71928704355736439</v>
       </c>
       <c r="K246" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>4.6175920529208186E-2</v>
       </c>
       <c r="L246" t="s">
         <v>660</v>
@@ -14399,17 +14600,20 @@
       <c r="C247">
         <v>22.92947050701051</v>
       </c>
+      <c r="D247">
+        <v>18.481838354350291</v>
+      </c>
       <c r="I247">
         <f t="shared" si="21"/>
-        <v>22.92947050701051</v>
+        <v>20.705654430680401</v>
       </c>
       <c r="J247">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2.2238160763301091</v>
       </c>
       <c r="K247" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>0.10740139046438404</v>
       </c>
       <c r="L247" t="s">
         <v>660</v>
@@ -14434,17 +14638,20 @@
       <c r="C248">
         <v>9.8628918088564603</v>
       </c>
+      <c r="D248">
+        <v>7.4892890129898424</v>
+      </c>
       <c r="I248">
         <f t="shared" si="21"/>
-        <v>9.8628918088564603</v>
+        <v>8.6760904109231518</v>
       </c>
       <c r="J248">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1.1868013979333045</v>
       </c>
       <c r="K248" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>0.13678988365994063</v>
       </c>
       <c r="L248" t="s">
         <v>660</v>
@@ -14469,17 +14676,20 @@
       <c r="C249">
         <v>15.087284290468199</v>
       </c>
+      <c r="D249">
+        <v>10.796011575395459</v>
+      </c>
       <c r="I249">
         <f t="shared" si="21"/>
-        <v>15.087284290468199</v>
+        <v>12.941647932931829</v>
       </c>
       <c r="J249">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2.1456363575363664</v>
       </c>
       <c r="K249" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>0.16579313304270124</v>
       </c>
       <c r="L249" t="s">
         <v>660</v>
@@ -14501,8 +14711,11 @@
       <c r="B250" t="s">
         <v>640</v>
       </c>
-      <c r="C250" t="s">
-        <v>34</v>
+      <c r="C250">
+        <v>149.64539007092199</v>
+      </c>
+      <c r="D250">
+        <v>130.10204081632651</v>
       </c>
       <c r="I250" t="s">
         <v>34</v>
@@ -14536,17 +14749,20 @@
       <c r="C251">
         <v>20.672712687325479</v>
       </c>
+      <c r="D251">
+        <v>15.751224161658939</v>
+      </c>
       <c r="I251">
         <f t="shared" si="21"/>
-        <v>20.672712687325479</v>
+        <v>18.211968424492209</v>
       </c>
       <c r="J251">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2.460744262833265</v>
       </c>
       <c r="K251" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>0.13511687509428988</v>
       </c>
       <c r="L251" t="s">
         <v>660</v>
@@ -14571,17 +14787,20 @@
       <c r="C252">
         <v>15.32296593744756</v>
       </c>
+      <c r="D252">
+        <v>16.905984683045901</v>
+      </c>
       <c r="I252">
         <f t="shared" si="21"/>
-        <v>15.32296593744756</v>
+        <v>16.114475310246732</v>
       </c>
       <c r="J252">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.79150937279917066</v>
       </c>
       <c r="K252" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>4.9117911539811203E-2</v>
       </c>
       <c r="L252" t="s">
         <v>660</v>
@@ -14606,17 +14825,20 @@
       <c r="C253">
         <v>6.9711446662118837</v>
       </c>
+      <c r="D253">
+        <v>14.34015398398418</v>
+      </c>
       <c r="I253">
         <f t="shared" si="21"/>
-        <v>6.9711446662118837</v>
+        <v>10.655649325098032</v>
       </c>
       <c r="J253">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>3.6845046588861488</v>
       </c>
       <c r="K253" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>0.34577945899624951</v>
       </c>
       <c r="L253" t="s">
         <v>660</v>
@@ -14641,17 +14863,20 @@
       <c r="C254">
         <v>8.4645157378005571</v>
       </c>
+      <c r="D254">
+        <v>8.6625672543966612</v>
+      </c>
       <c r="I254">
         <f t="shared" si="21"/>
-        <v>8.4645157378005571</v>
+        <v>8.5635414960986083</v>
       </c>
       <c r="J254">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>9.9025758298052047E-2</v>
       </c>
       <c r="K254" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1.156364552482946E-2</v>
       </c>
       <c r="L254" t="s">
         <v>660</v>
@@ -14676,17 +14901,20 @@
       <c r="C255">
         <v>9.926844513854677</v>
       </c>
+      <c r="D255">
+        <v>10.662139386728439</v>
+      </c>
       <c r="I255">
         <f t="shared" si="21"/>
-        <v>9.926844513854677</v>
+        <v>10.294491950291558</v>
       </c>
       <c r="J255">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.36764743643688114</v>
       </c>
       <c r="K255" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>3.5713023839556136E-2</v>
       </c>
       <c r="L255" t="s">
         <v>660</v>
@@ -14711,17 +14939,20 @@
       <c r="C256">
         <v>8.8544844918392407</v>
       </c>
+      <c r="D256">
+        <v>10.467766400790021</v>
+      </c>
       <c r="I256">
         <f t="shared" si="21"/>
-        <v>8.8544844918392407</v>
+        <v>9.6611254463146317</v>
       </c>
       <c r="J256">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.80664095447539008</v>
       </c>
       <c r="K256" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>8.3493476920237522E-2</v>
       </c>
       <c r="L256" t="s">
         <v>660</v>
@@ -14746,17 +14977,20 @@
       <c r="C257">
         <v>47.79599815420535</v>
       </c>
+      <c r="D257">
+        <v>44.542527907605788</v>
+      </c>
       <c r="I257">
         <f t="shared" si="21"/>
-        <v>47.79599815420535</v>
+        <v>46.169263030905569</v>
       </c>
       <c r="J257">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1.6267351232997811</v>
       </c>
       <c r="K257" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>3.5234158323273417E-2</v>
       </c>
       <c r="L257" t="s">
         <v>660</v>
@@ -14781,17 +15015,20 @@
       <c r="C258">
         <v>8.5762855005295542</v>
       </c>
+      <c r="D258">
+        <v>10.2709075756897</v>
+      </c>
       <c r="I258">
         <f t="shared" si="21"/>
-        <v>8.5762855005295542</v>
+        <v>9.4235965381096278</v>
       </c>
       <c r="J258">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.84731103758007276</v>
       </c>
       <c r="K258" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>8.9913764256936576E-2</v>
       </c>
       <c r="L258" t="s">
         <v>660</v>
@@ -14816,17 +15053,20 @@
       <c r="C259">
         <v>10.491138671958639</v>
       </c>
+      <c r="D259">
+        <v>12.05083057290954</v>
+      </c>
       <c r="I259">
         <f t="shared" si="21"/>
-        <v>10.491138671958639</v>
+        <v>11.270984622434089</v>
       </c>
       <c r="J259">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.77984595047545024</v>
       </c>
       <c r="K259" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>6.9190578871274708E-2</v>
       </c>
       <c r="L259" t="s">
         <v>660</v>
@@ -14851,17 +15091,20 @@
       <c r="C260">
         <v>15.37921241343753</v>
       </c>
+      <c r="D260">
+        <v>15.06758979438206</v>
+      </c>
       <c r="I260">
         <f t="shared" si="21"/>
-        <v>15.37921241343753</v>
+        <v>15.223401103909795</v>
       </c>
       <c r="J260">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.15581130952773492</v>
       </c>
       <c r="K260" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1.0234986811699931E-2</v>
       </c>
       <c r="L260" t="s">
         <v>660</v>
@@ -14886,17 +15129,20 @@
       <c r="C261">
         <v>14.41135335435682</v>
       </c>
+      <c r="D261">
+        <v>10.93833821790083</v>
+      </c>
       <c r="I261">
         <f t="shared" si="21"/>
-        <v>14.41135335435682</v>
+        <v>12.674845786128824</v>
       </c>
       <c r="J261">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1.7365075682280022</v>
       </c>
       <c r="K261" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>0.13700423638514103</v>
       </c>
       <c r="L261" t="s">
         <v>660</v>
@@ -14921,17 +15167,20 @@
       <c r="C262">
         <v>18.615068260065261</v>
       </c>
+      <c r="D262">
+        <v>13.929363070592951</v>
+      </c>
       <c r="I262">
         <f t="shared" si="21"/>
-        <v>18.615068260065261</v>
+        <v>16.272215665329107</v>
       </c>
       <c r="J262">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2.3428525947361485</v>
       </c>
       <c r="K262" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>0.1439787084267829</v>
       </c>
       <c r="L262" t="s">
         <v>660</v>
@@ -14956,17 +15205,20 @@
       <c r="C263">
         <v>21.37029019216477</v>
       </c>
+      <c r="D263">
+        <v>17.78874989846452</v>
+      </c>
       <c r="I263">
         <f t="shared" si="21"/>
-        <v>21.37029019216477</v>
+        <v>19.579520045314645</v>
       </c>
       <c r="J263">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1.7907701468501251</v>
       </c>
       <c r="K263" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>9.1461391428675709E-2</v>
       </c>
       <c r="L263" t="s">
         <v>660</v>
@@ -14991,17 +15243,20 @@
       <c r="C264">
         <v>16.354264778272231</v>
       </c>
+      <c r="D264">
+        <v>17.684737716487192</v>
+      </c>
       <c r="I264">
         <f t="shared" si="21"/>
-        <v>16.354264778272231</v>
+        <v>17.019501247379711</v>
       </c>
       <c r="J264">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.66523646910748013</v>
       </c>
       <c r="K264" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>3.9086719371985039E-2</v>
       </c>
       <c r="L264" t="s">
         <v>660</v>
@@ -15023,8 +15278,11 @@
       <c r="B265" t="s">
         <v>655</v>
       </c>
-      <c r="C265" t="s">
-        <v>34</v>
+      <c r="C265">
+        <v>140.2777777777778</v>
+      </c>
+      <c r="D265">
+        <v>144.89795918367341</v>
       </c>
       <c r="I265" t="s">
         <v>34</v>
@@ -15058,17 +15316,20 @@
       <c r="C266">
         <v>18.032698675709529</v>
       </c>
+      <c r="D266">
+        <v>15.5105973010117</v>
+      </c>
       <c r="I266">
         <f t="shared" si="21"/>
-        <v>18.032698675709529</v>
+        <v>16.771647988360613</v>
       </c>
       <c r="J266">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1.2610506873489147</v>
       </c>
       <c r="K266" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>7.5189432083482416E-2</v>
       </c>
       <c r="L266" t="s">
         <v>660</v>
@@ -15093,17 +15354,20 @@
       <c r="C267">
         <v>30.783890672369949</v>
       </c>
+      <c r="D267">
+        <v>29.832040883568709</v>
+      </c>
       <c r="I267">
         <f t="shared" si="21"/>
-        <v>30.783890672369949</v>
+        <v>30.307965777969329</v>
       </c>
       <c r="J267">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.47592489440062025</v>
       </c>
       <c r="K267" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1.5702963962911924E-2</v>
       </c>
       <c r="L267" t="s">
         <v>660</v>
@@ -15128,17 +15392,20 @@
       <c r="C268">
         <v>16.428919186466359</v>
       </c>
+      <c r="D268">
+        <v>16.141051668134089</v>
+      </c>
       <c r="I268">
         <f t="shared" si="21"/>
-        <v>16.428919186466359</v>
+        <v>16.284985427300224</v>
       </c>
       <c r="J268">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.14393375916613493</v>
       </c>
       <c r="K268" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>8.838433402884335E-3</v>
       </c>
       <c r="L268" t="s">
         <v>660</v>
@@ -15163,17 +15430,20 @@
       <c r="C269">
         <v>17.777483145106089</v>
       </c>
+      <c r="D269">
+        <v>17.799043798976768</v>
+      </c>
       <c r="I269">
         <f t="shared" si="21"/>
-        <v>17.777483145106089</v>
+        <v>17.788263472041429</v>
       </c>
       <c r="J269">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1.0780326935339701E-2</v>
       </c>
       <c r="K269" s="6">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>6.0603593781279443E-4</v>
       </c>
       <c r="L269" t="s">
         <v>660</v>

</xml_diff>

<commit_message>
Added Rep 6 and 7 Third Plate
</commit_message>
<xml_diff>
--- a/data/Results_Masterfile.xlsx
+++ b/data/Results_Masterfile.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOL428\Documents\GitHub\SynBioMLMH\SynbioML\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C038CB90-5620-4934-9577-557A72D1A978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F04DA01-5368-4AC6-B4D3-7F32BB3B52EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="3350" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53652" yWindow="-4668" windowWidth="30936" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microplate" sheetId="1" r:id="rId1"/>
     <sheet name="Flow Cytometer" sheetId="2" r:id="rId2"/>
     <sheet name="Archived Results" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2840" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2843" uniqueCount="665">
   <si>
     <t>RBS</t>
   </si>
@@ -2021,13 +2021,22 @@
   </si>
   <si>
     <t>01-Well-H6</t>
+  </si>
+  <si>
+    <t>Rep7</t>
+  </si>
+  <si>
+    <t>Rep8</t>
+  </si>
+  <si>
+    <t>Rep9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2057,6 +2066,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -2104,7 +2120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2129,6 +2145,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2542,10 +2559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P271"/>
+  <dimension ref="A1:T271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A188" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H198" sqref="H198"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R181" sqref="R181:R271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2563,7 +2580,7 @@
     <col min="19" max="1025" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2612,8 +2629,17 @@
       <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="R1" s="14" t="s">
+        <v>662</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>663</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -2666,7 +2692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:20">
       <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
@@ -2719,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:20">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -2772,7 +2798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -2825,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
@@ -2878,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:20">
       <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
@@ -2931,7 +2957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:20">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
@@ -2984,7 +3010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:20">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -3034,7 +3060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:20">
       <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
@@ -3087,7 +3113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:20">
       <c r="A11" s="4" t="s">
         <v>41</v>
       </c>
@@ -3140,7 +3166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:20">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -3193,7 +3219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:20">
       <c r="A13" s="4" t="s">
         <v>45</v>
       </c>
@@ -3246,7 +3272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:20">
       <c r="A14" s="4" t="s">
         <v>47</v>
       </c>
@@ -3299,7 +3325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:20">
       <c r="A15" s="4" t="s">
         <v>49</v>
       </c>
@@ -3352,7 +3378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:20">
       <c r="A16" s="4" t="s">
         <v>51</v>
       </c>
@@ -11882,7 +11908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:16">
+    <row r="177" spans="1:18">
       <c r="A177" s="9" t="s">
         <v>376</v>
       </c>
@@ -11935,7 +11961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:16">
+    <row r="178" spans="1:18">
       <c r="A178" s="9" t="s">
         <v>378</v>
       </c>
@@ -11988,7 +12014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:16">
+    <row r="179" spans="1:18">
       <c r="A179" s="9" t="s">
         <v>380</v>
       </c>
@@ -12041,7 +12067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:16">
+    <row r="180" spans="1:18">
       <c r="A180" s="9" t="s">
         <v>382</v>
       </c>
@@ -12094,7 +12120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:16">
+    <row r="181" spans="1:18">
       <c r="A181" t="s">
         <v>384</v>
       </c>
@@ -12116,17 +12142,20 @@
       <c r="G181">
         <v>82.435720702144096</v>
       </c>
+      <c r="H181">
+        <v>66.317294194942164</v>
+      </c>
       <c r="I181">
         <f t="shared" ref="I181:I212" si="21">AVERAGE(C181:H181)</f>
-        <v>45.518204200558209</v>
+        <v>48.984719199622198</v>
       </c>
       <c r="J181">
         <f t="shared" ref="J181:J212" si="22">_xlfn.STDEV.P(C181:H181)</f>
-        <v>27.886746326384511</v>
+        <v>26.610946652717548</v>
       </c>
       <c r="K181" s="7">
         <f t="shared" ref="K181:K212" si="23">J181/I181</f>
-        <v>0.61265040693416728</v>
+        <v>0.54324995809964327</v>
       </c>
       <c r="L181" t="s">
         <v>386</v>
@@ -12143,8 +12172,11 @@
       <c r="P181">
         <v>1</v>
       </c>
-    </row>
-    <row r="182" spans="1:16">
+      <c r="R181">
+        <v>60.616124137197758</v>
+      </c>
+    </row>
+    <row r="182" spans="1:18">
       <c r="A182" t="s">
         <v>389</v>
       </c>
@@ -12166,17 +12198,20 @@
       <c r="G182">
         <v>70.069982811195572</v>
       </c>
+      <c r="H182">
+        <v>65.462117603146098</v>
+      </c>
       <c r="I182">
         <f t="shared" si="21"/>
-        <v>39.590569003173286</v>
+        <v>43.902493769835424</v>
       </c>
       <c r="J182">
         <f t="shared" si="22"/>
-        <v>23.135075229814852</v>
+        <v>23.21615595961352</v>
       </c>
       <c r="K182" s="7">
         <f t="shared" si="23"/>
-        <v>0.58435824016473514</v>
+        <v>0.52881178188481182</v>
       </c>
       <c r="L182" t="s">
         <v>386</v>
@@ -12193,8 +12228,11 @@
       <c r="P182">
         <v>1</v>
       </c>
-    </row>
-    <row r="183" spans="1:16">
+      <c r="R182">
+        <v>52.354378703343663</v>
+      </c>
+    </row>
+    <row r="183" spans="1:18">
       <c r="A183" t="s">
         <v>391</v>
       </c>
@@ -12216,17 +12254,20 @@
       <c r="G183">
         <v>69.388412012398391</v>
       </c>
+      <c r="H183">
+        <v>64.119171993029767</v>
+      </c>
       <c r="I183">
         <f t="shared" si="21"/>
-        <v>39.010393394297367</v>
+        <v>43.195189827419426</v>
       </c>
       <c r="J183">
         <f t="shared" si="22"/>
-        <v>22.099804600264203</v>
+        <v>22.238789132389947</v>
       </c>
       <c r="K183" s="7">
         <f t="shared" si="23"/>
-        <v>0.56651068285547734</v>
+        <v>0.51484411160691823</v>
       </c>
       <c r="L183" t="s">
         <v>386</v>
@@ -12243,8 +12284,11 @@
       <c r="P183">
         <v>1</v>
       </c>
-    </row>
-    <row r="184" spans="1:16">
+      <c r="R183">
+        <v>46.98772540794323</v>
+      </c>
+    </row>
+    <row r="184" spans="1:18">
       <c r="A184" t="s">
         <v>393</v>
       </c>
@@ -12266,17 +12310,20 @@
       <c r="G184">
         <v>58.622310069384369</v>
       </c>
+      <c r="H184">
+        <v>54.944093685319046</v>
+      </c>
       <c r="I184">
         <f t="shared" si="21"/>
-        <v>34.279581354235702</v>
+        <v>37.723666742749593</v>
       </c>
       <c r="J184">
         <f t="shared" si="22"/>
-        <v>19.822014625184245</v>
+        <v>19.665591964589392</v>
       </c>
       <c r="K184" s="7">
         <f t="shared" si="23"/>
-        <v>0.5782455281570984</v>
+        <v>0.52130648111955014</v>
       </c>
       <c r="L184" t="s">
         <v>386</v>
@@ -12293,8 +12340,11 @@
       <c r="P184">
         <v>1</v>
       </c>
-    </row>
-    <row r="185" spans="1:16">
+      <c r="R184">
+        <v>42.602683618806957</v>
+      </c>
+    </row>
+    <row r="185" spans="1:18">
       <c r="A185" t="s">
         <v>395</v>
       </c>
@@ -12316,17 +12366,20 @@
       <c r="G185">
         <v>59.0187448440239</v>
       </c>
+      <c r="H185">
+        <v>52.499576505018581</v>
+      </c>
       <c r="I185">
         <f t="shared" si="21"/>
-        <v>31.77748354575753</v>
+        <v>35.231165705634375</v>
       </c>
       <c r="J185">
         <f t="shared" si="22"/>
-        <v>19.430590928855136</v>
+        <v>19.345873518083401</v>
       </c>
       <c r="K185" s="7">
         <f t="shared" si="23"/>
-        <v>0.61145782361514989</v>
+        <v>0.54911250112253585</v>
       </c>
       <c r="L185" t="s">
         <v>386</v>
@@ -12343,8 +12396,11 @@
       <c r="P185">
         <v>1</v>
       </c>
-    </row>
-    <row r="186" spans="1:16">
+      <c r="R185">
+        <v>37.827473433972322</v>
+      </c>
+    </row>
+    <row r="186" spans="1:18">
       <c r="A186" t="s">
         <v>397</v>
       </c>
@@ -12366,17 +12422,20 @@
       <c r="G186">
         <v>56.006820467604683</v>
       </c>
+      <c r="H186">
+        <v>50.850177971831563</v>
+      </c>
       <c r="I186">
         <f t="shared" si="21"/>
-        <v>31.402324033657372</v>
+        <v>34.643633023353068</v>
       </c>
       <c r="J186">
         <f t="shared" si="22"/>
-        <v>17.555542518328028</v>
+        <v>17.588670049042843</v>
       </c>
       <c r="K186" s="7">
         <f t="shared" si="23"/>
-        <v>0.55905233318119374</v>
+        <v>0.50770281619097002</v>
       </c>
       <c r="L186" t="s">
         <v>386</v>
@@ -12393,8 +12452,11 @@
       <c r="P186">
         <v>1</v>
       </c>
-    </row>
-    <row r="187" spans="1:16">
+      <c r="R186">
+        <v>37.33000186936124</v>
+      </c>
+    </row>
+    <row r="187" spans="1:18">
       <c r="A187" t="s">
         <v>399</v>
       </c>
@@ -12416,17 +12478,20 @@
       <c r="G187">
         <v>55.771221798968618</v>
       </c>
+      <c r="H187">
+        <v>48.889544900363717</v>
+      </c>
       <c r="I187">
         <f t="shared" si="21"/>
-        <v>31.11680309847041</v>
+        <v>34.078926732119292</v>
       </c>
       <c r="J187">
         <f t="shared" si="22"/>
-        <v>17.099017617274093</v>
+        <v>16.956352349536964</v>
       </c>
       <c r="K187" s="7">
         <f t="shared" si="23"/>
-        <v>0.54951074386284304</v>
+        <v>0.49756121965999739</v>
       </c>
       <c r="L187" t="s">
         <v>386</v>
@@ -12443,8 +12508,11 @@
       <c r="P187">
         <v>1</v>
       </c>
-    </row>
-    <row r="188" spans="1:16">
+      <c r="R187">
+        <v>37.981881890903338</v>
+      </c>
+    </row>
+    <row r="188" spans="1:18">
       <c r="A188" t="s">
         <v>401</v>
       </c>
@@ -12466,17 +12534,20 @@
       <c r="G188">
         <v>58.693251880493527</v>
       </c>
+      <c r="H188">
+        <v>52.588543808432867</v>
+      </c>
       <c r="I188">
         <f t="shared" si="21"/>
-        <v>34.1013801234878</v>
+        <v>37.182574070978639</v>
       </c>
       <c r="J188">
         <f t="shared" si="22"/>
-        <v>17.891928087466344</v>
+        <v>17.726713070471558</v>
       </c>
       <c r="K188" s="7">
         <f t="shared" si="23"/>
-        <v>0.5246687384110601</v>
+        <v>0.47674787217885028</v>
       </c>
       <c r="L188" t="s">
         <v>386</v>
@@ -12493,8 +12564,11 @@
       <c r="P188">
         <v>1</v>
       </c>
-    </row>
-    <row r="189" spans="1:16">
+      <c r="R188">
+        <v>40.766818948382728</v>
+      </c>
+    </row>
+    <row r="189" spans="1:18">
       <c r="A189" t="s">
         <v>403</v>
       </c>
@@ -12516,17 +12590,20 @@
       <c r="G189">
         <v>49.184777037298687</v>
       </c>
+      <c r="H189">
+        <v>49.696800589251758</v>
+      </c>
       <c r="I189">
         <f t="shared" si="21"/>
-        <v>28.829802192198464</v>
+        <v>32.307635258374013</v>
       </c>
       <c r="J189">
         <f t="shared" si="22"/>
-        <v>14.678626775223121</v>
+        <v>15.492848377649427</v>
       </c>
       <c r="K189" s="7">
         <f t="shared" si="23"/>
-        <v>0.5091476756366804</v>
+        <v>0.47954139180253808</v>
       </c>
       <c r="L189" t="s">
         <v>386</v>
@@ -12543,8 +12620,11 @@
       <c r="P189">
         <v>1</v>
       </c>
-    </row>
-    <row r="190" spans="1:16">
+      <c r="R189">
+        <v>35.215658261559653</v>
+      </c>
+    </row>
+    <row r="190" spans="1:18">
       <c r="A190" t="s">
         <v>405</v>
       </c>
@@ -12566,17 +12646,20 @@
       <c r="G190">
         <v>47.932265423780898</v>
       </c>
+      <c r="H190">
+        <v>43.264292177024558</v>
+      </c>
       <c r="I190">
         <f t="shared" si="21"/>
-        <v>28.024363463980876</v>
+        <v>30.564351582821491</v>
       </c>
       <c r="J190">
         <f t="shared" si="22"/>
-        <v>15.169052682648207</v>
+        <v>14.966891158823016</v>
       </c>
       <c r="K190" s="7">
         <f t="shared" si="23"/>
-        <v>0.54128090017618669</v>
+        <v>0.48968456334715982</v>
       </c>
       <c r="L190" t="s">
         <v>386</v>
@@ -12593,8 +12676,11 @@
       <c r="P190">
         <v>1</v>
       </c>
-    </row>
-    <row r="191" spans="1:16">
+      <c r="R190">
+        <v>31.351889736409952</v>
+      </c>
+    </row>
+    <row r="191" spans="1:18">
       <c r="A191" t="s">
         <v>407</v>
       </c>
@@ -12616,17 +12702,20 @@
       <c r="G191">
         <v>46.673721253489838</v>
       </c>
+      <c r="H191">
+        <v>44.60764170873292</v>
+      </c>
       <c r="I191">
         <f t="shared" si="21"/>
-        <v>26.400827619025272</v>
+        <v>29.435296633976549</v>
       </c>
       <c r="J191">
         <f t="shared" si="22"/>
-        <v>14.801669119780657</v>
+        <v>15.120003911696596</v>
       </c>
       <c r="K191" s="7">
         <f t="shared" si="23"/>
-        <v>0.56065170885454008</v>
+        <v>0.51366915372763366</v>
       </c>
       <c r="L191" t="s">
         <v>386</v>
@@ -12643,8 +12732,11 @@
       <c r="P191">
         <v>1</v>
       </c>
-    </row>
-    <row r="192" spans="1:16">
+      <c r="R191">
+        <v>29.511192561959479</v>
+      </c>
+    </row>
+    <row r="192" spans="1:18">
       <c r="A192" t="s">
         <v>409</v>
       </c>
@@ -12666,17 +12758,20 @@
       <c r="G192">
         <v>59.049737589294907</v>
       </c>
+      <c r="H192">
+        <v>50.196459154746982</v>
+      </c>
       <c r="I192">
         <f t="shared" si="21"/>
-        <v>33.220532575029864</v>
+        <v>36.04985367164938</v>
       </c>
       <c r="J192">
         <f t="shared" si="22"/>
-        <v>17.931616632983182</v>
+        <v>17.54929301232524</v>
       </c>
       <c r="K192" s="7">
         <f t="shared" si="23"/>
-        <v>0.53977511024195446</v>
+        <v>0.48680622041266419</v>
       </c>
       <c r="L192" t="s">
         <v>386</v>
@@ -12693,8 +12788,11 @@
       <c r="P192">
         <v>1</v>
       </c>
-    </row>
-    <row r="193" spans="1:16">
+      <c r="R192">
+        <v>38.511819634862057</v>
+      </c>
+    </row>
+    <row r="193" spans="1:18">
       <c r="A193" t="s">
         <v>411</v>
       </c>
@@ -12716,17 +12814,20 @@
       <c r="G193">
         <v>95.89028937693449</v>
       </c>
+      <c r="H193">
+        <v>84.241149825492982</v>
+      </c>
       <c r="I193">
         <f t="shared" si="21"/>
-        <v>60.839993532021765</v>
+        <v>64.740186247600306</v>
       </c>
       <c r="J193">
         <f t="shared" si="22"/>
-        <v>30.489067981577364</v>
+        <v>29.166937413464638</v>
       </c>
       <c r="K193" s="7">
         <f t="shared" si="23"/>
-        <v>0.50113529294723091</v>
+        <v>0.45052291480773665</v>
       </c>
       <c r="L193" t="s">
         <v>386</v>
@@ -12743,8 +12844,11 @@
       <c r="P193">
         <v>1</v>
       </c>
-    </row>
-    <row r="194" spans="1:16">
+      <c r="R193">
+        <v>71.904698779100457</v>
+      </c>
+    </row>
+    <row r="194" spans="1:18">
       <c r="A194" t="s">
         <v>413</v>
       </c>
@@ -12766,17 +12870,20 @@
       <c r="G194">
         <v>53.930017707901527</v>
       </c>
+      <c r="H194">
+        <v>51.123867469480153</v>
+      </c>
       <c r="I194">
         <f t="shared" si="21"/>
-        <v>30.517937565518316</v>
+        <v>33.952259216178625</v>
       </c>
       <c r="J194">
         <f t="shared" si="22"/>
-        <v>17.942719413531123</v>
+        <v>18.090249932718624</v>
       </c>
       <c r="K194" s="7">
         <f t="shared" si="23"/>
-        <v>0.58794010489766146</v>
+        <v>0.5328143207653887</v>
       </c>
       <c r="L194" t="s">
         <v>386</v>
@@ -12793,8 +12900,11 @@
       <c r="P194">
         <v>1</v>
       </c>
-    </row>
-    <row r="195" spans="1:16">
+      <c r="R194">
+        <v>44.298568690003989</v>
+      </c>
+    </row>
+    <row r="195" spans="1:18">
       <c r="A195" t="s">
         <v>415</v>
       </c>
@@ -12816,17 +12926,20 @@
       <c r="G195">
         <v>42.160390196351919</v>
       </c>
+      <c r="H195">
+        <v>38.736294671945167</v>
+      </c>
       <c r="I195">
         <f t="shared" si="21"/>
-        <v>24.856356387226253</v>
+        <v>27.169679434679406</v>
       </c>
       <c r="J195">
         <f t="shared" si="22"/>
-        <v>14.82494221746836</v>
+        <v>14.488147249923051</v>
       </c>
       <c r="K195" s="7">
         <f t="shared" si="23"/>
-        <v>0.596424592024555</v>
+        <v>0.53324689695934968</v>
       </c>
       <c r="L195" t="s">
         <v>386</v>
@@ -12843,8 +12956,11 @@
       <c r="P195">
         <v>1</v>
       </c>
-    </row>
-    <row r="196" spans="1:16">
+      <c r="R195">
+        <v>31.869409010829649</v>
+      </c>
+    </row>
+    <row r="196" spans="1:18">
       <c r="A196" t="s">
         <v>417</v>
       </c>
@@ -12866,17 +12982,20 @@
       <c r="G196">
         <v>16.363231708484491</v>
       </c>
+      <c r="H196">
+        <v>16.947890566024579</v>
+      </c>
       <c r="I196">
         <f t="shared" si="21"/>
-        <v>15.412854667788366</v>
+        <v>15.668693984161068</v>
       </c>
       <c r="J196">
         <f t="shared" si="22"/>
-        <v>3.2401213008233141</v>
+        <v>3.012627394105964</v>
       </c>
       <c r="K196" s="7">
         <f t="shared" si="23"/>
-        <v>0.21022201082547728</v>
+        <v>0.19227048515666481</v>
       </c>
       <c r="L196" t="s">
         <v>386</v>
@@ -12893,8 +13012,11 @@
       <c r="P196">
         <v>1</v>
       </c>
-    </row>
-    <row r="197" spans="1:16">
+      <c r="R196">
+        <v>19.692282713531618</v>
+      </c>
+    </row>
+    <row r="197" spans="1:18">
       <c r="A197" t="s">
         <v>419</v>
       </c>
@@ -12916,17 +13038,20 @@
       <c r="G197">
         <v>18.485373772205001</v>
       </c>
+      <c r="H197">
+        <v>16.512786229012701</v>
+      </c>
       <c r="I197">
         <f t="shared" si="21"/>
-        <v>16.338152910589326</v>
+        <v>16.367258463659891</v>
       </c>
       <c r="J197">
         <f t="shared" si="22"/>
-        <v>2.9031376741599</v>
+        <v>2.6509889906793624</v>
       </c>
       <c r="K197" s="7">
         <f t="shared" si="23"/>
-        <v>0.17769069062135387</v>
+        <v>0.16196903082854924</v>
       </c>
       <c r="L197" t="s">
         <v>386</v>
@@ -12943,8 +13068,11 @@
       <c r="P197">
         <v>1</v>
       </c>
-    </row>
-    <row r="198" spans="1:16">
+      <c r="R197">
+        <v>20.585729341340571</v>
+      </c>
+    </row>
+    <row r="198" spans="1:18">
       <c r="A198" t="s">
         <v>421</v>
       </c>
@@ -12966,17 +13094,20 @@
       <c r="G198">
         <v>22.629142911714052</v>
       </c>
+      <c r="H198">
+        <v>9.9330279857812105</v>
+      </c>
       <c r="I198">
         <f t="shared" si="21"/>
-        <v>13.637820685018974</v>
+        <v>13.020355235146013</v>
       </c>
       <c r="J198">
         <f t="shared" si="22"/>
-        <v>5.0193070793385637</v>
+        <v>4.7854836961568061</v>
       </c>
       <c r="K198" s="7">
         <f t="shared" si="23"/>
-        <v>0.36804319364986432</v>
+        <v>0.3675386431269777</v>
       </c>
       <c r="L198" t="s">
         <v>386</v>
@@ -12993,8 +13124,11 @@
       <c r="P198">
         <v>1</v>
       </c>
-    </row>
-    <row r="199" spans="1:16">
+      <c r="R198">
+        <v>11.71290099800253</v>
+      </c>
+    </row>
+    <row r="199" spans="1:18">
       <c r="A199" t="s">
         <v>423</v>
       </c>
@@ -13016,17 +13150,20 @@
       <c r="G199">
         <v>23.55526270266202</v>
       </c>
+      <c r="H199">
+        <v>19.88394295544563</v>
+      </c>
       <c r="I199">
         <f t="shared" si="21"/>
-        <v>14.745987746887533</v>
+        <v>15.602313614980551</v>
       </c>
       <c r="J199">
         <f t="shared" si="22"/>
-        <v>5.8828924862140592</v>
+        <v>5.7014755369805608</v>
       </c>
       <c r="K199" s="7">
         <f t="shared" si="23"/>
-        <v>0.39894868944644107</v>
+        <v>0.36542500539832073</v>
       </c>
       <c r="L199" t="s">
         <v>386</v>
@@ -13043,8 +13180,11 @@
       <c r="P199">
         <v>1</v>
       </c>
-    </row>
-    <row r="200" spans="1:16">
+      <c r="R199">
+        <v>9.7768687988655305</v>
+      </c>
+    </row>
+    <row r="200" spans="1:18">
       <c r="A200" t="s">
         <v>425</v>
       </c>
@@ -13066,17 +13206,20 @@
       <c r="G200">
         <v>21.981216030215482</v>
       </c>
+      <c r="H200">
+        <v>19.9037641552687</v>
+      </c>
       <c r="I200">
         <f t="shared" si="21"/>
-        <v>11.923728826375861</v>
+        <v>13.253734714524668</v>
       </c>
       <c r="J200">
         <f t="shared" si="22"/>
-        <v>5.1991573063704912</v>
+        <v>5.6009471424816946</v>
       </c>
       <c r="K200" s="7">
         <f t="shared" si="23"/>
-        <v>0.43603451420915457</v>
+        <v>0.42259387735772758</v>
       </c>
       <c r="L200" t="s">
         <v>386</v>
@@ -13093,8 +13236,11 @@
       <c r="P200">
         <v>1</v>
       </c>
-    </row>
-    <row r="201" spans="1:16">
+      <c r="R200">
+        <v>17.005224943999821</v>
+      </c>
+    </row>
+    <row r="201" spans="1:18">
       <c r="A201" t="s">
         <v>427</v>
       </c>
@@ -13116,17 +13262,20 @@
       <c r="G201">
         <v>17.864763669351159</v>
       </c>
+      <c r="H201">
+        <v>17.875787164609289</v>
+      </c>
       <c r="I201">
         <f t="shared" si="21"/>
-        <v>15.189190772819751</v>
+        <v>15.636956838118008</v>
       </c>
       <c r="J201">
         <f t="shared" si="22"/>
-        <v>3.1029304966170725</v>
+        <v>3.004322491876267</v>
       </c>
       <c r="K201" s="7">
         <f t="shared" si="23"/>
-        <v>0.20428543844281696</v>
+        <v>0.19212961466726497</v>
       </c>
       <c r="L201" t="s">
         <v>386</v>
@@ -13143,8 +13292,11 @@
       <c r="P201">
         <v>1</v>
       </c>
-    </row>
-    <row r="202" spans="1:16">
+      <c r="R201">
+        <v>12.00497265780519</v>
+      </c>
+    </row>
+    <row r="202" spans="1:18">
       <c r="A202" t="s">
         <v>429</v>
       </c>
@@ -13166,17 +13318,20 @@
       <c r="G202">
         <v>14.24612318822493</v>
       </c>
+      <c r="H202">
+        <v>14.24160204385112</v>
+      </c>
       <c r="I202">
         <f t="shared" si="21"/>
-        <v>10.531319237242394</v>
+        <v>11.149699705010514</v>
       </c>
       <c r="J202">
         <f t="shared" si="22"/>
-        <v>3.2346735776990698</v>
+        <v>3.2605571573693775</v>
       </c>
       <c r="K202" s="7">
         <f t="shared" si="23"/>
-        <v>0.30714799398162229</v>
+        <v>0.29243452681547377</v>
       </c>
       <c r="L202" t="s">
         <v>386</v>
@@ -13193,8 +13348,11 @@
       <c r="P202">
         <v>1</v>
       </c>
-    </row>
-    <row r="203" spans="1:16">
+      <c r="R202">
+        <v>22.664823542539139</v>
+      </c>
+    </row>
+    <row r="203" spans="1:18">
       <c r="A203" t="s">
         <v>431</v>
       </c>
@@ -13216,17 +13374,20 @@
       <c r="G203">
         <v>15.23753526548191</v>
       </c>
+      <c r="H203">
+        <v>14.69774894273894</v>
+      </c>
       <c r="I203">
         <f t="shared" si="21"/>
-        <v>10.980095206519419</v>
+        <v>11.599704162556007</v>
       </c>
       <c r="J203">
         <f t="shared" si="22"/>
-        <v>3.3634821036913261</v>
+        <v>3.3685436284662007</v>
       </c>
       <c r="K203" s="7">
         <f t="shared" si="23"/>
-        <v>0.30632540432748367</v>
+        <v>0.29039909822354804</v>
       </c>
       <c r="L203" t="s">
         <v>386</v>
@@ -13243,8 +13404,11 @@
       <c r="P203">
         <v>1</v>
       </c>
-    </row>
-    <row r="204" spans="1:16">
+      <c r="R203">
+        <v>9.5576432057042648</v>
+      </c>
+    </row>
+    <row r="204" spans="1:18">
       <c r="A204" t="s">
         <v>433</v>
       </c>
@@ -13266,17 +13430,20 @@
       <c r="G204">
         <v>38.774024109444767</v>
       </c>
+      <c r="H204">
+        <v>39.010538639598629</v>
+      </c>
       <c r="I204">
         <f t="shared" si="21"/>
-        <v>26.464540336891911</v>
+        <v>28.555540054009697</v>
       </c>
       <c r="J204">
         <f t="shared" si="22"/>
-        <v>11.94177799911791</v>
+        <v>11.861693972691274</v>
       </c>
       <c r="K204" s="7">
         <f t="shared" si="23"/>
-        <v>0.45123693240463797</v>
+        <v>0.41539028679745404</v>
       </c>
       <c r="L204" t="s">
         <v>386</v>
@@ -13293,8 +13460,11 @@
       <c r="P204">
         <v>1</v>
       </c>
-    </row>
-    <row r="205" spans="1:16">
+      <c r="R204">
+        <v>30.072345844462848</v>
+      </c>
+    </row>
+    <row r="205" spans="1:18">
       <c r="A205" t="s">
         <v>435</v>
       </c>
@@ -13316,17 +13486,20 @@
       <c r="G205">
         <v>65.441265300017406</v>
       </c>
+      <c r="H205">
+        <v>55.162844443056443</v>
+      </c>
       <c r="I205">
         <f t="shared" si="21"/>
-        <v>36.314388697796282</v>
+        <v>39.455797988672977</v>
       </c>
       <c r="J205">
         <f t="shared" si="22"/>
-        <v>21.84956809264456</v>
+        <v>21.146598225876062</v>
       </c>
       <c r="K205" s="7">
         <f t="shared" si="23"/>
-        <v>0.60167798154262997</v>
+        <v>0.53595667313449991</v>
       </c>
       <c r="L205" t="s">
         <v>386</v>
@@ -13343,8 +13516,11 @@
       <c r="P205">
         <v>1</v>
       </c>
-    </row>
-    <row r="206" spans="1:16">
+      <c r="R205">
+        <v>48.673487651027841</v>
+      </c>
+    </row>
+    <row r="206" spans="1:18">
       <c r="A206" t="s">
         <v>437</v>
       </c>
@@ -13366,17 +13542,20 @@
       <c r="G206">
         <v>37.688324459887028</v>
       </c>
+      <c r="H206">
+        <v>39.825022342042857</v>
+      </c>
       <c r="I206">
         <f t="shared" si="21"/>
-        <v>16.550439842875448</v>
+        <v>20.429536926070018</v>
       </c>
       <c r="J206">
         <f t="shared" si="22"/>
-        <v>11.048280260611975</v>
+        <v>13.302533023266653</v>
       </c>
       <c r="K206" s="7">
         <f t="shared" si="23"/>
-        <v>0.66755206299656045</v>
+        <v>0.65114217083850612</v>
       </c>
       <c r="L206" t="s">
         <v>386</v>
@@ -13393,8 +13572,11 @@
       <c r="P206">
         <v>1</v>
       </c>
-    </row>
-    <row r="207" spans="1:16">
+      <c r="R206">
+        <v>29.603940323779849</v>
+      </c>
+    </row>
+    <row r="207" spans="1:18">
       <c r="A207" t="s">
         <v>439</v>
       </c>
@@ -13416,17 +13598,20 @@
       <c r="G207">
         <v>41.324238391765633</v>
       </c>
+      <c r="H207">
+        <v>47.630942041171132</v>
+      </c>
       <c r="I207">
         <f t="shared" si="21"/>
-        <v>28.508790253551592</v>
+        <v>31.695815551488181</v>
       </c>
       <c r="J207">
         <f t="shared" si="22"/>
-        <v>11.52385968589744</v>
+        <v>12.706367286993665</v>
       </c>
       <c r="K207" s="7">
         <f t="shared" si="23"/>
-        <v>0.40422127994230872</v>
+        <v>0.40088469300790952</v>
       </c>
       <c r="L207" t="s">
         <v>386</v>
@@ -13443,8 +13628,11 @@
       <c r="P207">
         <v>1</v>
       </c>
-    </row>
-    <row r="208" spans="1:16">
+      <c r="R207">
+        <v>35.744036043706771</v>
+      </c>
+    </row>
+    <row r="208" spans="1:18">
       <c r="A208" t="s">
         <v>441</v>
       </c>
@@ -13466,17 +13654,20 @@
       <c r="G208">
         <v>16.27760045455474</v>
       </c>
+      <c r="H208">
+        <v>14.21775541639358</v>
+      </c>
       <c r="I208">
         <f t="shared" si="21"/>
-        <v>11.439501487424684</v>
+        <v>11.902543808919498</v>
       </c>
       <c r="J208">
         <f t="shared" si="22"/>
-        <v>2.879031904430533</v>
+        <v>2.8247822712114723</v>
       </c>
       <c r="K208" s="7">
         <f t="shared" si="23"/>
-        <v>0.25167459505079137</v>
+        <v>0.23732592936096938</v>
       </c>
       <c r="L208" t="s">
         <v>386</v>
@@ -13493,8 +13684,11 @@
       <c r="P208">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="1:16">
+      <c r="R208">
+        <v>10.394225791104949</v>
+      </c>
+    </row>
+    <row r="209" spans="1:18">
       <c r="A209" t="s">
         <v>443</v>
       </c>
@@ -13516,17 +13710,20 @@
       <c r="G209">
         <v>15.764079820638999</v>
       </c>
+      <c r="H209">
+        <v>14.584215669322569</v>
+      </c>
       <c r="I209">
         <f t="shared" si="21"/>
-        <v>12.31611998606194</v>
+        <v>12.694135933272046</v>
       </c>
       <c r="J209">
         <f t="shared" si="22"/>
-        <v>5.3729544314506175</v>
+        <v>4.9771156021431153</v>
       </c>
       <c r="K209" s="7">
         <f t="shared" si="23"/>
-        <v>0.43625382324393958</v>
+        <v>0.39207990432005813</v>
       </c>
       <c r="L209" t="s">
         <v>386</v>
@@ -13543,8 +13740,11 @@
       <c r="P209">
         <v>1</v>
       </c>
-    </row>
-    <row r="210" spans="1:16">
+      <c r="R209">
+        <v>8.2401195415027679</v>
+      </c>
+    </row>
+    <row r="210" spans="1:18">
       <c r="A210" t="s">
         <v>445</v>
       </c>
@@ -13566,17 +13766,20 @@
       <c r="G210">
         <v>12.094174851735261</v>
       </c>
+      <c r="H210">
+        <v>6.344072049713513</v>
+      </c>
       <c r="I210">
         <f t="shared" si="21"/>
-        <v>10.862474897839297</v>
+        <v>10.109407756485</v>
       </c>
       <c r="J210">
         <f t="shared" si="22"/>
-        <v>2.7595373495353206</v>
+        <v>3.0300862336196595</v>
       </c>
       <c r="K210" s="7">
         <f t="shared" si="23"/>
-        <v>0.25404315089227342</v>
+        <v>0.29972935176899107</v>
       </c>
       <c r="L210" t="s">
         <v>386</v>
@@ -13593,8 +13796,11 @@
       <c r="P210">
         <v>1</v>
       </c>
-    </row>
-    <row r="211" spans="1:16">
+      <c r="R210">
+        <v>7.3733235618530779</v>
+      </c>
+    </row>
+    <row r="211" spans="1:18">
       <c r="A211" t="s">
         <v>447</v>
       </c>
@@ -13616,17 +13822,20 @@
       <c r="G211">
         <v>14.39662204723767</v>
       </c>
+      <c r="H211">
+        <v>9.6346868003763468</v>
+      </c>
       <c r="I211">
         <f t="shared" si="21"/>
-        <v>11.240493875626715</v>
+        <v>10.972859363084986</v>
       </c>
       <c r="J211">
         <f t="shared" si="22"/>
-        <v>3.5896287704699219</v>
+        <v>3.3310664087753881</v>
       </c>
       <c r="K211" s="7">
         <f t="shared" si="23"/>
-        <v>0.31934795838939789</v>
+        <v>0.30357323451914442</v>
       </c>
       <c r="L211" t="s">
         <v>386</v>
@@ -13643,8 +13852,11 @@
       <c r="P211">
         <v>1</v>
       </c>
-    </row>
-    <row r="212" spans="1:16">
+      <c r="R211">
+        <v>8.8934045093842471</v>
+      </c>
+    </row>
+    <row r="212" spans="1:18">
       <c r="A212" t="s">
         <v>449</v>
       </c>
@@ -13666,17 +13878,20 @@
       <c r="G212">
         <v>8.9184271614043453</v>
       </c>
+      <c r="H212">
+        <v>20.224776242252041</v>
+      </c>
       <c r="I212">
         <f t="shared" si="21"/>
-        <v>8.7883747008603752</v>
+        <v>10.694441624425652</v>
       </c>
       <c r="J212">
         <f t="shared" si="22"/>
-        <v>1.7011200433297786</v>
+        <v>4.5361837948209969</v>
       </c>
       <c r="K212" s="7">
         <f t="shared" si="23"/>
-        <v>0.19356480592062605</v>
+        <v>0.42416275240219603</v>
       </c>
       <c r="L212" t="s">
         <v>386</v>
@@ -13693,8 +13908,11 @@
       <c r="P212">
         <v>1</v>
       </c>
-    </row>
-    <row r="213" spans="1:16">
+      <c r="R212">
+        <v>8.833028278434222</v>
+      </c>
+    </row>
+    <row r="213" spans="1:18">
       <c r="A213" t="s">
         <v>451</v>
       </c>
@@ -13716,17 +13934,20 @@
       <c r="G213">
         <v>11.15571690391018</v>
       </c>
+      <c r="H213">
+        <v>5.4426031018389738</v>
+      </c>
       <c r="I213">
         <f t="shared" ref="I213:I244" si="24">AVERAGE(C213:H213)</f>
-        <v>6.9503740641076543</v>
+        <v>6.699078903729542</v>
       </c>
       <c r="J213">
         <f t="shared" ref="J213:J244" si="25">_xlfn.STDEV.P(C213:H213)</f>
-        <v>4.1268112485152422</v>
+        <v>3.8089222695587512</v>
       </c>
       <c r="K213" s="7">
         <f t="shared" ref="K213:K244" si="26">J213/I213</f>
-        <v>0.59375383403124449</v>
+        <v>0.56857402701112092</v>
       </c>
       <c r="L213" t="s">
         <v>386</v>
@@ -13743,8 +13964,11 @@
       <c r="P213">
         <v>1</v>
       </c>
-    </row>
-    <row r="214" spans="1:16">
+      <c r="R213">
+        <v>8.9225307456956369</v>
+      </c>
+    </row>
+    <row r="214" spans="1:18">
       <c r="A214" t="s">
         <v>453</v>
       </c>
@@ -13766,17 +13990,20 @@
       <c r="G214">
         <v>13.58617957328107</v>
       </c>
+      <c r="H214">
+        <v>5.5812222655178374</v>
+      </c>
       <c r="I214">
         <f t="shared" si="24"/>
-        <v>11.162915101284153</v>
+        <v>10.232632961989767</v>
       </c>
       <c r="J214">
         <f t="shared" si="25"/>
-        <v>4.6978639810221265</v>
+        <v>4.7664168177228898</v>
       </c>
       <c r="K214" s="7">
         <f t="shared" si="26"/>
-        <v>0.42084562485669147</v>
+        <v>0.46580551021699557</v>
       </c>
       <c r="L214" t="s">
         <v>386</v>
@@ -13793,8 +14020,11 @@
       <c r="P214">
         <v>1</v>
       </c>
-    </row>
-    <row r="215" spans="1:16">
+      <c r="R214">
+        <v>12.225007822311129</v>
+      </c>
+    </row>
+    <row r="215" spans="1:18">
       <c r="A215" t="s">
         <v>455</v>
       </c>
@@ -13816,17 +14046,20 @@
       <c r="G215">
         <v>7.2857224603766149</v>
       </c>
+      <c r="H215">
+        <v>7.7026190226245141</v>
+      </c>
       <c r="I215">
         <f t="shared" si="24"/>
-        <v>7.1102320872243849</v>
+        <v>7.2089632431244057</v>
       </c>
       <c r="J215">
         <f t="shared" si="25"/>
-        <v>2.7549475328664981</v>
+        <v>2.5245829615534778</v>
       </c>
       <c r="K215" s="7">
         <f t="shared" si="26"/>
-        <v>0.38746239209498778</v>
+        <v>0.35020055955498386</v>
       </c>
       <c r="L215" t="s">
         <v>386</v>
@@ -13843,8 +14076,11 @@
       <c r="P215">
         <v>1</v>
       </c>
-    </row>
-    <row r="216" spans="1:16">
+      <c r="R215">
+        <v>5.663604156394304</v>
+      </c>
+    </row>
+    <row r="216" spans="1:18">
       <c r="A216" t="s">
         <v>457</v>
       </c>
@@ -13866,17 +14102,20 @@
       <c r="G216">
         <v>44.985598869119023</v>
       </c>
+      <c r="H216">
+        <v>37.503519389935619</v>
+      </c>
       <c r="I216">
         <f t="shared" si="24"/>
-        <v>27.590070041672057</v>
+        <v>29.242311599715986</v>
       </c>
       <c r="J216">
         <f t="shared" si="25"/>
-        <v>13.53776582905248</v>
+        <v>12.898660028565802</v>
       </c>
       <c r="K216" s="7">
         <f t="shared" si="26"/>
-        <v>0.49067529761994194</v>
+        <v>0.44109577263006389</v>
       </c>
       <c r="L216" t="s">
         <v>386</v>
@@ -13893,8 +14132,11 @@
       <c r="P216">
         <v>1</v>
       </c>
-    </row>
-    <row r="217" spans="1:16">
+      <c r="R216">
+        <v>30.387529423238131</v>
+      </c>
+    </row>
+    <row r="217" spans="1:18">
       <c r="A217" t="s">
         <v>459</v>
       </c>
@@ -13916,17 +14158,20 @@
       <c r="G217">
         <v>78.436236136925658</v>
       </c>
+      <c r="H217">
+        <v>67.99383854319403</v>
+      </c>
       <c r="I217">
         <f t="shared" si="24"/>
-        <v>49.137096533078136</v>
+        <v>52.279886868097456</v>
       </c>
       <c r="J217">
         <f t="shared" si="25"/>
-        <v>24.13769130732426</v>
+        <v>23.128102101610452</v>
       </c>
       <c r="K217" s="7">
         <f t="shared" si="26"/>
-        <v>0.49123153402186143</v>
+        <v>0.44239005642768175</v>
       </c>
       <c r="L217" t="s">
         <v>386</v>
@@ -13943,8 +14188,11 @@
       <c r="P217">
         <v>1</v>
       </c>
-    </row>
-    <row r="218" spans="1:16">
+      <c r="R217">
+        <v>63.644095684410892</v>
+      </c>
+    </row>
+    <row r="218" spans="1:18">
       <c r="A218" t="s">
         <v>461</v>
       </c>
@@ -13966,17 +14214,20 @@
       <c r="G218">
         <v>39.34682663594613</v>
       </c>
+      <c r="H218">
+        <v>25.535325888100122</v>
+      </c>
       <c r="I218">
         <f t="shared" si="24"/>
-        <v>19.836783343533746</v>
+        <v>20.786540434294807</v>
       </c>
       <c r="J218">
         <f t="shared" si="25"/>
-        <v>11.457533197830385</v>
+        <v>10.6726792234538</v>
       </c>
       <c r="K218" s="7">
         <f t="shared" si="26"/>
-        <v>0.57759027758727977</v>
+        <v>0.51344182343327371</v>
       </c>
       <c r="L218" t="s">
         <v>386</v>
@@ -13993,8 +14244,11 @@
       <c r="P218">
         <v>1</v>
       </c>
-    </row>
-    <row r="219" spans="1:16">
+      <c r="R218">
+        <v>29.699901471340301</v>
+      </c>
+    </row>
+    <row r="219" spans="1:18">
       <c r="A219" t="s">
         <v>463</v>
       </c>
@@ -14016,17 +14270,20 @@
       <c r="G219">
         <v>22.673730773123321</v>
       </c>
+      <c r="H219">
+        <v>22.391552229287971</v>
+      </c>
       <c r="I219">
         <f t="shared" si="24"/>
-        <v>15.259297541345939</v>
+        <v>16.448006656002942</v>
       </c>
       <c r="J219">
         <f t="shared" si="25"/>
-        <v>6.3004797308820644</v>
+        <v>6.3360227400467632</v>
       </c>
       <c r="K219" s="7">
         <f t="shared" si="26"/>
-        <v>0.41289448048382005</v>
+        <v>0.38521523443902173</v>
       </c>
       <c r="L219" t="s">
         <v>386</v>
@@ -14043,8 +14300,11 @@
       <c r="P219">
         <v>1</v>
       </c>
-    </row>
-    <row r="220" spans="1:16">
+      <c r="R219">
+        <v>24.671657860364402</v>
+      </c>
+    </row>
+    <row r="220" spans="1:18">
       <c r="A220" t="s">
         <v>465</v>
       </c>
@@ -14066,17 +14326,20 @@
       <c r="G220">
         <v>10.900127739654851</v>
       </c>
+      <c r="H220">
+        <v>15.718866822038949</v>
+      </c>
       <c r="I220">
         <f t="shared" si="24"/>
-        <v>11.163514128405334</v>
+        <v>11.922739577344268</v>
       </c>
       <c r="J220">
         <f t="shared" si="25"/>
-        <v>2.8196892892618859</v>
+        <v>3.0834487431388387</v>
       </c>
       <c r="K220" s="7">
         <f t="shared" si="26"/>
-        <v>0.25258079640775877</v>
+        <v>0.25861914731393149</v>
       </c>
       <c r="L220" t="s">
         <v>386</v>
@@ -14093,8 +14356,11 @@
       <c r="P220">
         <v>1</v>
       </c>
-    </row>
-    <row r="221" spans="1:16">
+      <c r="R220">
+        <v>24.716442150748058</v>
+      </c>
+    </row>
+    <row r="221" spans="1:18">
       <c r="A221" t="s">
         <v>467</v>
       </c>
@@ -14116,17 +14382,20 @@
       <c r="G221">
         <v>18.993616280427439</v>
       </c>
+      <c r="H221">
+        <v>7.9586441958815204</v>
+      </c>
       <c r="I221">
         <f t="shared" si="24"/>
-        <v>9.936572928732307</v>
+        <v>9.6069181399238417</v>
       </c>
       <c r="J221">
         <f t="shared" si="25"/>
-        <v>4.6481032176039321</v>
+        <v>4.3066709107505696</v>
       </c>
       <c r="K221" s="7">
         <f t="shared" si="26"/>
-        <v>0.4677772961504274</v>
+        <v>0.44828849876977411</v>
       </c>
       <c r="L221" t="s">
         <v>386</v>
@@ -14143,8 +14412,11 @@
       <c r="P221">
         <v>1</v>
       </c>
-    </row>
-    <row r="222" spans="1:16">
+      <c r="R221">
+        <v>2.776372216807919</v>
+      </c>
+    </row>
+    <row r="222" spans="1:18">
       <c r="A222" t="s">
         <v>469</v>
       </c>
@@ -14166,17 +14438,20 @@
       <c r="G222">
         <v>11.27195014027256</v>
       </c>
+      <c r="H222">
+        <v>14.123033041405019</v>
+      </c>
       <c r="I222">
         <f t="shared" si="24"/>
-        <v>7.5470037428399905</v>
+        <v>8.6430086259341632</v>
       </c>
       <c r="J222">
         <f t="shared" si="25"/>
-        <v>2.3705606955756053</v>
+        <v>3.2694186835487891</v>
       </c>
       <c r="K222" s="7">
         <f t="shared" si="26"/>
-        <v>0.31410620377982568</v>
+        <v>0.3782732177009045</v>
       </c>
       <c r="L222" t="s">
         <v>386</v>
@@ -14193,8 +14468,11 @@
       <c r="P222">
         <v>1</v>
       </c>
-    </row>
-    <row r="223" spans="1:16">
+      <c r="R222">
+        <v>6.1484268921560368</v>
+      </c>
+    </row>
+    <row r="223" spans="1:18">
       <c r="A223" t="s">
         <v>471</v>
       </c>
@@ -14216,17 +14494,20 @@
       <c r="G223">
         <v>1.182965299684543</v>
       </c>
+      <c r="H223">
+        <v>7.9030441454716174</v>
+      </c>
       <c r="I223">
         <f t="shared" si="24"/>
-        <v>8.3834254442032368</v>
+        <v>8.3033618944146337</v>
       </c>
       <c r="J223">
         <f t="shared" si="25"/>
-        <v>5.0285907444187101</v>
+        <v>4.5939440124002751</v>
       </c>
       <c r="K223" s="7">
         <f t="shared" si="26"/>
-        <v>0.59982530743393869</v>
+        <v>0.55326313255001591</v>
       </c>
       <c r="L223" t="s">
         <v>386</v>
@@ -14243,8 +14524,11 @@
       <c r="P223">
         <v>1</v>
       </c>
-    </row>
-    <row r="224" spans="1:16">
+      <c r="R223">
+        <v>9.5863060283881012</v>
+      </c>
+    </row>
+    <row r="224" spans="1:18">
       <c r="A224" t="s">
         <v>473</v>
       </c>
@@ -14266,17 +14550,20 @@
       <c r="G224">
         <v>7.2176438846190827</v>
       </c>
+      <c r="H224">
+        <v>15.120870520453639</v>
+      </c>
       <c r="I224">
         <f t="shared" si="24"/>
-        <v>9.8125983785721047</v>
+        <v>10.697310402219026</v>
       </c>
       <c r="J224">
         <f t="shared" si="25"/>
-        <v>3.5130467248335324</v>
+        <v>3.7680443070174787</v>
       </c>
       <c r="K224" s="7">
         <f t="shared" si="26"/>
-        <v>0.35801391122916199</v>
+        <v>0.35224221466321515</v>
       </c>
       <c r="L224" t="s">
         <v>386</v>
@@ -14293,8 +14580,11 @@
       <c r="P224">
         <v>1</v>
       </c>
-    </row>
-    <row r="225" spans="1:16">
+      <c r="R224">
+        <v>5.0574712852081953</v>
+      </c>
+    </row>
+    <row r="225" spans="1:18">
       <c r="A225" t="s">
         <v>475</v>
       </c>
@@ -14316,17 +14606,20 @@
       <c r="G225">
         <v>9.5819379999116823</v>
       </c>
+      <c r="H225">
+        <v>8.6973232298316585</v>
+      </c>
       <c r="I225">
         <f t="shared" si="24"/>
-        <v>7.0301121336021026</v>
+        <v>7.3079806496403625</v>
       </c>
       <c r="J225">
         <f t="shared" si="25"/>
-        <v>2.218718565080982</v>
+        <v>2.1185642827684901</v>
       </c>
       <c r="K225" s="7">
         <f t="shared" si="26"/>
-        <v>0.31560215867341374</v>
+        <v>0.28989735801677963</v>
       </c>
       <c r="L225" t="s">
         <v>386</v>
@@ -14343,8 +14636,11 @@
       <c r="P225">
         <v>1</v>
       </c>
-    </row>
-    <row r="226" spans="1:16">
+      <c r="R225">
+        <v>8.6159611012787547</v>
+      </c>
+    </row>
+    <row r="226" spans="1:18">
       <c r="A226" t="s">
         <v>477</v>
       </c>
@@ -14366,17 +14662,20 @@
       <c r="G226">
         <v>5.7579530075554581</v>
       </c>
+      <c r="H226">
+        <v>12.109805584087059</v>
+      </c>
       <c r="I226">
         <f t="shared" si="24"/>
-        <v>8.7003221236344306</v>
+        <v>9.2685693670432006</v>
       </c>
       <c r="J226">
         <f t="shared" si="25"/>
-        <v>1.6881136180653462</v>
+        <v>1.9973226173529763</v>
       </c>
       <c r="K226" s="7">
         <f t="shared" si="26"/>
-        <v>0.19402886399798744</v>
+        <v>0.21549416509250871</v>
       </c>
       <c r="L226" t="s">
         <v>386</v>
@@ -14393,8 +14692,11 @@
       <c r="P226">
         <v>1</v>
       </c>
-    </row>
-    <row r="227" spans="1:16">
+      <c r="R226">
+        <v>10.408015738755079</v>
+      </c>
+    </row>
+    <row r="227" spans="1:18">
       <c r="A227" t="s">
         <v>479</v>
       </c>
@@ -14416,17 +14718,20 @@
       <c r="G227">
         <v>8.1603847784885826</v>
       </c>
+      <c r="H227">
+        <v>13.54997897495338</v>
+      </c>
       <c r="I227">
         <f t="shared" si="24"/>
-        <v>9.4676846217638886</v>
+        <v>10.148067013962136</v>
       </c>
       <c r="J227">
         <f t="shared" si="25"/>
-        <v>2.5416193321717455</v>
+        <v>2.7744894466294197</v>
       </c>
       <c r="K227" s="7">
         <f t="shared" si="26"/>
-        <v>0.26845204859582933</v>
+        <v>0.27340078093809994</v>
       </c>
       <c r="L227" t="s">
         <v>386</v>
@@ -14443,8 +14748,11 @@
       <c r="P227">
         <v>1</v>
       </c>
-    </row>
-    <row r="228" spans="1:16">
+      <c r="R227">
+        <v>9.1035382592763554</v>
+      </c>
+    </row>
+    <row r="228" spans="1:18">
       <c r="A228" t="s">
         <v>481</v>
       </c>
@@ -14466,17 +14774,20 @@
       <c r="G228">
         <v>39.123769902857568</v>
       </c>
+      <c r="H228">
+        <v>29.751320853314681</v>
+      </c>
       <c r="I228">
         <f t="shared" si="24"/>
-        <v>21.818934261074485</v>
+        <v>23.140998693114522</v>
       </c>
       <c r="J228">
         <f t="shared" si="25"/>
-        <v>9.0750494941225721</v>
+        <v>8.7960052247012648</v>
       </c>
       <c r="K228" s="7">
         <f t="shared" si="26"/>
-        <v>0.41592542447468128</v>
+        <v>0.38010482353635272</v>
       </c>
       <c r="L228" t="s">
         <v>386</v>
@@ -14493,8 +14804,11 @@
       <c r="P228">
         <v>1</v>
       </c>
-    </row>
-    <row r="229" spans="1:16">
+      <c r="R228">
+        <v>11.630091382536669</v>
+      </c>
+    </row>
+    <row r="229" spans="1:18">
       <c r="A229" t="s">
         <v>483</v>
       </c>
@@ -14516,17 +14830,20 @@
       <c r="G229">
         <v>56.360832749467043</v>
       </c>
+      <c r="H229">
+        <v>48.712627515404662</v>
+      </c>
       <c r="I229">
         <f t="shared" si="24"/>
-        <v>33.587531623417874</v>
+        <v>36.108380938749008</v>
       </c>
       <c r="J229">
         <f t="shared" si="25"/>
-        <v>19.690944782806234</v>
+        <v>18.838378249006208</v>
       </c>
       <c r="K229" s="7">
         <f t="shared" si="26"/>
-        <v>0.58625757330369965</v>
+        <v>0.52171761123717864</v>
       </c>
       <c r="L229" t="s">
         <v>386</v>
@@ -14543,8 +14860,11 @@
       <c r="P229">
         <v>1</v>
       </c>
-    </row>
-    <row r="230" spans="1:16">
+      <c r="R229">
+        <v>43.882224957425073</v>
+      </c>
+    </row>
+    <row r="230" spans="1:18">
       <c r="A230" t="s">
         <v>485</v>
       </c>
@@ -14566,17 +14886,20 @@
       <c r="G230">
         <v>40.579958887270983</v>
       </c>
+      <c r="H230">
+        <v>35.550511879635508</v>
+      </c>
       <c r="I230">
         <f t="shared" si="24"/>
-        <v>20.811336592387043</v>
+        <v>23.267865806928455</v>
       </c>
       <c r="J230">
         <f t="shared" si="25"/>
-        <v>14.977254412856718</v>
+        <v>14.73446539124083</v>
       </c>
       <c r="K230" s="7">
         <f t="shared" si="26"/>
-        <v>0.71966806871671662</v>
+        <v>0.63325384087668923</v>
       </c>
       <c r="L230" t="s">
         <v>386</v>
@@ -14593,8 +14916,11 @@
       <c r="P230">
         <v>1</v>
       </c>
-    </row>
-    <row r="231" spans="1:16">
+      <c r="R230">
+        <v>25.63279310911545</v>
+      </c>
+    </row>
+    <row r="231" spans="1:18">
       <c r="A231" t="s">
         <v>487</v>
       </c>
@@ -14616,17 +14942,20 @@
       <c r="G231">
         <v>7.5273003826764358</v>
       </c>
+      <c r="H231">
+        <v>18.307742840593789</v>
+      </c>
       <c r="I231">
         <f t="shared" si="24"/>
-        <v>8.292179140019174</v>
+        <v>9.9614397567816102</v>
       </c>
       <c r="J231">
         <f t="shared" si="25"/>
-        <v>4.5135485716373926</v>
+        <v>5.5595793267547515</v>
       </c>
       <c r="K231" s="7">
         <f t="shared" si="26"/>
-        <v>0.54431392465394279</v>
+        <v>0.55811001848099984</v>
       </c>
       <c r="L231" t="s">
         <v>386</v>
@@ -14643,8 +14972,11 @@
       <c r="P231">
         <v>1</v>
       </c>
-    </row>
-    <row r="232" spans="1:16">
+      <c r="R231">
+        <v>21.331018794319281</v>
+      </c>
+    </row>
+    <row r="232" spans="1:18">
       <c r="A232" t="s">
         <v>489</v>
       </c>
@@ -14666,17 +14998,20 @@
       <c r="G232">
         <v>5.7292368786407533</v>
       </c>
+      <c r="H232">
+        <v>16.218502455044309</v>
+      </c>
       <c r="I232">
         <f t="shared" si="24"/>
-        <v>8.9992546337641084</v>
+        <v>10.202462603977475</v>
       </c>
       <c r="J232">
         <f t="shared" si="25"/>
-        <v>4.4841989697891416</v>
+        <v>4.8984944045907106</v>
       </c>
       <c r="K232" s="7">
         <f t="shared" si="26"/>
-        <v>0.4982855972276829</v>
+        <v>0.48012863116802906</v>
       </c>
       <c r="L232" t="s">
         <v>386</v>
@@ -14693,8 +15028,11 @@
       <c r="P232">
         <v>1</v>
       </c>
-    </row>
-    <row r="233" spans="1:16">
+      <c r="R232">
+        <v>8.3489769468045019</v>
+      </c>
+    </row>
+    <row r="233" spans="1:18">
       <c r="A233" t="s">
         <v>491</v>
       </c>
@@ -14716,17 +15054,20 @@
       <c r="G233">
         <v>18.474804090843332</v>
       </c>
+      <c r="H233">
+        <v>8.4608974555202074</v>
+      </c>
       <c r="I233">
         <f t="shared" si="24"/>
-        <v>10.278533432771468</v>
+        <v>9.9755941032295912</v>
       </c>
       <c r="J233">
         <f t="shared" si="25"/>
-        <v>5.5636825422208611</v>
+        <v>5.1238979998071192</v>
       </c>
       <c r="K233" s="7">
         <f t="shared" si="26"/>
-        <v>0.54129147690291546</v>
+        <v>0.51364339274272008</v>
       </c>
       <c r="L233" t="s">
         <v>386</v>
@@ -14743,8 +15084,11 @@
       <c r="P233">
         <v>1</v>
       </c>
-    </row>
-    <row r="234" spans="1:16">
+      <c r="R233">
+        <v>9.7565575507955149</v>
+      </c>
+    </row>
+    <row r="234" spans="1:18">
       <c r="A234" t="s">
         <v>493</v>
       </c>
@@ -14766,17 +15110,20 @@
       <c r="G234">
         <v>36.493102626849499</v>
       </c>
+      <c r="H234">
+        <v>41.031614522627599</v>
+      </c>
       <c r="I234">
         <f t="shared" si="24"/>
-        <v>26.620343063888225</v>
+        <v>29.022221640344785</v>
       </c>
       <c r="J234">
         <f t="shared" si="25"/>
-        <v>8.4696911795433945</v>
+        <v>9.4140760235706509</v>
       </c>
       <c r="K234" s="7">
         <f t="shared" si="26"/>
-        <v>0.31816611676327111</v>
+        <v>0.32437475463573129</v>
       </c>
       <c r="L234" t="s">
         <v>386</v>
@@ -14793,8 +15140,11 @@
       <c r="P234">
         <v>1</v>
       </c>
-    </row>
-    <row r="235" spans="1:16">
+      <c r="R234">
+        <v>32.969105903915263</v>
+      </c>
+    </row>
+    <row r="235" spans="1:18">
       <c r="A235" t="s">
         <v>495</v>
       </c>
@@ -14816,17 +15166,20 @@
       <c r="G235">
         <v>16.028644568881301</v>
       </c>
+      <c r="H235">
+        <v>16.851569935763781</v>
+      </c>
       <c r="I235">
         <f t="shared" si="24"/>
-        <v>8.7629821151029166</v>
+        <v>10.111080085213061</v>
       </c>
       <c r="J235">
         <f t="shared" si="25"/>
-        <v>5.7290063742669242</v>
+        <v>6.0363981298509426</v>
       </c>
       <c r="K235" s="7">
         <f t="shared" si="26"/>
-        <v>0.65377360115719463</v>
+        <v>0.5970082403638427</v>
       </c>
       <c r="L235" t="s">
         <v>386</v>
@@ -14843,8 +15196,11 @@
       <c r="P235">
         <v>1</v>
       </c>
-    </row>
-    <row r="236" spans="1:16">
+      <c r="R235">
+        <v>9.5575777182820865</v>
+      </c>
+    </row>
+    <row r="236" spans="1:18">
       <c r="A236" t="s">
         <v>497</v>
       </c>
@@ -14866,17 +15222,20 @@
       <c r="G236">
         <v>18.019875396504311</v>
       </c>
+      <c r="H236">
+        <v>15.36987940891259</v>
+      </c>
       <c r="I236">
         <f t="shared" si="24"/>
-        <v>9.5756456424052381</v>
+        <v>10.541351270156463</v>
       </c>
       <c r="J236">
         <f t="shared" si="25"/>
-        <v>5.08772219249198</v>
+        <v>5.1218845217359288</v>
       </c>
       <c r="K236" s="7">
         <f t="shared" si="26"/>
-        <v>0.53131897132463557</v>
+        <v>0.48588500567630794</v>
       </c>
       <c r="L236" t="s">
         <v>386</v>
@@ -14893,8 +15252,11 @@
       <c r="P236">
         <v>1</v>
       </c>
-    </row>
-    <row r="237" spans="1:16">
+      <c r="R236">
+        <v>10.08820888967192</v>
+      </c>
+    </row>
+    <row r="237" spans="1:18">
       <c r="A237" t="s">
         <v>499</v>
       </c>
@@ -14916,17 +15278,20 @@
       <c r="G237">
         <v>12.25221564157968</v>
       </c>
+      <c r="H237">
+        <v>9.839391310670063</v>
+      </c>
       <c r="I237">
         <f t="shared" si="24"/>
-        <v>8.8060178402709486</v>
+        <v>8.978246752004134</v>
       </c>
       <c r="J237">
         <f t="shared" si="25"/>
-        <v>3.2789573768453364</v>
+        <v>3.0179377985899047</v>
       </c>
       <c r="K237" s="7">
         <f t="shared" si="26"/>
-        <v>0.37235416011199535</v>
+        <v>0.33613887899842332</v>
       </c>
       <c r="L237" t="s">
         <v>386</v>
@@ -14943,8 +15308,11 @@
       <c r="P237">
         <v>1</v>
       </c>
-    </row>
-    <row r="238" spans="1:16">
+      <c r="R237">
+        <v>10.187416578721811</v>
+      </c>
+    </row>
+    <row r="238" spans="1:18">
       <c r="A238" t="s">
         <v>501</v>
       </c>
@@ -14966,17 +15334,20 @@
       <c r="G238">
         <v>22.387061675911809</v>
       </c>
+      <c r="H238">
+        <v>11.075680217396121</v>
+      </c>
       <c r="I238">
         <f t="shared" si="24"/>
-        <v>13.578082243651641</v>
+        <v>13.161015239275722</v>
       </c>
       <c r="J238">
         <f t="shared" si="25"/>
-        <v>4.646202417907813</v>
+        <v>4.3427013698279815</v>
       </c>
       <c r="K238" s="7">
         <f t="shared" si="26"/>
-        <v>0.34218399436195196</v>
+        <v>0.32996704972032004</v>
       </c>
       <c r="L238" t="s">
         <v>386</v>
@@ -14993,8 +15364,11 @@
       <c r="P238">
         <v>1</v>
       </c>
-    </row>
-    <row r="239" spans="1:16">
+      <c r="R238">
+        <v>11.401303796366941</v>
+      </c>
+    </row>
+    <row r="239" spans="1:18">
       <c r="A239" t="s">
         <v>503</v>
       </c>
@@ -15016,17 +15390,20 @@
       <c r="G239">
         <v>13.387097218826449</v>
       </c>
+      <c r="H239">
+        <v>14.87402520625306</v>
+      </c>
       <c r="I239">
         <f t="shared" si="24"/>
-        <v>11.480986969857039</v>
+        <v>12.046493342589708</v>
       </c>
       <c r="J239">
         <f t="shared" si="25"/>
-        <v>3.313064289703052</v>
+        <v>3.278106635101171</v>
       </c>
       <c r="K239" s="7">
         <f t="shared" si="26"/>
-        <v>0.28856964112940775</v>
+        <v>0.27212123411147432</v>
       </c>
       <c r="L239" t="s">
         <v>386</v>
@@ -15043,8 +15420,11 @@
       <c r="P239">
         <v>1</v>
       </c>
-    </row>
-    <row r="240" spans="1:16">
+      <c r="R239">
+        <v>10.68140896845156</v>
+      </c>
+    </row>
+    <row r="240" spans="1:18">
       <c r="A240" t="s">
         <v>505</v>
       </c>
@@ -15066,17 +15446,20 @@
       <c r="G240">
         <v>43.306649679189377</v>
       </c>
+      <c r="H240">
+        <v>41.524520824390713</v>
+      </c>
       <c r="I240">
         <f t="shared" si="24"/>
-        <v>29.785880454948927</v>
+        <v>31.742320516522557</v>
       </c>
       <c r="J240">
         <f t="shared" si="25"/>
-        <v>12.321452159438429</v>
+        <v>12.068696753879131</v>
       </c>
       <c r="K240" s="7">
         <f t="shared" si="26"/>
-        <v>0.41366754889366442</v>
+        <v>0.38020839552663188</v>
       </c>
       <c r="L240" t="s">
         <v>386</v>
@@ -15093,8 +15476,11 @@
       <c r="P240">
         <v>1</v>
       </c>
-    </row>
-    <row r="241" spans="1:16">
+      <c r="R240">
+        <v>36.160525992599148</v>
+      </c>
+    </row>
+    <row r="241" spans="1:18">
       <c r="A241" t="s">
         <v>507</v>
       </c>
@@ -15116,17 +15502,20 @@
       <c r="G241">
         <v>62.440011985040407</v>
       </c>
+      <c r="H241">
+        <v>54.129108749910571</v>
+      </c>
       <c r="I241">
         <f t="shared" si="24"/>
-        <v>34.287310512068544</v>
+        <v>37.594276885042213</v>
       </c>
       <c r="J241">
         <f t="shared" si="25"/>
-        <v>20.708202990675623</v>
+        <v>20.298723906009851</v>
       </c>
       <c r="K241" s="7">
         <f t="shared" si="26"/>
-        <v>0.60396113551649644</v>
+        <v>0.53994186317455639</v>
       </c>
       <c r="L241" t="s">
         <v>386</v>
@@ -15143,8 +15532,11 @@
       <c r="P241">
         <v>1</v>
       </c>
-    </row>
-    <row r="242" spans="1:16">
+      <c r="R241">
+        <v>41.715393995644668</v>
+      </c>
+    </row>
+    <row r="242" spans="1:18">
       <c r="A242" t="s">
         <v>509</v>
       </c>
@@ -15166,17 +15558,20 @@
       <c r="G242">
         <v>43.036386643188287</v>
       </c>
+      <c r="H242">
+        <v>15.46976228897856</v>
+      </c>
       <c r="I242">
         <f t="shared" si="24"/>
-        <v>20.357128650222098</v>
+        <v>19.542567590014841</v>
       </c>
       <c r="J242">
         <f t="shared" si="25"/>
-        <v>11.966323183990376</v>
+        <v>11.074518381873373</v>
       </c>
       <c r="K242" s="7">
         <f t="shared" si="26"/>
-        <v>0.58781979470664802</v>
+        <v>0.5666869683762451</v>
       </c>
       <c r="L242" t="s">
         <v>386</v>
@@ -15193,8 +15588,11 @@
       <c r="P242">
         <v>1</v>
       </c>
-    </row>
-    <row r="243" spans="1:16">
+      <c r="R242">
+        <v>32.477527569856917</v>
+      </c>
+    </row>
+    <row r="243" spans="1:18">
       <c r="A243" t="s">
         <v>511</v>
       </c>
@@ -15216,17 +15614,20 @@
       <c r="G243">
         <v>28.229946166412109</v>
       </c>
+      <c r="H243">
+        <v>19.372184635131859</v>
+      </c>
       <c r="I243">
         <f t="shared" si="24"/>
-        <v>12.73707531678825</v>
+        <v>13.842926869845519</v>
       </c>
       <c r="J243">
         <f t="shared" si="25"/>
-        <v>8.8637748828299312</v>
+        <v>8.4608880108158928</v>
       </c>
       <c r="K243" s="7">
         <f t="shared" si="26"/>
-        <v>0.69590346781940826</v>
+        <v>0.61120658155368213</v>
       </c>
       <c r="L243" t="s">
         <v>386</v>
@@ -15243,8 +15644,11 @@
       <c r="P243">
         <v>1</v>
       </c>
-    </row>
-    <row r="244" spans="1:16">
+      <c r="R243">
+        <v>14.2855291155558</v>
+      </c>
+    </row>
+    <row r="244" spans="1:18">
       <c r="A244" t="s">
         <v>513</v>
       </c>
@@ -15266,17 +15670,20 @@
       <c r="G244">
         <v>2.7800546448087431</v>
       </c>
+      <c r="H244">
+        <v>10.250822628055049</v>
+      </c>
       <c r="I244">
         <f t="shared" si="24"/>
-        <v>7.8385736623891216</v>
+        <v>8.2406151566667756</v>
       </c>
       <c r="J244">
         <f t="shared" si="25"/>
-        <v>3.3454435764112493</v>
+        <v>3.1835275117492641</v>
       </c>
       <c r="K244" s="7">
         <f t="shared" si="26"/>
-        <v>0.42679238857743801</v>
+        <v>0.38632158537020683</v>
       </c>
       <c r="L244" t="s">
         <v>386</v>
@@ -15293,8 +15700,11 @@
       <c r="P244">
         <v>1</v>
       </c>
-    </row>
-    <row r="245" spans="1:16">
+      <c r="R244">
+        <v>9.0273144009971169</v>
+      </c>
+    </row>
+    <row r="245" spans="1:18">
       <c r="A245" t="s">
         <v>515</v>
       </c>
@@ -15316,17 +15726,20 @@
       <c r="G245">
         <v>16.985366145569941</v>
       </c>
+      <c r="H245">
+        <v>17.611655366730648</v>
+      </c>
       <c r="I245">
         <f t="shared" ref="I245:I250" si="27">AVERAGE(C245:H245)</f>
-        <v>10.875391595158067</v>
+        <v>11.998102223753499</v>
       </c>
       <c r="J245">
         <f t="shared" ref="J245:J250" si="28">_xlfn.STDEV.P(C245:H245)</f>
-        <v>4.5168348906286111</v>
+        <v>4.8274106553588725</v>
       </c>
       <c r="K245" s="7">
         <f t="shared" ref="K245:K250" si="29">J245/I245</f>
-        <v>0.41532618399135096</v>
+        <v>0.40234785179623683</v>
       </c>
       <c r="L245" t="s">
         <v>386</v>
@@ -15343,8 +15756,11 @@
       <c r="P245">
         <v>1</v>
       </c>
-    </row>
-    <row r="246" spans="1:16">
+      <c r="R245">
+        <v>8.9082148394256837</v>
+      </c>
+    </row>
+    <row r="246" spans="1:18">
       <c r="A246" t="s">
         <v>517</v>
       </c>
@@ -15366,17 +15782,20 @@
       <c r="G246">
         <v>14.49447899339251</v>
       </c>
+      <c r="H246">
+        <v>13.41690462426874</v>
+      </c>
       <c r="I246">
         <f t="shared" si="27"/>
-        <v>9.6691712987944936</v>
+        <v>10.293793519706869</v>
       </c>
       <c r="J246">
         <f t="shared" si="28"/>
-        <v>4.7360183741478874</v>
+        <v>4.5433823261064221</v>
       </c>
       <c r="K246" s="7">
         <f t="shared" si="29"/>
-        <v>0.48980602657627459</v>
+        <v>0.44137103754882795</v>
       </c>
       <c r="L246" t="s">
         <v>386</v>
@@ -15393,8 +15812,11 @@
       <c r="P246">
         <v>1</v>
       </c>
-    </row>
-    <row r="247" spans="1:16">
+      <c r="R246">
+        <v>10.29256095264779</v>
+      </c>
+    </row>
+    <row r="247" spans="1:18">
       <c r="A247" t="s">
         <v>519</v>
       </c>
@@ -15416,17 +15838,20 @@
       <c r="G247">
         <v>16.279926708154779</v>
       </c>
+      <c r="H247">
+        <v>33.680712756860501</v>
+      </c>
       <c r="I247">
         <f t="shared" si="27"/>
-        <v>17.557352415642193</v>
+        <v>20.24457913917858</v>
       </c>
       <c r="J247">
         <f t="shared" si="28"/>
-        <v>3.0255728042052561</v>
+        <v>6.6131948642893068</v>
       </c>
       <c r="K247" s="7">
         <f t="shared" si="29"/>
-        <v>0.17232511671348086</v>
+        <v>0.3266649713399592</v>
       </c>
       <c r="L247" t="s">
         <v>386</v>
@@ -15443,8 +15868,11 @@
       <c r="P247">
         <v>1</v>
       </c>
-    </row>
-    <row r="248" spans="1:16">
+      <c r="R247">
+        <v>23.352465364651302</v>
+      </c>
+    </row>
+    <row r="248" spans="1:18">
       <c r="A248" t="s">
         <v>521</v>
       </c>
@@ -15466,17 +15894,20 @@
       <c r="G248">
         <v>38.370866772570089</v>
       </c>
+      <c r="H248">
+        <v>43.363140379836132</v>
+      </c>
       <c r="I248">
         <f t="shared" si="27"/>
-        <v>28.229844980026286</v>
+        <v>30.752060879994591</v>
       </c>
       <c r="J248">
         <f t="shared" si="28"/>
-        <v>9.8326262060934972</v>
+        <v>10.600706595359354</v>
       </c>
       <c r="K248" s="7">
         <f t="shared" si="29"/>
-        <v>0.34830606448779522</v>
+        <v>0.34471532287631246</v>
       </c>
       <c r="L248" t="s">
         <v>386</v>
@@ -15493,8 +15924,11 @@
       <c r="P248">
         <v>1</v>
       </c>
-    </row>
-    <row r="249" spans="1:16">
+      <c r="R248">
+        <v>35.164548316459381</v>
+      </c>
+    </row>
+    <row r="249" spans="1:18">
       <c r="A249" t="s">
         <v>523</v>
       </c>
@@ -15516,17 +15950,20 @@
       <c r="G249">
         <v>16.667857307796869</v>
       </c>
+      <c r="H249">
+        <v>9.1619299943472576</v>
+      </c>
       <c r="I249">
         <f t="shared" si="27"/>
-        <v>12.912125858045068</v>
+        <v>12.287093214095433</v>
       </c>
       <c r="J249">
         <f t="shared" si="28"/>
-        <v>4.4658149676922498</v>
+        <v>4.3096305102332666</v>
       </c>
       <c r="K249" s="7">
         <f t="shared" si="29"/>
-        <v>0.34586210022958891</v>
+        <v>0.35074451175232974</v>
       </c>
       <c r="L249" t="s">
         <v>386</v>
@@ -15543,8 +15980,11 @@
       <c r="P249">
         <v>1</v>
       </c>
-    </row>
-    <row r="250" spans="1:16">
+      <c r="R249">
+        <v>22.902050939290721</v>
+      </c>
+    </row>
+    <row r="250" spans="1:18">
       <c r="A250" t="s">
         <v>525</v>
       </c>
@@ -15566,17 +16006,20 @@
       <c r="G250">
         <v>7.3361498003814809</v>
       </c>
+      <c r="H250">
+        <v>12.18067373669621</v>
+      </c>
       <c r="I250">
         <f t="shared" si="27"/>
-        <v>9.851508505690493</v>
+        <v>10.239702710858111</v>
       </c>
       <c r="J250">
         <f t="shared" si="28"/>
-        <v>3.2918767204335215</v>
+        <v>3.1279147457593477</v>
       </c>
       <c r="K250" s="7">
         <f t="shared" si="29"/>
-        <v>0.33414950802022308</v>
+        <v>0.30546929281868002</v>
       </c>
       <c r="L250" t="s">
         <v>386</v>
@@ -15593,8 +16036,11 @@
       <c r="P250">
         <v>1</v>
       </c>
-    </row>
-    <row r="251" spans="1:16">
+      <c r="R250">
+        <v>8.8011930394032554</v>
+      </c>
+    </row>
+    <row r="251" spans="1:18">
       <c r="A251" t="s">
         <v>527</v>
       </c>
@@ -15616,6 +16062,9 @@
       <c r="G251">
         <v>350.16025641025652</v>
       </c>
+      <c r="H251">
+        <v>357.43464052287578</v>
+      </c>
       <c r="I251" t="s">
         <v>37</v>
       </c>
@@ -15640,8 +16089,11 @@
       <c r="P251">
         <v>1</v>
       </c>
-    </row>
-    <row r="252" spans="1:16">
+      <c r="R251">
+        <v>18.243423307179519</v>
+      </c>
+    </row>
+    <row r="252" spans="1:18">
       <c r="A252" t="s">
         <v>529</v>
       </c>
@@ -15663,17 +16115,20 @@
       <c r="G252">
         <v>43.7433505164271</v>
       </c>
+      <c r="H252">
+        <v>41.329516778434957</v>
+      </c>
       <c r="I252">
         <f t="shared" ref="I252:I265" si="30">AVERAGE(C252:H252)</f>
-        <v>26.715853910948965</v>
+        <v>29.1514643888633</v>
       </c>
       <c r="J252">
         <f t="shared" ref="J252:J265" si="31">_xlfn.STDEV.P(C252:H252)</f>
-        <v>13.372929951155934</v>
+        <v>13.36751179412483</v>
       </c>
       <c r="K252" s="7">
         <f t="shared" ref="K252:K265" si="32">J252/I252</f>
-        <v>0.50056157649803967</v>
+        <v>0.45855369787980893</v>
       </c>
       <c r="L252" t="s">
         <v>386</v>
@@ -15690,8 +16145,11 @@
       <c r="P252">
         <v>1</v>
       </c>
-    </row>
-    <row r="253" spans="1:16">
+      <c r="R252">
+        <v>32.01976502203668</v>
+      </c>
+    </row>
+    <row r="253" spans="1:18">
       <c r="A253" t="s">
         <v>531</v>
       </c>
@@ -15713,17 +16171,20 @@
       <c r="G253">
         <v>58.666062961644577</v>
       </c>
+      <c r="H253">
+        <v>49.967245119219122</v>
+      </c>
       <c r="I253">
         <f t="shared" si="30"/>
-        <v>33.597522768724609</v>
+        <v>36.325809827140361</v>
       </c>
       <c r="J253">
         <f t="shared" si="31"/>
-        <v>19.217656092262708</v>
+        <v>18.573718154944888</v>
       </c>
       <c r="K253" s="7">
         <f t="shared" si="32"/>
-        <v>0.57199622199979916</v>
+        <v>0.51130912822947649</v>
       </c>
       <c r="L253" t="s">
         <v>386</v>
@@ -15740,8 +16201,11 @@
       <c r="P253">
         <v>1</v>
       </c>
-    </row>
-    <row r="254" spans="1:16">
+      <c r="R253">
+        <v>42.244563378756972</v>
+      </c>
+    </row>
+    <row r="254" spans="1:18">
       <c r="A254" t="s">
         <v>533</v>
       </c>
@@ -15763,17 +16227,20 @@
       <c r="G254">
         <v>42.797708957270842</v>
       </c>
+      <c r="H254">
+        <v>37.171311845659687</v>
+      </c>
       <c r="I254">
         <f t="shared" si="30"/>
-        <v>22.547330733236603</v>
+        <v>24.984660918640447</v>
       </c>
       <c r="J254">
         <f t="shared" si="31"/>
-        <v>14.968020166054798</v>
+        <v>14.710684843776756</v>
       </c>
       <c r="K254" s="7">
         <f t="shared" si="32"/>
-        <v>0.6638488760884993</v>
+        <v>0.58878865283304571</v>
       </c>
       <c r="L254" t="s">
         <v>386</v>
@@ -15790,8 +16257,11 @@
       <c r="P254">
         <v>1</v>
       </c>
-    </row>
-    <row r="255" spans="1:16">
+      <c r="R254">
+        <v>30.254139878501629</v>
+      </c>
+    </row>
+    <row r="255" spans="1:18">
       <c r="A255" t="s">
         <v>535</v>
       </c>
@@ -15813,17 +16283,20 @@
       <c r="G255">
         <v>24.884076373449592</v>
       </c>
+      <c r="H255">
+        <v>19.888987808841762</v>
+      </c>
       <c r="I255">
         <f t="shared" si="30"/>
-        <v>13.748027224463101</v>
+        <v>14.771520655192878</v>
       </c>
       <c r="J255">
         <f t="shared" si="31"/>
-        <v>6.3543534968690674</v>
+        <v>6.2358534018778675</v>
       </c>
       <c r="K255" s="7">
         <f t="shared" si="32"/>
-        <v>0.46220111388506674</v>
+        <v>0.42215378818738436</v>
       </c>
       <c r="L255" t="s">
         <v>386</v>
@@ -15840,8 +16313,11 @@
       <c r="P255">
         <v>1</v>
       </c>
-    </row>
-    <row r="256" spans="1:16">
+      <c r="R255">
+        <v>29.458627850955018</v>
+      </c>
+    </row>
+    <row r="256" spans="1:18">
       <c r="A256" t="s">
         <v>537</v>
       </c>
@@ -15863,17 +16339,20 @@
       <c r="G256">
         <v>9.3571313148655157</v>
       </c>
+      <c r="H256">
+        <v>33.489583474517659</v>
+      </c>
       <c r="I256">
         <f t="shared" si="30"/>
-        <v>11.654954453970825</v>
+        <v>15.294059290728631</v>
       </c>
       <c r="J256">
         <f t="shared" si="31"/>
-        <v>3.4600986197482841</v>
+        <v>8.7288213473082159</v>
       </c>
       <c r="K256" s="7">
         <f t="shared" si="32"/>
-        <v>0.29687791860648877</v>
+        <v>0.57073280424639716</v>
       </c>
       <c r="L256" t="s">
         <v>386</v>
@@ -15890,8 +16369,11 @@
       <c r="P256">
         <v>1</v>
       </c>
-    </row>
-    <row r="257" spans="1:16">
+      <c r="R256">
+        <v>11.15117097327186</v>
+      </c>
+    </row>
+    <row r="257" spans="1:18">
       <c r="A257" t="s">
         <v>539</v>
       </c>
@@ -15913,17 +16395,20 @@
       <c r="G257">
         <v>35.24928018165933</v>
       </c>
+      <c r="H257">
+        <v>15.153656877128491</v>
+      </c>
       <c r="I257">
         <f t="shared" si="30"/>
-        <v>14.192345421401702</v>
+        <v>14.352563997356166</v>
       </c>
       <c r="J257">
         <f t="shared" si="31"/>
-        <v>10.561864181722893</v>
+        <v>9.6482725114242687</v>
       </c>
       <c r="K257" s="7">
         <f t="shared" si="32"/>
-        <v>0.74419441382788398</v>
+        <v>0.67223337329842547</v>
       </c>
       <c r="L257" t="s">
         <v>386</v>
@@ -15940,8 +16425,11 @@
       <c r="P257">
         <v>1</v>
       </c>
-    </row>
-    <row r="258" spans="1:16">
+      <c r="R257">
+        <v>21.800193319875309</v>
+      </c>
+    </row>
+    <row r="258" spans="1:18">
       <c r="A258" t="s">
         <v>541</v>
       </c>
@@ -15963,17 +16451,20 @@
       <c r="G258">
         <v>83.558753949881037</v>
       </c>
+      <c r="H258">
+        <v>75.003904578915737</v>
+      </c>
       <c r="I258">
         <f t="shared" si="30"/>
-        <v>59.086817357582689</v>
+        <v>61.739665227804863</v>
       </c>
       <c r="J258">
         <f t="shared" si="31"/>
-        <v>16.817355264782837</v>
+        <v>16.458256515529751</v>
       </c>
       <c r="K258" s="7">
         <f t="shared" si="32"/>
-        <v>0.28462110529675777</v>
+        <v>0.26657508515478096</v>
       </c>
       <c r="L258" t="s">
         <v>386</v>
@@ -15990,8 +16481,11 @@
       <c r="P258">
         <v>1</v>
       </c>
-    </row>
-    <row r="259" spans="1:16">
+      <c r="R258">
+        <v>62.315128718244942</v>
+      </c>
+    </row>
+    <row r="259" spans="1:18">
       <c r="A259" t="s">
         <v>543</v>
       </c>
@@ -16013,17 +16507,20 @@
       <c r="G259">
         <v>14.89639133432596</v>
       </c>
+      <c r="H259">
+        <v>18.541705598893842</v>
+      </c>
       <c r="I259">
         <f t="shared" si="30"/>
-        <v>15.946069653935485</v>
+        <v>16.378675644761877</v>
       </c>
       <c r="J259">
         <f t="shared" si="31"/>
-        <v>9.0534657841918182</v>
+        <v>8.3210641529657199</v>
       </c>
       <c r="K259" s="7">
         <f t="shared" si="32"/>
-        <v>0.56775531404739765</v>
+        <v>0.50804255078016081</v>
       </c>
       <c r="L259" t="s">
         <v>386</v>
@@ -16040,8 +16537,11 @@
       <c r="P259">
         <v>1</v>
       </c>
-    </row>
-    <row r="260" spans="1:16">
+      <c r="R259">
+        <v>16.05038853828443</v>
+      </c>
+    </row>
+    <row r="260" spans="1:18">
       <c r="A260" t="s">
         <v>545</v>
       </c>
@@ -16063,17 +16563,20 @@
       <c r="G260">
         <v>17.464262845692751</v>
       </c>
+      <c r="H260">
+        <v>28.929509627072271</v>
+      </c>
       <c r="I260">
         <f t="shared" si="30"/>
-        <v>14.108050721218898</v>
+        <v>16.578293872194461</v>
       </c>
       <c r="J260">
         <f t="shared" si="31"/>
-        <v>3.2822181146636584</v>
+        <v>6.2839453571433648</v>
       </c>
       <c r="K260" s="7">
         <f t="shared" si="32"/>
-        <v>0.23264859047657885</v>
+        <v>0.37904656568327327</v>
       </c>
       <c r="L260" t="s">
         <v>386</v>
@@ -16090,8 +16593,11 @@
       <c r="P260">
         <v>1</v>
       </c>
-    </row>
-    <row r="261" spans="1:16">
+      <c r="R260">
+        <v>11.96662773884338</v>
+      </c>
+    </row>
+    <row r="261" spans="1:18">
       <c r="A261" t="s">
         <v>547</v>
       </c>
@@ -16113,17 +16619,20 @@
       <c r="G261">
         <v>40.292994650791933</v>
       </c>
+      <c r="H261">
+        <v>19.207723163410989</v>
+      </c>
       <c r="I261">
         <f t="shared" si="30"/>
-        <v>24.956677188890261</v>
+        <v>23.998518184643718</v>
       </c>
       <c r="J261">
         <f t="shared" si="31"/>
-        <v>11.857091808594829</v>
+        <v>11.034001926694549</v>
       </c>
       <c r="K261" s="7">
         <f t="shared" si="32"/>
-        <v>0.47510699116119287</v>
+        <v>0.45977846806204209</v>
       </c>
       <c r="L261" t="s">
         <v>386</v>
@@ -16140,8 +16649,11 @@
       <c r="P261">
         <v>1</v>
       </c>
-    </row>
-    <row r="262" spans="1:16">
+      <c r="R261">
+        <v>28.075877432702189</v>
+      </c>
+    </row>
+    <row r="262" spans="1:18">
       <c r="A262" t="s">
         <v>549</v>
       </c>
@@ -16163,17 +16675,20 @@
       <c r="G262">
         <v>20.159219863657821</v>
       </c>
+      <c r="H262">
+        <v>10.9946055143972</v>
+      </c>
       <c r="I262">
         <f t="shared" si="30"/>
-        <v>18.131767162175276</v>
+        <v>16.942240220878929</v>
       </c>
       <c r="J262">
         <f t="shared" si="31"/>
-        <v>7.9857464625574686</v>
+        <v>7.7600468549201924</v>
       </c>
       <c r="K262" s="7">
         <f t="shared" si="32"/>
-        <v>0.44042846960976612</v>
+        <v>0.45802956124757488</v>
       </c>
       <c r="L262" t="s">
         <v>386</v>
@@ -16190,8 +16705,11 @@
       <c r="P262">
         <v>1</v>
       </c>
-    </row>
-    <row r="263" spans="1:16">
+      <c r="R262">
+        <v>27.37521847044345</v>
+      </c>
+    </row>
+    <row r="263" spans="1:18">
       <c r="A263" t="s">
         <v>551</v>
       </c>
@@ -16213,17 +16731,20 @@
       <c r="G263">
         <v>40.814894287049768</v>
       </c>
+      <c r="H263">
+        <v>39.490772126386041</v>
+      </c>
       <c r="I263">
         <f t="shared" si="30"/>
-        <v>26.185412914276281</v>
+        <v>28.402972782961243</v>
       </c>
       <c r="J263">
         <f t="shared" si="31"/>
-        <v>12.248377671449395</v>
+        <v>12.231386750544418</v>
       </c>
       <c r="K263" s="7">
         <f t="shared" si="32"/>
-        <v>0.46775575819816778</v>
+        <v>0.4306375548788311</v>
       </c>
       <c r="L263" t="s">
         <v>386</v>
@@ -16240,8 +16761,11 @@
       <c r="P263">
         <v>1</v>
       </c>
-    </row>
-    <row r="264" spans="1:16">
+      <c r="R263">
+        <v>24.556019036620839</v>
+      </c>
+    </row>
+    <row r="264" spans="1:18">
       <c r="A264" t="s">
         <v>553</v>
       </c>
@@ -16263,17 +16787,20 @@
       <c r="G264">
         <v>51.022474448356967</v>
       </c>
+      <c r="H264">
+        <v>48.517920682377607</v>
+      </c>
       <c r="I264">
         <f t="shared" si="30"/>
-        <v>30.737674891133036</v>
+        <v>33.701049189673796</v>
       </c>
       <c r="J264">
         <f t="shared" si="31"/>
-        <v>14.735746349800802</v>
+        <v>14.995325490664845</v>
       </c>
       <c r="K264" s="7">
         <f t="shared" si="32"/>
-        <v>0.47940341623079807</v>
+        <v>0.44495129532226857</v>
       </c>
       <c r="L264" t="s">
         <v>386</v>
@@ -16290,8 +16817,11 @@
       <c r="P264">
         <v>1</v>
       </c>
-    </row>
-    <row r="265" spans="1:16">
+      <c r="R264">
+        <v>39.355472473674688</v>
+      </c>
+    </row>
+    <row r="265" spans="1:18">
       <c r="A265" t="s">
         <v>555</v>
       </c>
@@ -16313,17 +16843,20 @@
       <c r="G265">
         <v>61.012420455950974</v>
       </c>
+      <c r="H265">
+        <v>53.105797652005201</v>
+      </c>
       <c r="I265">
         <f t="shared" si="30"/>
-        <v>35.8082543674061</v>
+        <v>38.691178248172619</v>
       </c>
       <c r="J265">
         <f t="shared" si="31"/>
-        <v>20.576400308515289</v>
+        <v>19.858997756475336</v>
       </c>
       <c r="K265" s="7">
         <f t="shared" si="32"/>
-        <v>0.57462729395836265</v>
+        <v>0.51326939771893032</v>
       </c>
       <c r="L265" t="s">
         <v>386</v>
@@ -16340,8 +16873,11 @@
       <c r="P265">
         <v>1</v>
       </c>
-    </row>
-    <row r="266" spans="1:16">
+      <c r="R265">
+        <v>47.445940242342303</v>
+      </c>
+    </row>
+    <row r="266" spans="1:18">
       <c r="A266" t="s">
         <v>557</v>
       </c>
@@ -16363,6 +16899,9 @@
       <c r="G266">
         <v>410.72530864197529</v>
       </c>
+      <c r="H266">
+        <v>401.20192307692321</v>
+      </c>
       <c r="I266" t="s">
         <v>37</v>
       </c>
@@ -16387,8 +16926,11 @@
       <c r="P266">
         <v>1</v>
       </c>
-    </row>
-    <row r="267" spans="1:16">
+      <c r="R266">
+        <v>38.674173290335133</v>
+      </c>
+    </row>
+    <row r="267" spans="1:18">
       <c r="A267" t="s">
         <v>559</v>
       </c>
@@ -16410,17 +16952,20 @@
       <c r="G267">
         <v>55.543098876913213</v>
       </c>
+      <c r="H267">
+        <v>51.343166450700593</v>
+      </c>
       <c r="I267">
         <f>AVERAGE(C267:H267)</f>
-        <v>31.533636950459009</v>
+        <v>34.835225200499274</v>
       </c>
       <c r="J267">
         <f>_xlfn.STDEV.P(C267:H267)</f>
-        <v>17.301572795134611</v>
+        <v>17.434337073291264</v>
       </c>
       <c r="K267" s="7">
         <f>J267/I267</f>
-        <v>0.54867038719055106</v>
+        <v>0.50048010233737161</v>
       </c>
       <c r="L267" t="s">
         <v>386</v>
@@ -16437,8 +16982,11 @@
       <c r="P267">
         <v>1</v>
       </c>
-    </row>
-    <row r="268" spans="1:16">
+      <c r="R267">
+        <v>35.905190819583453</v>
+      </c>
+    </row>
+    <row r="268" spans="1:18">
       <c r="A268" t="s">
         <v>561</v>
       </c>
@@ -16460,17 +17008,20 @@
       <c r="G268">
         <v>73.146660111629672</v>
       </c>
+      <c r="H268">
+        <v>70.40888542841671</v>
+      </c>
       <c r="I268">
         <f>AVERAGE(C268:H268)</f>
-        <v>45.285413401953051</v>
+        <v>49.472658739696989</v>
       </c>
       <c r="J268">
         <f>_xlfn.STDEV.P(C268:H268)</f>
-        <v>19.100996747859806</v>
+        <v>19.791543182895509</v>
       </c>
       <c r="K268" s="7">
         <f>J268/I268</f>
-        <v>0.42179137415219059</v>
+        <v>0.40005012237223314</v>
       </c>
       <c r="L268" t="s">
         <v>386</v>
@@ -16487,8 +17038,11 @@
       <c r="P268">
         <v>1</v>
       </c>
-    </row>
-    <row r="269" spans="1:16">
+      <c r="R268">
+        <v>51.316625039898383</v>
+      </c>
+    </row>
+    <row r="269" spans="1:18">
       <c r="A269" t="s">
         <v>563</v>
       </c>
@@ -16510,17 +17064,20 @@
       <c r="G269">
         <v>53.53558260249261</v>
       </c>
+      <c r="H269">
+        <v>49.018155753719739</v>
+      </c>
       <c r="I269">
         <f>AVERAGE(C269:H269)</f>
-        <v>29.116731804933284</v>
+        <v>32.433635796397688</v>
       </c>
       <c r="J269">
         <f>_xlfn.STDEV.P(C269:H269)</f>
-        <v>16.920817151594154</v>
+        <v>17.134885604355965</v>
       </c>
       <c r="K269" s="7">
         <f>J269/I269</f>
-        <v>0.58113723974773979</v>
+        <v>0.52830603734716319</v>
       </c>
       <c r="L269" t="s">
         <v>386</v>
@@ -16537,8 +17094,11 @@
       <c r="P269">
         <v>1</v>
       </c>
-    </row>
-    <row r="270" spans="1:16">
+      <c r="R269">
+        <v>34.505611946694373</v>
+      </c>
+    </row>
+    <row r="270" spans="1:18">
       <c r="A270" t="s">
         <v>565</v>
       </c>
@@ -16560,17 +17120,20 @@
       <c r="G270">
         <v>58.773355359141512</v>
       </c>
+      <c r="H270">
+        <v>48.436283334740892</v>
+      </c>
       <c r="I270">
         <f>AVERAGE(C270:H270)</f>
-        <v>31.933838532728238</v>
+        <v>34.684245999730344</v>
       </c>
       <c r="J270">
         <f>_xlfn.STDEV.P(C270:H270)</f>
-        <v>17.488569232141153</v>
+        <v>17.108440928253319</v>
       </c>
       <c r="K270" s="7">
         <f>J270/I270</f>
-        <v>0.54765008015611816</v>
+        <v>0.49326258752709606</v>
       </c>
       <c r="L270" t="s">
         <v>386</v>
@@ -16587,8 +17150,11 @@
       <c r="P270">
         <v>1</v>
       </c>
-    </row>
-    <row r="271" spans="1:16">
+      <c r="R270">
+        <v>37.20617317293366</v>
+      </c>
+    </row>
+    <row r="271" spans="1:18">
       <c r="A271" s="4" t="s">
         <v>16</v>
       </c>
@@ -16610,17 +17176,20 @@
       <c r="G271">
         <v>84.532944201257422</v>
       </c>
+      <c r="H271">
+        <v>89.839164896926007</v>
+      </c>
       <c r="I271">
         <f>AVERAGE(C271:H271)</f>
-        <v>62.664750925473257</v>
+        <v>68.099633719763801</v>
       </c>
       <c r="J271">
         <f>_xlfn.STDEV.P(C271:H271)</f>
-        <v>20.79442730604773</v>
+        <v>21.542478259009702</v>
       </c>
       <c r="K271" s="7">
         <f>J271/I271</f>
-        <v>0.33183611199186597</v>
+        <v>0.31633765238237493</v>
       </c>
       <c r="L271" t="s">
         <v>18</v>
@@ -16636,6 +17205,9 @@
       </c>
       <c r="P271">
         <v>1</v>
+      </c>
+      <c r="R271">
+        <v>64.82870094818027</v>
       </c>
     </row>
   </sheetData>
@@ -16674,7 +17246,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
repeat kfold for kernel normalisation adjusting
</commit_message>
<xml_diff>
--- a/data/Results_Masterfile.xlsx
+++ b/data/Results_Masterfile.xlsx
@@ -2217,8 +2217,8 @@
   </sheetPr>
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A92" activeCellId="0" sqref="A92"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F106" activeCellId="0" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added Rep4 for Plate 4.
</commit_message>
<xml_diff>
--- a/data/Results_Masterfile.xlsx
+++ b/data/Results_Masterfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOL428\Documents\Repos\SynbioML\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85916326-DB2F-4FDE-ABF2-624A34C2A41B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9215DA13-B57C-4960-8B85-87D7FC3A0349}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3081,8 +3081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="K276" sqref="K276"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="G274" sqref="G274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -18244,17 +18244,20 @@
       <c r="E271">
         <v>70.450757151683831</v>
       </c>
+      <c r="F271">
+        <v>83.065130222739668</v>
+      </c>
       <c r="I271" s="14">
         <f t="shared" si="25"/>
-        <v>65.580402895989835</v>
+        <v>69.9515847276773</v>
       </c>
       <c r="J271">
         <f t="shared" ref="J271:J334" si="26">_xlfn.STDEV.P(C271:H271)</f>
-        <v>9.7903791766799095</v>
+        <v>11.367072408250003</v>
       </c>
       <c r="K271" s="8">
         <f t="shared" ref="K271:K334" si="27">J271/I271</f>
-        <v>0.14928818281594577</v>
+        <v>0.16249914069141116</v>
       </c>
       <c r="L271" t="s">
         <v>847</v>
@@ -18288,17 +18291,20 @@
       <c r="E272">
         <v>74.303543033773678</v>
       </c>
+      <c r="F272">
+        <v>82.587079759994396</v>
+      </c>
       <c r="I272" s="14">
         <f t="shared" si="25"/>
-        <v>68.143369443940998</v>
+        <v>71.754297022954347</v>
       </c>
       <c r="J272">
         <f t="shared" si="26"/>
-        <v>11.225274245015138</v>
+        <v>11.559475781776944</v>
       </c>
       <c r="K272" s="8">
         <f t="shared" si="27"/>
-        <v>0.1647302494228694</v>
+        <v>0.16109802842997742</v>
       </c>
       <c r="L272" t="s">
         <v>847</v>
@@ -18332,17 +18338,20 @@
       <c r="E273">
         <v>54.594405007949113</v>
       </c>
+      <c r="F273">
+        <v>56.263396249730341</v>
+      </c>
       <c r="I273" s="14">
         <f t="shared" si="25"/>
-        <v>51.786280043169427</v>
+        <v>52.905559094809654</v>
       </c>
       <c r="J273">
         <f t="shared" si="26"/>
-        <v>4.1143833346737733</v>
+        <v>4.0564109080322366</v>
       </c>
       <c r="K273" s="8">
         <f t="shared" si="27"/>
-        <v>7.9449292964159479E-2</v>
+        <v>7.6672678210675874E-2</v>
       </c>
       <c r="L273" t="s">
         <v>847</v>
@@ -18376,17 +18385,20 @@
       <c r="E274">
         <v>72.037888175290945</v>
       </c>
+      <c r="F274">
+        <v>86.82215934586003</v>
+      </c>
       <c r="I274" s="14">
         <f t="shared" si="25"/>
-        <v>67.500311892644561</v>
+        <v>72.330773755948428</v>
       </c>
       <c r="J274">
         <f t="shared" si="26"/>
-        <v>11.726295349538631</v>
+        <v>13.157871689865249</v>
       </c>
       <c r="K274" s="8">
         <f t="shared" si="27"/>
-        <v>0.17372209136142427</v>
+        <v>0.1819124973591639</v>
       </c>
       <c r="L274" t="s">
         <v>847</v>
@@ -18420,17 +18432,20 @@
       <c r="E275">
         <v>62.157774286345749</v>
       </c>
+      <c r="F275">
+        <v>66.649424052389634</v>
+      </c>
       <c r="I275" s="14">
         <f t="shared" si="25"/>
-        <v>58.334679737182967</v>
+        <v>60.413365815984633</v>
       </c>
       <c r="J275">
         <f t="shared" si="26"/>
-        <v>5.5103765844013601</v>
+        <v>5.9779591014869498</v>
       </c>
       <c r="K275" s="8">
         <f t="shared" si="27"/>
-        <v>9.4461418306013331E-2</v>
+        <v>9.8950936117273167E-2</v>
       </c>
       <c r="L275" t="s">
         <v>847</v>
@@ -18464,17 +18479,20 @@
       <c r="E276">
         <v>56.275467645094992</v>
       </c>
+      <c r="F276">
+        <v>63.862375215489742</v>
+      </c>
       <c r="I276" s="14">
         <f t="shared" si="25"/>
-        <v>55.045071472856911</v>
+        <v>57.249397408515122</v>
       </c>
       <c r="J276">
         <f t="shared" si="26"/>
-        <v>2.9455900910736141</v>
+        <v>4.5917898721870536</v>
       </c>
       <c r="K276" s="8">
         <f t="shared" si="27"/>
-        <v>5.3512331118074831E-2</v>
+        <v>8.020678085782057E-2</v>
       </c>
       <c r="L276" t="s">
         <v>847</v>
@@ -18508,17 +18526,20 @@
       <c r="E277">
         <v>43.630078372552937</v>
       </c>
+      <c r="F277">
+        <v>50.020114144528549</v>
+      </c>
       <c r="I277" s="14">
         <f t="shared" si="25"/>
-        <v>42.354936024426983</v>
+        <v>44.271230554452373</v>
       </c>
       <c r="J277">
         <f t="shared" si="26"/>
-        <v>3.6207276737661731</v>
+        <v>4.5660492598194313</v>
       </c>
       <c r="K277" s="8">
         <f t="shared" si="27"/>
-        <v>8.5485376997807838E-2</v>
+        <v>0.10313806963651753</v>
       </c>
       <c r="L277" t="s">
         <v>847</v>
@@ -18552,17 +18573,20 @@
       <c r="E278">
         <v>46.177300103649742</v>
       </c>
+      <c r="F278">
+        <v>50.46158798194049</v>
+      </c>
       <c r="I278" s="14">
         <f t="shared" si="25"/>
-        <v>43.916024856807674</v>
+        <v>45.552415638090878</v>
       </c>
       <c r="J278">
         <f t="shared" si="26"/>
-        <v>3.7832163135316139</v>
+        <v>4.3321898184907317</v>
       </c>
       <c r="K278" s="8">
         <f t="shared" si="27"/>
-        <v>8.6146601971994197E-2</v>
+        <v>9.5103404678020184E-2</v>
       </c>
       <c r="L278" t="s">
         <v>847</v>
@@ -18596,17 +18620,20 @@
       <c r="E279">
         <v>50.163482013707188</v>
       </c>
+      <c r="F279">
+        <v>58.577819048872428</v>
+      </c>
       <c r="I279" s="14">
         <f t="shared" si="25"/>
-        <v>49.110326541985842</v>
+        <v>51.477199668707485</v>
       </c>
       <c r="J279">
         <f t="shared" si="26"/>
-        <v>4.4798732141196913</v>
+        <v>5.6443080359714886</v>
       </c>
       <c r="K279" s="8">
         <f t="shared" si="27"/>
-        <v>9.1220595128597204E-2</v>
+        <v>0.1096467576382678</v>
       </c>
       <c r="L279" t="s">
         <v>847</v>
@@ -18640,17 +18667,20 @@
       <c r="E280">
         <v>35.468997733769221</v>
       </c>
+      <c r="F280">
+        <v>45.332108400493119</v>
+      </c>
       <c r="I280" s="14">
         <f t="shared" si="25"/>
-        <v>32.541618777176581</v>
+        <v>35.739241183005717</v>
       </c>
       <c r="J280">
         <f t="shared" si="26"/>
-        <v>2.7921389586766026</v>
+        <v>6.0432935659457465</v>
       </c>
       <c r="K280" s="8">
         <f t="shared" si="27"/>
-        <v>8.5802091708937961E-2</v>
+        <v>0.16909406484039674</v>
       </c>
       <c r="L280" t="s">
         <v>847</v>
@@ -18684,17 +18714,20 @@
       <c r="E281">
         <v>70.365903061486293</v>
       </c>
+      <c r="F281">
+        <v>70.601183311142151</v>
+      </c>
       <c r="I281" s="14">
         <f t="shared" si="25"/>
-        <v>64.586186442269792</v>
+        <v>66.089935659487878</v>
       </c>
       <c r="J281">
         <f t="shared" si="26"/>
-        <v>7.0670575866735028</v>
+        <v>6.6514105515199597</v>
       </c>
       <c r="K281" s="8">
         <f t="shared" si="27"/>
-        <v>0.10942057390229062</v>
+        <v>0.10064180703382304</v>
       </c>
       <c r="L281" t="s">
         <v>847</v>
@@ -18728,17 +18761,20 @@
       <c r="E282">
         <v>38.618477632947567</v>
       </c>
+      <c r="F282">
+        <v>52.250425761063603</v>
+      </c>
       <c r="I282" s="14">
         <f t="shared" si="25"/>
-        <v>42.28378393306928</v>
+        <v>44.775444390067861</v>
       </c>
       <c r="J282">
         <f t="shared" si="26"/>
-        <v>5.4644650887410791</v>
+        <v>6.404716974891512</v>
       </c>
       <c r="K282" s="8">
         <f t="shared" si="27"/>
-        <v>0.12923311445803301</v>
+        <v>0.14304083548777047</v>
       </c>
       <c r="L282" t="s">
         <v>847</v>
@@ -18772,17 +18808,20 @@
       <c r="E283">
         <v>79.583741412890419</v>
       </c>
+      <c r="F283">
+        <v>89.136395070589543</v>
+      </c>
       <c r="I283" s="14">
         <f t="shared" si="25"/>
-        <v>74.175544821625053</v>
+        <v>77.915757383866179</v>
       </c>
       <c r="J283">
         <f t="shared" si="26"/>
-        <v>10.745251539202577</v>
+        <v>11.338557801272152</v>
       </c>
       <c r="K283" s="8">
         <f t="shared" si="27"/>
-        <v>0.14486245520733834</v>
+        <v>0.14552329569756578</v>
       </c>
       <c r="L283" t="s">
         <v>847</v>
@@ -18816,17 +18855,20 @@
       <c r="E284">
         <v>69.901823834207235</v>
       </c>
+      <c r="F284">
+        <v>79.347156119293885</v>
+      </c>
       <c r="I284" s="14">
         <f t="shared" si="25"/>
-        <v>63.629525011105009</v>
+        <v>67.558932788152219</v>
       </c>
       <c r="J284">
         <f t="shared" si="26"/>
-        <v>8.8359136042181419</v>
+        <v>10.240886843963464</v>
       </c>
       <c r="K284" s="8">
         <f t="shared" si="27"/>
-        <v>0.13886499392657803</v>
+        <v>0.151584496991335</v>
       </c>
       <c r="L284" t="s">
         <v>847</v>
@@ -18860,17 +18902,20 @@
       <c r="E285">
         <v>46.994036542262648</v>
       </c>
+      <c r="F285">
+        <v>45.750606145881719</v>
+      </c>
       <c r="I285" s="14">
         <f t="shared" si="25"/>
-        <v>44.493342966521418</v>
+        <v>44.807658761361495</v>
       </c>
       <c r="J285">
         <f t="shared" si="26"/>
-        <v>2.2152960816632752</v>
+        <v>1.9942506872839083</v>
       </c>
       <c r="K285" s="8">
         <f t="shared" si="27"/>
-        <v>4.978938272474049E-2</v>
+        <v>4.4506915612461971E-2</v>
       </c>
       <c r="L285" t="s">
         <v>847</v>
@@ -18904,17 +18949,20 @@
       <c r="E286">
         <v>64.011740630241803</v>
       </c>
+      <c r="F286">
+        <v>68.024863647142482</v>
+      </c>
       <c r="I286" s="14">
         <f t="shared" si="25"/>
-        <v>62.448662517883655</v>
+        <v>63.842712800198356</v>
       </c>
       <c r="J286">
         <f t="shared" si="26"/>
-        <v>1.5513536233042082</v>
+        <v>2.7631779018495104</v>
       </c>
       <c r="K286" s="8">
         <f t="shared" si="27"/>
-        <v>2.4842063236501524E-2</v>
+        <v>4.3281022698661471E-2</v>
       </c>
       <c r="L286" t="s">
         <v>847</v>
@@ -18948,17 +18996,20 @@
       <c r="E287">
         <v>13.472394828750931</v>
       </c>
+      <c r="F287">
+        <v>18.989488228185149</v>
+      </c>
       <c r="I287" s="14">
         <f t="shared" si="25"/>
-        <v>19.797865297580653</v>
+        <v>19.595771030231777</v>
       </c>
       <c r="J287">
         <f t="shared" si="26"/>
-        <v>7.2137037668618351</v>
+        <v>6.2570494488787078</v>
       </c>
       <c r="K287" s="8">
         <f t="shared" si="27"/>
-        <v>0.36436775674715632</v>
+        <v>0.31930611146790377</v>
       </c>
       <c r="L287" t="s">
         <v>847</v>
@@ -18992,17 +19043,20 @@
       <c r="E288">
         <v>19.362898559677529</v>
       </c>
+      <c r="F288">
+        <v>13.569693423040951</v>
+      </c>
       <c r="I288" s="14">
         <f t="shared" si="25"/>
-        <v>21.068704125759897</v>
+        <v>19.19395145008016</v>
       </c>
       <c r="J288">
         <f t="shared" si="26"/>
-        <v>7.2324491750791395</v>
+        <v>7.0551636116735308</v>
       </c>
       <c r="K288" s="8">
         <f t="shared" si="27"/>
-        <v>0.34327926064689956</v>
+        <v>0.36757223388954996</v>
       </c>
       <c r="L288" t="s">
         <v>847</v>
@@ -19036,17 +19090,20 @@
       <c r="E289">
         <v>56.549436474791108</v>
       </c>
+      <c r="F289">
+        <v>69.131080256621999</v>
+      </c>
       <c r="I289" s="14">
         <f t="shared" si="25"/>
-        <v>61.123088569831395</v>
+        <v>63.125086491529046</v>
       </c>
       <c r="J289">
         <f t="shared" si="26"/>
-        <v>4.475713537908339</v>
+        <v>5.2007687691827975</v>
       </c>
       <c r="K289" s="8">
         <f t="shared" si="27"/>
-        <v>7.3224597163393718E-2</v>
+        <v>8.2388303260078774E-2</v>
       </c>
       <c r="L289" t="s">
         <v>847</v>
@@ -19080,17 +19137,20 @@
       <c r="E290">
         <v>20.113246113891929</v>
       </c>
+      <c r="F290">
+        <v>26.09679026936282</v>
+      </c>
       <c r="I290" s="14">
         <f t="shared" si="25"/>
-        <v>28.054143914287664</v>
+        <v>27.564805503056455</v>
       </c>
       <c r="J290">
         <f t="shared" si="26"/>
-        <v>8.203494239001035</v>
+        <v>7.1548126837193307</v>
       </c>
       <c r="K290" s="8">
         <f t="shared" si="27"/>
-        <v>0.29241648806196813</v>
+        <v>0.25956332914904795</v>
       </c>
       <c r="L290" t="s">
         <v>847</v>
@@ -19124,17 +19184,20 @@
       <c r="E291">
         <v>16.542663596905829</v>
       </c>
+      <c r="F291">
+        <v>2.6991478265963029</v>
+      </c>
       <c r="I291" s="14">
         <f t="shared" si="25"/>
-        <v>16.100883454929171</v>
+        <v>12.750449547845953</v>
       </c>
       <c r="J291">
         <f t="shared" si="26"/>
-        <v>9.7476160070921019</v>
+        <v>10.243936521839997</v>
       </c>
       <c r="K291" s="8">
         <f t="shared" si="27"/>
-        <v>0.60540876743679173</v>
+        <v>0.8034176742866761</v>
       </c>
       <c r="L291" t="s">
         <v>847</v>
@@ -19168,17 +19231,20 @@
       <c r="E292">
         <v>55.064030157826579</v>
       </c>
+      <c r="F292">
+        <v>64.467007333367704</v>
+      </c>
       <c r="I292" s="14">
         <f t="shared" si="25"/>
-        <v>59.609468240090223</v>
+        <v>60.82385301340959</v>
       </c>
       <c r="J292">
         <f t="shared" si="26"/>
-        <v>6.3627691894323668</v>
+        <v>5.8981196114949768</v>
       </c>
       <c r="K292" s="8">
         <f t="shared" si="27"/>
-        <v>0.10674091511443982</v>
+        <v>9.6970502841946596E-2</v>
       </c>
       <c r="L292" t="s">
         <v>847</v>
@@ -19212,17 +19278,20 @@
       <c r="E293">
         <v>12.540205695787121</v>
       </c>
+      <c r="F293">
+        <v>17.323546065493758</v>
+      </c>
       <c r="I293" s="14">
         <f t="shared" si="25"/>
-        <v>15.975286831841951</v>
+        <v>16.312351640254903</v>
       </c>
       <c r="J293">
         <f t="shared" si="26"/>
-        <v>2.7295259576720374</v>
+        <v>2.4348659142579909</v>
       </c>
       <c r="K293" s="8">
         <f t="shared" si="27"/>
-        <v>0.17085927698221637</v>
+        <v>0.14926516838009646</v>
       </c>
       <c r="L293" t="s">
         <v>847</v>
@@ -19256,17 +19325,20 @@
       <c r="E294">
         <v>17.394768992752901</v>
       </c>
+      <c r="F294">
+        <v>21.104464673896501</v>
+      </c>
       <c r="I294" s="14">
         <f t="shared" si="25"/>
-        <v>27.421275996480674</v>
+        <v>25.842073165834631</v>
       </c>
       <c r="J294">
         <f t="shared" si="26"/>
-        <v>7.1991404912227912</v>
+        <v>6.8082569428770885</v>
       </c>
       <c r="K294" s="8">
         <f t="shared" si="27"/>
-        <v>0.26253849354591485</v>
+        <v>0.2634562985402491</v>
       </c>
       <c r="L294" t="s">
         <v>847</v>
@@ -19300,17 +19372,20 @@
       <c r="E295">
         <v>54.008316469934513</v>
       </c>
+      <c r="F295">
+        <v>60.918689629508371</v>
+      </c>
       <c r="I295" s="14">
         <f t="shared" si="25"/>
-        <v>51.87894173208349</v>
+        <v>54.138878706439712</v>
       </c>
       <c r="J295">
         <f t="shared" si="26"/>
-        <v>7.9464517318397796</v>
+        <v>7.9171659531066449</v>
       </c>
       <c r="K295" s="8">
         <f t="shared" si="27"/>
-        <v>0.1531729728196336</v>
+        <v>0.14623808512984429</v>
       </c>
       <c r="L295" t="s">
         <v>847</v>
@@ -19344,17 +19419,20 @@
       <c r="E296">
         <v>38.04015402558155</v>
       </c>
+      <c r="F296">
+        <v>45.159103384323103</v>
+      </c>
       <c r="I296" s="14">
         <f t="shared" si="25"/>
-        <v>37.904504236293036</v>
+        <v>39.718154023300556</v>
       </c>
       <c r="J296">
         <f t="shared" si="26"/>
-        <v>1.241954679755914</v>
+        <v>3.3203637179777385</v>
       </c>
       <c r="K296" s="8">
         <f t="shared" si="27"/>
-        <v>3.2765358755616161E-2</v>
+        <v>8.3598137920253182E-2</v>
       </c>
       <c r="L296" t="s">
         <v>847</v>
@@ -19388,17 +19466,20 @@
       <c r="E297">
         <v>28.360162008830631</v>
       </c>
+      <c r="F297">
+        <v>16.919184466310401</v>
+      </c>
       <c r="I297" s="14">
         <f t="shared" si="25"/>
-        <v>23.010780683737764</v>
+        <v>21.487881629380922</v>
       </c>
       <c r="J297">
         <f t="shared" si="26"/>
-        <v>8.773652869925666</v>
+        <v>8.0430344460750085</v>
       </c>
       <c r="K297" s="8">
         <f t="shared" si="27"/>
-        <v>0.38128445055869853</v>
+        <v>0.37430560093357756</v>
       </c>
       <c r="L297" t="s">
         <v>847</v>
@@ -19432,17 +19513,20 @@
       <c r="E298">
         <v>9.2234944650871515</v>
       </c>
+      <c r="F298">
+        <v>18.373507206732999</v>
+      </c>
       <c r="I298" s="14">
         <f t="shared" si="25"/>
-        <v>18.072505559233569</v>
+        <v>18.147755971108428</v>
       </c>
       <c r="J298">
         <f t="shared" si="26"/>
-        <v>9.3761753827790724</v>
+        <v>8.1210520549948573</v>
       </c>
       <c r="K298" s="8">
         <f t="shared" si="27"/>
-        <v>0.51880882548621576</v>
+        <v>0.44749621208945761</v>
       </c>
       <c r="L298" t="s">
         <v>847</v>
@@ -19476,17 +19560,20 @@
       <c r="E299">
         <v>14.57990433998298</v>
       </c>
+      <c r="F299">
+        <v>8.0001242060555349</v>
+      </c>
       <c r="I299" s="14">
         <f t="shared" si="25"/>
-        <v>18.74988616708314</v>
+        <v>16.06244567682624</v>
       </c>
       <c r="J299">
         <f t="shared" si="26"/>
-        <v>4.8245621455750332</v>
+        <v>6.2549427725922033</v>
       </c>
       <c r="K299" s="8">
         <f t="shared" si="27"/>
-        <v>0.25731154325858901</v>
+        <v>0.38941409661023119</v>
       </c>
       <c r="L299" t="s">
         <v>847</v>
@@ -19520,17 +19607,20 @@
       <c r="E300">
         <v>14.31757441413291</v>
       </c>
+      <c r="F300">
+        <v>16.456885437463711</v>
+      </c>
       <c r="I300" s="14">
         <f t="shared" si="25"/>
-        <v>19.384827269261645</v>
+        <v>18.652841811312161</v>
       </c>
       <c r="J300">
         <f t="shared" si="26"/>
-        <v>4.7575329039009677</v>
+        <v>4.3108001149118254</v>
       </c>
       <c r="K300" s="8">
         <f t="shared" si="27"/>
-        <v>0.24542560208648065</v>
+        <v>0.23110688218550737</v>
       </c>
       <c r="L300" t="s">
         <v>847</v>
@@ -19564,17 +19654,20 @@
       <c r="E301">
         <v>11.770384055606931</v>
       </c>
+      <c r="F301">
+        <v>14.915221188115281</v>
+      </c>
       <c r="I301" s="14">
         <f t="shared" si="25"/>
-        <v>11.937855716888146</v>
+        <v>12.682197084694931</v>
       </c>
       <c r="J301">
         <f t="shared" si="26"/>
-        <v>5.0009882834027044</v>
+        <v>4.5187990742600794</v>
       </c>
       <c r="K301" s="8">
         <f t="shared" si="27"/>
-        <v>0.4189184726305536</v>
+        <v>0.35631042823908132</v>
       </c>
       <c r="L301" t="s">
         <v>847</v>
@@ -19608,17 +19701,20 @@
       <c r="E302">
         <v>7.8698508223269634</v>
       </c>
+      <c r="F302">
+        <v>5.4030328730850981</v>
+      </c>
       <c r="I302" s="14">
         <f t="shared" si="25"/>
-        <v>9.3929574738983845</v>
+        <v>8.3954763236950622</v>
       </c>
       <c r="J302">
         <f t="shared" si="26"/>
-        <v>7.5657455295180984</v>
+        <v>6.7760818323054632</v>
       </c>
       <c r="K302" s="8">
         <f t="shared" si="27"/>
-        <v>0.80547000777360767</v>
+        <v>0.80711106446467085</v>
       </c>
       <c r="L302" t="s">
         <v>847</v>
@@ -19652,17 +19748,20 @@
       <c r="E303">
         <v>13.36773058774352</v>
       </c>
+      <c r="F303">
+        <v>7.7493783108749836</v>
+      </c>
       <c r="I303" s="14">
         <f t="shared" si="25"/>
-        <v>13.627756213668215</v>
+        <v>12.158161737969907</v>
       </c>
       <c r="J303">
         <f t="shared" si="26"/>
-        <v>0.29936286214740632</v>
+        <v>2.5585811226994122</v>
       </c>
       <c r="K303" s="8">
         <f t="shared" si="27"/>
-        <v>2.1967142459384081E-2</v>
+        <v>0.21044144483692548</v>
       </c>
       <c r="L303" t="s">
         <v>847</v>
@@ -19696,17 +19795,20 @@
       <c r="E304">
         <v>4.8686115732378719</v>
       </c>
+      <c r="F304">
+        <v>8.1291762856273895</v>
+      </c>
       <c r="I304" s="14">
         <f t="shared" si="25"/>
-        <v>8.0722608341406374</v>
+        <v>8.0864896970123255</v>
       </c>
       <c r="J304">
         <f t="shared" si="26"/>
-        <v>4.4951970421487388</v>
+        <v>3.8930328430958472</v>
       </c>
       <c r="K304" s="8">
         <f t="shared" si="27"/>
-        <v>0.55686964711755271</v>
+        <v>0.48142432488774289</v>
       </c>
       <c r="L304" t="s">
         <v>847</v>
@@ -19740,17 +19842,20 @@
       <c r="E305">
         <v>20.728416737081989</v>
       </c>
+      <c r="F305">
+        <v>23.268641247014969</v>
+      </c>
       <c r="I305" s="14">
         <f t="shared" si="25"/>
-        <v>29.615361200263433</v>
+        <v>28.028681211951316</v>
       </c>
       <c r="J305">
         <f t="shared" si="26"/>
-        <v>6.4072462820117195</v>
+        <v>6.1921130355231035</v>
       </c>
       <c r="K305" s="8">
         <f t="shared" si="27"/>
-        <v>0.2163487468103116</v>
+        <v>0.22092059875021203</v>
       </c>
       <c r="L305" t="s">
         <v>847</v>
@@ -19784,17 +19889,20 @@
       <c r="E306">
         <v>31.589811937627712</v>
       </c>
+      <c r="F306">
+        <v>15.088385560283839</v>
+      </c>
       <c r="I306" s="14">
         <f t="shared" si="25"/>
-        <v>31.188605340874375</v>
+        <v>27.163550395726741</v>
       </c>
       <c r="J306">
         <f t="shared" si="26"/>
-        <v>6.9293038032170591</v>
+        <v>9.1986216539398491</v>
       </c>
       <c r="K306" s="8">
         <f t="shared" si="27"/>
-        <v>0.22217421162259626</v>
+        <v>0.33863841507945658</v>
       </c>
       <c r="L306" t="s">
         <v>847</v>
@@ -19828,17 +19936,20 @@
       <c r="E307">
         <v>71.796188212389382</v>
       </c>
+      <c r="F307">
+        <v>89.882574529611091</v>
+      </c>
       <c r="I307" s="14">
         <f t="shared" si="25"/>
-        <v>70.776689609820565</v>
+        <v>75.553160839768196</v>
       </c>
       <c r="J307">
         <f t="shared" si="26"/>
-        <v>4.7567107809307556</v>
+        <v>9.2419562497135654</v>
       </c>
       <c r="K307" s="8">
         <f t="shared" si="27"/>
-        <v>6.7207308043844172E-2</v>
+        <v>0.12232388621455219</v>
       </c>
       <c r="L307" t="s">
         <v>847</v>
@@ -19872,17 +19983,20 @@
       <c r="E308">
         <v>26.822779322022051</v>
       </c>
+      <c r="F308">
+        <v>32.219401258811999</v>
+      </c>
       <c r="I308" s="14">
         <f t="shared" si="25"/>
-        <v>32.601705732125133</v>
+        <v>32.506129613796844</v>
       </c>
       <c r="J308">
         <f t="shared" si="26"/>
-        <v>4.8755632683964354</v>
+        <v>4.2256055508396395</v>
       </c>
       <c r="K308" s="8">
         <f t="shared" si="27"/>
-        <v>0.14954933059199241</v>
+        <v>0.12999411498827382</v>
       </c>
       <c r="L308" t="s">
         <v>847</v>
@@ -19916,17 +20030,20 @@
       <c r="E309">
         <v>18.399902810762509</v>
       </c>
+      <c r="F309">
+        <v>11.21348331748481</v>
+      </c>
       <c r="I309" s="14">
         <f t="shared" si="25"/>
-        <v>19.943063571746013</v>
+        <v>17.760668508180714</v>
       </c>
       <c r="J309">
         <f t="shared" si="26"/>
-        <v>10.205508782953235</v>
+        <v>9.612640208580796</v>
       </c>
       <c r="K309" s="8">
         <f t="shared" si="27"/>
-        <v>0.51173224947303042</v>
+        <v>0.54123189136451322</v>
       </c>
       <c r="L309" t="s">
         <v>847</v>
@@ -19960,17 +20077,20 @@
       <c r="E310">
         <v>9.0491950355523691</v>
       </c>
+      <c r="F310">
+        <v>13.62745948965553</v>
+      </c>
       <c r="I310" s="14">
         <f t="shared" si="25"/>
-        <v>10.076720923264759</v>
+        <v>10.964405564862451</v>
       </c>
       <c r="J310">
         <f t="shared" si="26"/>
-        <v>2.3283543663751614</v>
+        <v>2.5357203336229692</v>
       </c>
       <c r="K310" s="8">
         <f t="shared" si="27"/>
-        <v>0.23106270225262895</v>
+        <v>0.23126838191293955</v>
       </c>
       <c r="L310" t="s">
         <v>847</v>
@@ -20004,17 +20124,20 @@
       <c r="E311">
         <v>49.914210089557763</v>
       </c>
+      <c r="F311">
+        <v>59.514519934187312</v>
+      </c>
       <c r="I311" s="14">
         <f t="shared" si="25"/>
-        <v>50.616914837558333</v>
+        <v>52.841316111715578</v>
       </c>
       <c r="J311">
         <f t="shared" si="26"/>
-        <v>1.9898248624206802</v>
+        <v>4.2205965600549566</v>
       </c>
       <c r="K311" s="8">
         <f t="shared" si="27"/>
-        <v>3.9311460779593133E-2</v>
+        <v>7.9873040087266062E-2</v>
       </c>
       <c r="L311" t="s">
         <v>847</v>
@@ -20048,17 +20171,20 @@
       <c r="E312">
         <v>36.176170841313471</v>
       </c>
+      <c r="F312">
+        <v>42.85580830200518</v>
+      </c>
       <c r="I312" s="14">
         <f t="shared" si="25"/>
-        <v>36.965393314220314</v>
+        <v>38.437997061166534</v>
       </c>
       <c r="J312">
         <f t="shared" si="26"/>
-        <v>1.8215424927486401</v>
+        <v>2.9990328734821832</v>
       </c>
       <c r="K312" s="8">
         <f t="shared" si="27"/>
-        <v>4.927696771044246E-2</v>
+        <v>7.8022610509850723E-2</v>
       </c>
       <c r="L312" t="s">
         <v>847</v>
@@ -20092,17 +20218,20 @@
       <c r="E313">
         <v>14.737488438686009</v>
       </c>
+      <c r="F313">
+        <v>11.87765403184908</v>
+      </c>
       <c r="I313" s="14">
         <f t="shared" si="25"/>
-        <v>9.5034836982366855</v>
+        <v>10.097026281639785</v>
       </c>
       <c r="J313">
         <f t="shared" si="26"/>
-        <v>4.6633377773331963</v>
+        <v>4.1673634127665968</v>
       </c>
       <c r="K313" s="8">
         <f t="shared" si="27"/>
-        <v>0.49069771942666146</v>
+        <v>0.41273175849254157</v>
       </c>
       <c r="L313" t="s">
         <v>847</v>
@@ -20136,17 +20265,20 @@
       <c r="E314">
         <v>14.135681748559771</v>
       </c>
+      <c r="F314">
+        <v>13.525935844677351</v>
+      </c>
       <c r="I314" s="14">
         <f t="shared" si="25"/>
-        <v>18.9356295572119</v>
+        <v>17.583206129078263</v>
       </c>
       <c r="J314">
         <f t="shared" si="26"/>
-        <v>6.0301898516556962</v>
+        <v>5.7235949911006685</v>
       </c>
       <c r="K314" s="8">
         <f t="shared" si="27"/>
-        <v>0.31845732054675807</v>
+        <v>0.32551486623564413</v>
       </c>
       <c r="L314" t="s">
         <v>847</v>
@@ -20180,17 +20312,20 @@
       <c r="E315">
         <v>12.010141276985591</v>
       </c>
+      <c r="F315">
+        <v>12.39404573053123</v>
+      </c>
       <c r="I315" s="14">
         <f t="shared" si="25"/>
-        <v>14.163865913937103</v>
+        <v>13.721410868085636</v>
       </c>
       <c r="J315">
         <f t="shared" si="26"/>
-        <v>6.5733368309216713</v>
+        <v>5.7440288319577393</v>
       </c>
       <c r="K315" s="8">
         <f t="shared" si="27"/>
-        <v>0.46409199796600542</v>
+        <v>0.41861794586427442</v>
       </c>
       <c r="L315" t="s">
         <v>847</v>
@@ -20224,17 +20359,20 @@
       <c r="E316">
         <v>17.37710933431849</v>
       </c>
+      <c r="F316">
+        <v>14.69466976978117</v>
+      </c>
       <c r="I316" s="14">
         <f t="shared" si="25"/>
-        <v>22.008606909327</v>
+        <v>20.180122624440543</v>
       </c>
       <c r="J316">
         <f t="shared" si="26"/>
-        <v>7.2367216232130405</v>
+        <v>7.0219419841764292</v>
       </c>
       <c r="K316" s="8">
         <f t="shared" si="27"/>
-        <v>0.32881325260737876</v>
+        <v>0.34796329610366278</v>
       </c>
       <c r="L316" t="s">
         <v>847</v>
@@ -20268,17 +20406,20 @@
       <c r="E317">
         <v>0.89510842158345916</v>
       </c>
+      <c r="F317">
+        <v>4.7817698602933891</v>
+      </c>
       <c r="I317" s="14">
         <f t="shared" si="25"/>
-        <v>13.785423624897541</v>
+        <v>11.534510183746503</v>
       </c>
       <c r="J317">
         <f t="shared" si="26"/>
-        <v>9.5257573198857415</v>
+        <v>9.1244108492921807</v>
       </c>
       <c r="K317" s="8">
         <f t="shared" si="27"/>
-        <v>0.69100214683874395</v>
+        <v>0.79105317035044631</v>
       </c>
       <c r="L317" t="s">
         <v>847</v>
@@ -20312,17 +20453,20 @@
       <c r="E318">
         <v>16.433822422820739</v>
       </c>
+      <c r="F318">
+        <v>14.988720978901121</v>
+      </c>
       <c r="I318" s="14">
         <f t="shared" si="25"/>
-        <v>21.439132828371964</v>
+        <v>19.82652986600425</v>
       </c>
       <c r="J318">
         <f t="shared" si="26"/>
-        <v>5.8460888938375106</v>
+        <v>5.7822168290975711</v>
       </c>
       <c r="K318" s="8">
         <f t="shared" si="27"/>
-        <v>0.27268308567503979</v>
+        <v>0.29164038629937478</v>
       </c>
       <c r="L318" t="s">
         <v>847</v>
@@ -20356,17 +20500,20 @@
       <c r="E319">
         <v>51.515873282441767</v>
       </c>
+      <c r="F319">
+        <v>61.428485121814177</v>
+      </c>
       <c r="I319" s="14">
         <f t="shared" si="25"/>
-        <v>50.205457578725323</v>
+        <v>53.011214464497542</v>
       </c>
       <c r="J319">
         <f t="shared" si="26"/>
-        <v>3.7848436711585407</v>
+        <v>5.8617912209073051</v>
       </c>
       <c r="K319" s="8">
         <f t="shared" si="27"/>
-        <v>7.5387096417230487E-2</v>
+        <v>0.11057643708262976</v>
       </c>
       <c r="L319" t="s">
         <v>847</v>
@@ -20400,17 +20547,20 @@
       <c r="E320">
         <v>45.130380852834307</v>
       </c>
+      <c r="F320">
+        <v>54.146838096544641</v>
+      </c>
       <c r="I320" s="14">
         <f t="shared" si="25"/>
-        <v>47.599007487383155</v>
+        <v>49.235965139673525</v>
       </c>
       <c r="J320">
         <f t="shared" si="26"/>
-        <v>3.9576573308304814</v>
+        <v>4.448165883528084</v>
       </c>
       <c r="K320" s="8">
         <f t="shared" si="27"/>
-        <v>8.3145795253808996E-2</v>
+        <v>9.0343834449257615E-2</v>
       </c>
       <c r="L320" t="s">
         <v>847</v>
@@ -20444,17 +20594,20 @@
       <c r="E321">
         <v>15.66542232486397</v>
       </c>
+      <c r="F321">
+        <v>6.037470323235544</v>
+      </c>
       <c r="I321" s="14">
         <f t="shared" si="25"/>
-        <v>15.626451398590456</v>
+        <v>13.229206129751729</v>
       </c>
       <c r="J321">
         <f t="shared" si="26"/>
-        <v>5.7815068436322212</v>
+        <v>6.5045922757797543</v>
       </c>
       <c r="K321" s="8">
         <f t="shared" si="27"/>
-        <v>0.36998207053929899</v>
+        <v>0.49168424862254567</v>
       </c>
       <c r="L321" t="s">
         <v>847</v>
@@ -20488,17 +20641,20 @@
       <c r="E322">
         <v>15.44641800070068</v>
       </c>
+      <c r="F322">
+        <v>5.3194443276589816</v>
+      </c>
       <c r="I322" s="14">
         <f t="shared" si="25"/>
-        <v>17.987788596473283</v>
+        <v>14.82070252926971</v>
       </c>
       <c r="J322">
         <f t="shared" si="26"/>
-        <v>6.2261231746372525</v>
+        <v>7.6918632209979751</v>
       </c>
       <c r="K322" s="8">
         <f t="shared" si="27"/>
-        <v>0.34613055080366895</v>
+        <v>0.51899450824326021</v>
       </c>
       <c r="L322" t="s">
         <v>847</v>
@@ -20532,17 +20688,20 @@
       <c r="E323">
         <v>13.211065369449701</v>
       </c>
+      <c r="F323">
+        <v>7.9222173277807597</v>
+      </c>
       <c r="I323" s="14">
         <f t="shared" ref="I323:I363" si="28">AVERAGE(C323:H323)</f>
-        <v>16.229089026380915</v>
+        <v>14.152371101730877</v>
       </c>
       <c r="J323">
         <f t="shared" si="26"/>
-        <v>5.771975048217497</v>
+        <v>6.1583312661485126</v>
       </c>
       <c r="K323" s="8">
         <f t="shared" si="27"/>
-        <v>0.35565613318375189</v>
+        <v>0.43514484052748803</v>
       </c>
       <c r="L323" t="s">
         <v>847</v>
@@ -20576,17 +20735,20 @@
       <c r="E324">
         <v>44.614826534934629</v>
       </c>
+      <c r="F324">
+        <v>50.5976117553884</v>
+      </c>
       <c r="I324" s="14">
         <f t="shared" si="28"/>
-        <v>43.861040377099727</v>
+        <v>45.545183221671891</v>
       </c>
       <c r="J324">
         <f t="shared" si="26"/>
-        <v>0.82412349257630435</v>
+        <v>3.0030644367101109</v>
       </c>
       <c r="K324" s="8">
         <f t="shared" si="27"/>
-        <v>1.8789419619115719E-2</v>
+        <v>6.593593930875119E-2</v>
       </c>
       <c r="L324" t="s">
         <v>847</v>
@@ -20620,17 +20782,20 @@
       <c r="E325">
         <v>33.690481289677393</v>
       </c>
+      <c r="F325">
+        <v>19.80230871036359</v>
+      </c>
       <c r="I325" s="14">
         <f t="shared" si="28"/>
-        <v>30.178502570876052</v>
+        <v>27.584454105747938</v>
       </c>
       <c r="J325">
         <f t="shared" si="26"/>
-        <v>2.5471396129589343</v>
+        <v>5.0053174199274322</v>
       </c>
       <c r="K325" s="8">
         <f t="shared" si="27"/>
-        <v>8.4402451943293794E-2</v>
+        <v>0.18145428583574705</v>
       </c>
       <c r="L325" t="s">
         <v>847</v>
@@ -20664,17 +20829,20 @@
       <c r="E326">
         <v>11.010069096958089</v>
       </c>
+      <c r="F326">
+        <v>13.923157565179469</v>
+      </c>
       <c r="I326" s="14">
         <f t="shared" si="28"/>
-        <v>13.7928280829816</v>
+        <v>13.825410453531067</v>
       </c>
       <c r="J326">
         <f t="shared" si="26"/>
-        <v>4.8877085055674945</v>
+        <v>4.2332559170406325</v>
       </c>
       <c r="K326" s="8">
         <f t="shared" si="27"/>
-        <v>0.35436594120956499</v>
+        <v>0.30619386898270651</v>
       </c>
       <c r="L326" t="s">
         <v>847</v>
@@ -20708,17 +20876,20 @@
       <c r="E327">
         <v>5.296649088817075</v>
       </c>
+      <c r="F327">
+        <v>17.809341736959858</v>
+      </c>
       <c r="I327" s="14">
         <f t="shared" si="28"/>
-        <v>14.748186888791663</v>
+        <v>15.513475600833711</v>
       </c>
       <c r="J327">
         <f t="shared" si="26"/>
-        <v>7.8022335963101463</v>
+        <v>6.8857198067362564</v>
       </c>
       <c r="K327" s="8">
         <f t="shared" si="27"/>
-        <v>0.5290300194283335</v>
+        <v>0.44385410361339084</v>
       </c>
       <c r="L327" t="s">
         <v>847</v>
@@ -20752,17 +20923,20 @@
       <c r="E328">
         <v>6.0941143249034271</v>
       </c>
+      <c r="F328">
+        <v>7.3765270073928493</v>
+      </c>
       <c r="I328" s="14">
         <f t="shared" si="28"/>
-        <v>9.9179594149672212</v>
+        <v>9.2826013130736289</v>
       </c>
       <c r="J328">
         <f t="shared" si="26"/>
-        <v>7.4472056909213817</v>
+        <v>6.5426824930676828</v>
       </c>
       <c r="K328" s="8">
         <f t="shared" si="27"/>
-        <v>0.75088083942779416</v>
+        <v>0.70483286660744116</v>
       </c>
       <c r="L328" t="s">
         <v>847</v>
@@ -20796,17 +20970,20 @@
       <c r="E329">
         <v>39.359695465066828</v>
       </c>
+      <c r="F329">
+        <v>22.82435073904491</v>
+      </c>
       <c r="I329" s="14">
         <f t="shared" si="28"/>
-        <v>38.884381141689438</v>
+        <v>34.86937354102831</v>
       </c>
       <c r="J329">
         <f t="shared" si="26"/>
-        <v>2.5870068999249414</v>
+        <v>7.3061831092092193</v>
       </c>
       <c r="K329" s="8">
         <f t="shared" si="27"/>
-        <v>6.6530746381130185E-2</v>
+        <v>0.20953009381176732</v>
       </c>
       <c r="L329" t="s">
         <v>847</v>
@@ -20840,17 +21017,20 @@
       <c r="E330">
         <v>34.087198319593178</v>
       </c>
+      <c r="F330">
+        <v>43.793319772082327</v>
+      </c>
       <c r="I330" s="14">
         <f t="shared" si="28"/>
-        <v>38.404461416293238</v>
+        <v>39.751676005240512</v>
       </c>
       <c r="J330">
         <f t="shared" si="26"/>
-        <v>3.35633398179883</v>
+        <v>3.7274246865698428</v>
       </c>
       <c r="K330" s="8">
         <f t="shared" si="27"/>
-        <v>8.7394377059923894E-2</v>
+        <v>9.3767736637782317E-2</v>
       </c>
       <c r="L330" t="s">
         <v>847</v>
@@ -20884,17 +21064,20 @@
       <c r="E331">
         <v>47.212266565509474</v>
       </c>
+      <c r="F331">
+        <v>57.717812493380549</v>
+      </c>
       <c r="I331" s="14">
         <f t="shared" si="28"/>
-        <v>50.840453415231572</v>
+        <v>52.559793184768822</v>
       </c>
       <c r="J331">
         <f t="shared" si="26"/>
-        <v>3.5001762665287828</v>
+        <v>4.2493309063799307</v>
       </c>
       <c r="K331" s="8">
         <f t="shared" si="27"/>
-        <v>6.8846283449552112E-2</v>
+        <v>8.0847557589159888E-2</v>
       </c>
       <c r="L331" t="s">
         <v>847</v>
@@ -20928,17 +21111,20 @@
       <c r="E332">
         <v>17.617270925167318</v>
       </c>
+      <c r="F332">
+        <v>42.210383108132163</v>
+      </c>
       <c r="I332" s="14">
         <f t="shared" si="28"/>
-        <v>19.407490763814661</v>
+        <v>25.108213849894035</v>
       </c>
       <c r="J332">
         <f t="shared" si="26"/>
-        <v>2.897649800807967</v>
+        <v>10.187836467502166</v>
       </c>
       <c r="K332" s="8">
         <f t="shared" si="27"/>
-        <v>0.14930574158564824</v>
+        <v>0.40575711710951362</v>
       </c>
       <c r="L332" t="s">
         <v>847</v>
@@ -20972,17 +21158,20 @@
       <c r="E333">
         <v>17.037341129753781</v>
       </c>
+      <c r="F333">
+        <v>13.370286977171739</v>
+      </c>
       <c r="I333" s="14">
         <f t="shared" si="28"/>
-        <v>15.938460542058765</v>
+        <v>15.296417150837009</v>
       </c>
       <c r="J333">
         <f t="shared" si="26"/>
-        <v>6.1787640830273292</v>
+        <v>5.4652999317435444</v>
       </c>
       <c r="K333" s="8">
         <f t="shared" si="27"/>
-        <v>0.38766379392304978</v>
+        <v>0.35729281424862863</v>
       </c>
       <c r="L333" t="s">
         <v>847</v>
@@ -21016,17 +21205,20 @@
       <c r="E334">
         <v>11.030444264822711</v>
       </c>
+      <c r="F334">
+        <v>15.980092200586309</v>
+      </c>
       <c r="I334" s="14">
         <f t="shared" si="28"/>
-        <v>14.518194162284118</v>
+        <v>14.883668671859667</v>
       </c>
       <c r="J334">
         <f t="shared" si="26"/>
-        <v>2.5267862291648489</v>
+        <v>2.2779818562427767</v>
       </c>
       <c r="K334" s="8">
         <f t="shared" si="27"/>
-        <v>0.17404273568189521</v>
+        <v>0.15305244335018847</v>
       </c>
       <c r="L334" t="s">
         <v>847</v>
@@ -21060,17 +21252,20 @@
       <c r="E335">
         <v>41.308135140171579</v>
       </c>
+      <c r="F335">
+        <v>49.398536169383789</v>
+      </c>
       <c r="I335" s="14">
         <f t="shared" si="28"/>
-        <v>40.948675901261431</v>
+        <v>43.061140968292023</v>
       </c>
       <c r="J335">
         <f t="shared" ref="J335:J363" si="29">_xlfn.STDEV.P(C335:H335)</f>
-        <v>0.47128394282516251</v>
+        <v>3.6815903349432131</v>
       </c>
       <c r="K335" s="8">
         <f t="shared" ref="K335:K363" si="30">J335/I335</f>
-        <v>1.1509137535034302E-2</v>
+        <v>8.549681341825438E-2</v>
       </c>
       <c r="L335" t="s">
         <v>847</v>
@@ -21104,17 +21299,20 @@
       <c r="E336">
         <v>11.87705972021276</v>
       </c>
+      <c r="F336">
+        <v>3.7767528180292769</v>
+      </c>
       <c r="I336" s="14">
         <f t="shared" si="28"/>
-        <v>9.1609492945641069</v>
+        <v>7.8149001754303997</v>
       </c>
       <c r="J336">
         <f t="shared" si="29"/>
-        <v>5.7614875863714348</v>
+        <v>5.5074131041075889</v>
       </c>
       <c r="K336" s="8">
         <f t="shared" si="30"/>
-        <v>0.62891818316145109</v>
+        <v>0.70473236771757897</v>
       </c>
       <c r="L336" t="s">
         <v>847</v>
@@ -21148,17 +21346,20 @@
       <c r="E337">
         <v>8.4242715453386996</v>
       </c>
+      <c r="F337">
+        <v>34.335774456700541</v>
+      </c>
       <c r="I337" s="14">
         <f t="shared" si="28"/>
-        <v>14.688597611401553</v>
+        <v>19.600391822726301</v>
       </c>
       <c r="J337">
         <f t="shared" si="29"/>
-        <v>8.9461652899781097</v>
+        <v>11.506631660478083</v>
       </c>
       <c r="K337" s="8">
         <f t="shared" si="30"/>
-        <v>0.60905510019785247</v>
+        <v>0.58706130798550415</v>
       </c>
       <c r="L337" t="s">
         <v>847</v>
@@ -21192,17 +21393,20 @@
       <c r="E338">
         <v>15.74758015144714</v>
       </c>
+      <c r="F338">
+        <v>35.341539352408837</v>
+      </c>
       <c r="I338" s="14">
         <f t="shared" si="28"/>
-        <v>26.577754073925636</v>
+        <v>28.768700393546439</v>
       </c>
       <c r="J338">
         <f t="shared" si="29"/>
-        <v>8.2542236203826853</v>
+        <v>8.0932004181190518</v>
       </c>
       <c r="K338" s="8">
         <f t="shared" si="30"/>
-        <v>0.31056889146553479</v>
+        <v>0.28131963930962156</v>
       </c>
       <c r="L338" t="s">
         <v>847</v>
@@ -21236,17 +21440,20 @@
       <c r="E339">
         <v>15.475533739345041</v>
       </c>
+      <c r="F339">
+        <v>15.991758025073651</v>
+      </c>
       <c r="I339" s="14">
         <f t="shared" si="28"/>
-        <v>15.737554611028983</v>
+        <v>15.80110546454015</v>
       </c>
       <c r="J339">
         <f t="shared" si="29"/>
-        <v>4.1061843150201129</v>
+        <v>3.5577631110901553</v>
       </c>
       <c r="K339" s="8">
         <f t="shared" si="30"/>
-        <v>0.26091628696509633</v>
+        <v>0.22515912694047036</v>
       </c>
       <c r="L339" t="s">
         <v>847</v>
@@ -21280,17 +21487,20 @@
       <c r="E340">
         <v>15.97840801613591</v>
       </c>
+      <c r="F340">
+        <v>15.066307756774091</v>
+      </c>
       <c r="I340" s="14">
         <f t="shared" si="28"/>
-        <v>20.175462820016289</v>
+        <v>18.898174054205739</v>
       </c>
       <c r="J340">
         <f t="shared" si="29"/>
-        <v>3.3515333799963205</v>
+        <v>3.6495180190978278</v>
       </c>
       <c r="K340" s="8">
         <f t="shared" si="30"/>
-        <v>0.16611928112356505</v>
+        <v>0.19311484848376856</v>
       </c>
       <c r="L340" t="s">
         <v>847</v>
@@ -21324,17 +21534,20 @@
       <c r="E341">
         <v>21.33025345838281</v>
       </c>
+      <c r="F341">
+        <v>37.339752398011179</v>
+      </c>
       <c r="I341" s="14">
         <f t="shared" si="28"/>
-        <v>25.104875707926812</v>
+        <v>28.163594880447903</v>
       </c>
       <c r="J341">
         <f t="shared" si="29"/>
-        <v>6.7172835924718166</v>
+        <v>7.868209013194349</v>
       </c>
       <c r="K341" s="8">
         <f t="shared" si="30"/>
-        <v>0.26756888465099427</v>
+        <v>0.27937516665021761</v>
       </c>
       <c r="L341" t="s">
         <v>847</v>
@@ -21368,17 +21581,20 @@
       <c r="E342">
         <v>33.777893003108566</v>
       </c>
+      <c r="F342">
+        <v>41.051381499986931</v>
+      </c>
       <c r="I342" s="14">
         <f t="shared" si="28"/>
-        <v>33.301129052193943</v>
+        <v>35.238692164142194</v>
       </c>
       <c r="J342">
         <f t="shared" si="29"/>
-        <v>5.1285805289193833</v>
+        <v>5.5667949593599886</v>
       </c>
       <c r="K342" s="8">
         <f t="shared" si="30"/>
-        <v>0.15400620564189257</v>
+        <v>0.15797393766572834</v>
       </c>
       <c r="L342" t="s">
         <v>847</v>
@@ -21412,17 +21628,20 @@
       <c r="E343">
         <v>50.996543881919187</v>
       </c>
+      <c r="F343">
+        <v>59.908813495018087</v>
+      </c>
       <c r="I343" s="14">
         <f t="shared" si="28"/>
-        <v>47.399077312639008</v>
+        <v>50.526511358233776</v>
       </c>
       <c r="J343">
         <f t="shared" si="29"/>
-        <v>3.9690899953972698</v>
+        <v>6.4154335529492998</v>
       </c>
       <c r="K343" s="8">
         <f t="shared" si="30"/>
-        <v>8.3737705888610375E-2</v>
+        <v>0.12697163094170055</v>
       </c>
       <c r="L343" t="s">
         <v>847</v>
@@ -21456,17 +21675,20 @@
       <c r="E344">
         <v>44.868301593892063</v>
       </c>
+      <c r="F344">
+        <v>54.955635649626338</v>
+      </c>
       <c r="I344" s="14">
         <f t="shared" si="28"/>
-        <v>48.04431048239843</v>
+        <v>49.772141774205409</v>
       </c>
       <c r="J344">
         <f t="shared" si="29"/>
-        <v>6.290615568883875</v>
+        <v>6.2157128388829932</v>
       </c>
       <c r="K344" s="8">
         <f t="shared" si="30"/>
-        <v>0.1309336216030931</v>
+        <v>0.12488337084389461</v>
       </c>
       <c r="L344" t="s">
         <v>847</v>
@@ -21500,17 +21722,20 @@
       <c r="E345">
         <v>19.412400052400351</v>
       </c>
+      <c r="F345">
+        <v>16.213307937128889</v>
+      </c>
       <c r="I345" s="14">
         <f t="shared" si="28"/>
-        <v>23.781035394800337</v>
+        <v>21.889103530382474</v>
       </c>
       <c r="J345">
         <f t="shared" si="29"/>
-        <v>4.0192612113411261</v>
+        <v>4.780592437401709</v>
       </c>
       <c r="K345" s="8">
         <f t="shared" si="30"/>
-        <v>0.16901119503904893</v>
+        <v>0.21840055855947502</v>
       </c>
       <c r="L345" t="s">
         <v>847</v>
@@ -21544,17 +21769,20 @@
       <c r="E346">
         <v>18.654898623864032</v>
       </c>
+      <c r="F346">
+        <v>16.878535047358341</v>
+      </c>
       <c r="I346" s="14">
         <f t="shared" si="28"/>
-        <v>18.92676533601843</v>
+        <v>18.414707763853407</v>
       </c>
       <c r="J346">
         <f t="shared" si="29"/>
-        <v>5.749017989312132</v>
+        <v>5.0571745819884883</v>
       </c>
       <c r="K346" s="8">
         <f t="shared" si="30"/>
-        <v>0.30375068783525883</v>
+        <v>0.27462692576177156</v>
       </c>
       <c r="L346" t="s">
         <v>847</v>
@@ -21588,17 +21816,20 @@
       <c r="E347">
         <v>34.273200751473247</v>
       </c>
+      <c r="F347">
+        <v>23.087856587034949</v>
+      </c>
       <c r="I347" s="14">
         <f t="shared" si="28"/>
-        <v>28.152732276566002</v>
+        <v>26.88651335418324</v>
       </c>
       <c r="J347">
         <f t="shared" si="29"/>
-        <v>8.0592373192206193</v>
+        <v>7.3159695669022025</v>
       </c>
       <c r="K347" s="8">
         <f t="shared" si="30"/>
-        <v>0.28626838915841329</v>
+        <v>0.27210555234615125</v>
       </c>
       <c r="L347" t="s">
         <v>847</v>
@@ -21632,17 +21863,20 @@
       <c r="E348">
         <v>36.541310433870223</v>
       </c>
+      <c r="F348">
+        <v>28.96326294484966</v>
+      </c>
       <c r="I348" s="14">
         <f t="shared" si="28"/>
-        <v>39.844258923017371</v>
+        <v>37.124009928475445</v>
       </c>
       <c r="J348">
         <f t="shared" si="29"/>
-        <v>3.1533653868258291</v>
+        <v>5.445828561756457</v>
       </c>
       <c r="K348" s="8">
         <f t="shared" si="30"/>
-        <v>7.9142277258021282E-2</v>
+        <v>0.14669289692165802</v>
       </c>
       <c r="L348" t="s">
         <v>847</v>
@@ -21676,17 +21910,20 @@
       <c r="E349">
         <v>19.689662273439929</v>
       </c>
+      <c r="F349">
+        <v>10.355626276117951</v>
+      </c>
       <c r="I349" s="14">
         <f t="shared" si="28"/>
-        <v>20.802072667980404</v>
+        <v>18.190461070014791</v>
       </c>
       <c r="J349">
         <f t="shared" si="29"/>
-        <v>2.3025948667648088</v>
+        <v>4.9434808340100105</v>
       </c>
       <c r="K349" s="8">
         <f t="shared" si="30"/>
-        <v>0.11069064624070267</v>
+        <v>0.27176226127433672</v>
       </c>
       <c r="L349" t="s">
         <v>847</v>
@@ -21720,17 +21957,20 @@
       <c r="E350">
         <v>11.842480018876969</v>
       </c>
+      <c r="F350">
+        <v>15.52656798360014</v>
+      </c>
       <c r="I350" s="14">
         <f t="shared" si="28"/>
-        <v>22.622187702086318</v>
+        <v>20.848282772464774</v>
       </c>
       <c r="J350">
         <f t="shared" si="29"/>
-        <v>7.8269974584280133</v>
+        <v>7.4422196291621097</v>
       </c>
       <c r="K350" s="8">
         <f t="shared" si="30"/>
-        <v>0.34598764547012278</v>
+        <v>0.35697038985826546</v>
       </c>
       <c r="L350" t="s">
         <v>847</v>
@@ -21764,17 +22004,20 @@
       <c r="E351">
         <v>33.805972872339048</v>
       </c>
+      <c r="F351">
+        <v>37.437905613859179</v>
+      </c>
       <c r="I351" s="14">
         <f t="shared" si="28"/>
-        <v>31.486631963587126</v>
+        <v>32.97445037615514</v>
       </c>
       <c r="J351">
         <f t="shared" si="29"/>
-        <v>2.7819372260495365</v>
+        <v>3.5277743597896838</v>
       </c>
       <c r="K351" s="8">
         <f t="shared" si="30"/>
-        <v>8.8352962910314511E-2</v>
+        <v>0.10698508449865561</v>
       </c>
       <c r="L351" t="s">
         <v>847</v>
@@ -21808,17 +22051,20 @@
       <c r="E352">
         <v>28.448832780609401</v>
       </c>
+      <c r="F352">
+        <v>22.177426705704409</v>
+      </c>
       <c r="I352" s="14">
         <f t="shared" si="28"/>
-        <v>24.503889960733556</v>
+        <v>23.922274146976267</v>
       </c>
       <c r="J352">
         <f t="shared" si="29"/>
-        <v>8.1363229440182678</v>
+        <v>7.1179100971743301</v>
       </c>
       <c r="K352" s="8">
         <f t="shared" si="30"/>
-        <v>0.33204209442077892</v>
+        <v>0.29754320402159679</v>
       </c>
       <c r="L352" t="s">
         <v>847</v>
@@ -21852,17 +22098,20 @@
       <c r="E353">
         <v>23.875062735151779</v>
       </c>
+      <c r="F353">
+        <v>28.065890675003839</v>
+      </c>
       <c r="I353" s="14">
         <f t="shared" si="28"/>
-        <v>21.793507252373463</v>
+        <v>23.361603108031058</v>
       </c>
       <c r="J353">
         <f t="shared" si="29"/>
-        <v>6.6838028702022356</v>
+        <v>6.3938790607411535</v>
       </c>
       <c r="K353" s="8">
         <f t="shared" si="30"/>
-        <v>0.30668780351883579</v>
+        <v>0.27369179380258879</v>
       </c>
       <c r="L353" t="s">
         <v>847</v>
@@ -21896,17 +22145,20 @@
       <c r="E354">
         <v>31.197961606782279</v>
       </c>
+      <c r="F354">
+        <v>46.206009721908941</v>
+      </c>
       <c r="I354" s="14">
         <f t="shared" si="28"/>
-        <v>34.718684562190248</v>
+        <v>37.590515852119921</v>
       </c>
       <c r="J354">
         <f t="shared" si="29"/>
-        <v>3.0689959856900613</v>
+        <v>5.6397071859799057</v>
       </c>
       <c r="K354" s="8">
         <f t="shared" si="30"/>
-        <v>8.8396090588993559E-2</v>
+        <v>0.15003005567059421</v>
       </c>
       <c r="L354" t="s">
         <v>847</v>
@@ -21940,17 +22192,20 @@
       <c r="E355">
         <v>55.759891262719847</v>
       </c>
+      <c r="F355">
+        <v>68.983092258026645</v>
+      </c>
       <c r="I355" s="14">
         <f t="shared" si="28"/>
-        <v>59.260164485890471</v>
+        <v>61.690896428924518</v>
       </c>
       <c r="J355">
         <f t="shared" si="29"/>
-        <v>6.8982490304486559</v>
+        <v>7.3085397379518833</v>
       </c>
       <c r="K355" s="8">
         <f t="shared" si="30"/>
-        <v>0.11640617420309544</v>
+        <v>0.1184703118453177</v>
       </c>
       <c r="L355" t="s">
         <v>847</v>
@@ -21984,17 +22239,20 @@
       <c r="E356">
         <v>43.930156242789472</v>
       </c>
+      <c r="F356">
+        <v>54.511250183058699</v>
+      </c>
       <c r="I356" s="14">
         <f t="shared" si="28"/>
-        <v>42.972961004857574</v>
+        <v>45.857533299407855</v>
       </c>
       <c r="J356">
         <f t="shared" si="29"/>
-        <v>4.9653701230556013</v>
+        <v>6.5919228842319919</v>
       </c>
       <c r="K356" s="8">
         <f t="shared" si="30"/>
-        <v>0.11554638095555776</v>
+        <v>0.14374787324893273</v>
       </c>
       <c r="L356" t="s">
         <v>847</v>
@@ -22028,17 +22286,20 @@
       <c r="E357">
         <v>70.661567934323472</v>
       </c>
+      <c r="F357">
+        <v>89.886536340641243</v>
+      </c>
       <c r="I357" s="14">
         <f t="shared" si="28"/>
-        <v>68.611297394991041</v>
+        <v>73.930107131403588</v>
       </c>
       <c r="J357">
         <f t="shared" si="29"/>
-        <v>6.0735892138391971</v>
+        <v>10.608278629934279</v>
       </c>
       <c r="K357" s="8">
         <f t="shared" si="30"/>
-        <v>8.8521707713438438E-2</v>
+        <v>0.14349064327851024</v>
       </c>
       <c r="L357" t="s">
         <v>847</v>
@@ -22072,17 +22333,20 @@
       <c r="E358">
         <v>39.110768382489589</v>
       </c>
+      <c r="F358">
+        <v>48.582384912766017</v>
+      </c>
       <c r="I358" s="14">
         <f t="shared" si="28"/>
-        <v>41.42578929771765</v>
+        <v>43.21493820147974</v>
       </c>
       <c r="J358">
         <f t="shared" si="29"/>
-        <v>3.0132073345238526</v>
+        <v>4.0512621774109538</v>
       </c>
       <c r="K358" s="8">
         <f t="shared" si="30"/>
-        <v>7.2737475509968494E-2</v>
+        <v>9.3746800204199593E-2</v>
       </c>
       <c r="L358" t="s">
         <v>847</v>
@@ -22116,17 +22380,20 @@
       <c r="E359">
         <v>50.353316446892308</v>
       </c>
+      <c r="F359">
+        <v>62.486154121198417</v>
+      </c>
       <c r="I359" s="14">
         <f t="shared" si="28"/>
-        <v>50.384877851072737</v>
+        <v>53.410196918604157</v>
       </c>
       <c r="J359">
         <f t="shared" si="29"/>
-        <v>8.2584835202082481</v>
+        <v>8.8662043130795762</v>
       </c>
       <c r="K359" s="8">
         <f t="shared" si="30"/>
-        <v>0.16390797938656546</v>
+        <v>0.16600208994906826</v>
       </c>
       <c r="L359" t="s">
         <v>847</v>
@@ -22160,17 +22427,20 @@
       <c r="E360">
         <v>39.906405526312312</v>
       </c>
+      <c r="F360">
+        <v>21.184160551327121</v>
+      </c>
       <c r="I360" s="14">
         <f t="shared" si="28"/>
-        <v>38.984896766340775</v>
+        <v>34.534712712587364</v>
       </c>
       <c r="J360">
         <f t="shared" si="29"/>
-        <v>3.8130840679401192</v>
+        <v>8.3855305090809669</v>
       </c>
       <c r="K360" s="8">
         <f t="shared" si="30"/>
-        <v>9.7809264207986912E-2</v>
+        <v>0.24281454369894243</v>
       </c>
       <c r="L360" t="s">
         <v>847</v>
@@ -22204,17 +22474,20 @@
       <c r="E361">
         <v>73.733250937657246</v>
       </c>
+      <c r="F361">
+        <v>82.179403371862776</v>
+      </c>
       <c r="I361" s="14">
         <f t="shared" si="28"/>
-        <v>72.552051616998256</v>
+        <v>74.958889555714393</v>
       </c>
       <c r="J361">
         <f t="shared" si="29"/>
-        <v>6.5088789789398991</v>
+        <v>7.0109012089455547</v>
       </c>
       <c r="K361" s="8">
         <f t="shared" si="30"/>
-        <v>8.9713231175049646E-2</v>
+        <v>9.3529950223376651E-2</v>
       </c>
       <c r="L361" t="s">
         <v>21</v>
@@ -22248,17 +22521,20 @@
       <c r="E362">
         <v>71.563921200926572</v>
       </c>
+      <c r="F362">
+        <v>90.201779023215764</v>
+      </c>
       <c r="I362" s="14">
         <f t="shared" si="28"/>
-        <v>73.348009414606523</v>
+        <v>77.561451816758833</v>
       </c>
       <c r="J362">
         <f t="shared" si="29"/>
-        <v>9.6949947690725971</v>
+        <v>11.124476765584243</v>
       </c>
       <c r="K362" s="8">
         <f t="shared" si="30"/>
-        <v>0.13217802155026084</v>
+        <v>0.14342790787189158</v>
       </c>
       <c r="L362" t="s">
         <v>21</v>
@@ -22292,17 +22568,20 @@
       <c r="E363">
         <v>65.817343897764076</v>
       </c>
+      <c r="F363">
+        <v>84.824484261908083</v>
+      </c>
       <c r="I363" s="14">
         <f t="shared" si="28"/>
-        <v>70.623537710363678</v>
+        <v>74.173774348249779</v>
       </c>
       <c r="J363">
         <f t="shared" si="29"/>
-        <v>12.502800691739223</v>
+        <v>12.452010255696978</v>
       </c>
       <c r="K363" s="8">
         <f t="shared" si="30"/>
-        <v>0.17703447175097398</v>
+        <v>0.16787618487949843</v>
       </c>
       <c r="L363" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Added Replicate 6 for Plate 4.
</commit_message>
<xml_diff>
--- a/data/Results_Masterfile.xlsx
+++ b/data/Results_Masterfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOL428\Documents\Repos\SynbioML\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2B823F-E79D-4826-A01E-D395AAE96688}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68848F7-EC7C-4A7D-B6AC-D49577355A05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3078,8 +3078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
-      <selection activeCell="H356" sqref="H356"/>
+    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="H282" sqref="H282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -18247,17 +18247,20 @@
       <c r="G271">
         <v>62.19745211087217</v>
       </c>
+      <c r="H271">
+        <v>54.246293767506877</v>
+      </c>
       <c r="I271" s="14">
         <f t="shared" si="25"/>
-        <v>68.400758204316276</v>
+        <v>66.041680798181375</v>
       </c>
       <c r="J271">
         <f t="shared" ref="J271:J334" si="26">_xlfn.STDEV.P(C271:H271)</f>
-        <v>10.629605812529375</v>
+        <v>11.044606412882262</v>
       </c>
       <c r="K271" s="8">
         <f t="shared" ref="K271:K334" si="27">J271/I271</f>
-        <v>0.15540187114268886</v>
+        <v>0.16723690674429961</v>
       </c>
       <c r="L271" t="s">
         <v>847</v>
@@ -18297,17 +18300,20 @@
       <c r="G272">
         <v>72.15598806579581</v>
       </c>
+      <c r="H272">
+        <v>60.732381104619762</v>
+      </c>
       <c r="I272" s="14">
         <f t="shared" si="25"/>
-        <v>71.83463523152264</v>
+        <v>69.984259543705491</v>
       </c>
       <c r="J272">
         <f t="shared" si="26"/>
-        <v>10.340357885035454</v>
+        <v>10.30640344264196</v>
       </c>
       <c r="K272" s="8">
         <f t="shared" si="27"/>
-        <v>0.14394668883204512</v>
+        <v>0.14726744999288824</v>
       </c>
       <c r="L272" t="s">
         <v>847</v>
@@ -18347,17 +18353,20 @@
       <c r="G273">
         <v>52.163030614147672</v>
       </c>
+      <c r="H273">
+        <v>42.195739812308751</v>
+      </c>
       <c r="I273" s="14">
         <f t="shared" si="25"/>
-        <v>52.757053398677257</v>
+        <v>50.996834467615848</v>
       </c>
       <c r="J273">
         <f t="shared" si="26"/>
-        <v>3.6403009945576481</v>
+        <v>5.1512146983809473</v>
       </c>
       <c r="K273" s="8">
         <f t="shared" si="27"/>
-        <v>6.9001218984851773E-2</v>
+        <v>0.10101047941813106</v>
       </c>
       <c r="L273" t="s">
         <v>847</v>
@@ -18397,17 +18406,20 @@
       <c r="G274">
         <v>77.380682018118847</v>
       </c>
+      <c r="H274">
+        <v>64.286716218123303</v>
+      </c>
       <c r="I274" s="14">
         <f t="shared" si="25"/>
-        <v>73.340755408382506</v>
+        <v>71.831748876672634</v>
       </c>
       <c r="J274">
         <f t="shared" si="26"/>
-        <v>11.940850961241448</v>
+        <v>11.410759759799816</v>
       </c>
       <c r="K274" s="8">
         <f t="shared" si="27"/>
-        <v>0.16281330748164977</v>
+        <v>0.15885398780128354</v>
       </c>
       <c r="L274" t="s">
         <v>847</v>
@@ -18447,17 +18459,20 @@
       <c r="G275">
         <v>55.405716968783871</v>
       </c>
+      <c r="H275">
+        <v>47.375126820368138</v>
+      </c>
       <c r="I275" s="14">
         <f t="shared" si="25"/>
-        <v>59.411836046544479</v>
+        <v>57.405717842181751</v>
       </c>
       <c r="J275">
         <f t="shared" si="26"/>
-        <v>5.709732352005644</v>
+        <v>6.8767788626407116</v>
       </c>
       <c r="K275" s="8">
         <f t="shared" si="27"/>
-        <v>9.6104290524408637E-2</v>
+        <v>0.11979257678731875</v>
       </c>
       <c r="L275" t="s">
         <v>847</v>
@@ -18497,17 +18512,20 @@
       <c r="G276">
         <v>50.706305467875758</v>
       </c>
+      <c r="H276">
+        <v>50.875409690646443</v>
+      </c>
       <c r="I276" s="14">
         <f t="shared" si="25"/>
-        <v>55.940779020387254</v>
+        <v>55.096550798763786</v>
       </c>
       <c r="J276">
         <f t="shared" si="26"/>
-        <v>4.8700673226600504</v>
+        <v>4.8299312856011358</v>
       </c>
       <c r="K276" s="8">
         <f t="shared" si="27"/>
-        <v>8.7057552789623932E-2</v>
+        <v>8.7663042705560912E-2</v>
       </c>
       <c r="L276" t="s">
         <v>847</v>
@@ -18547,17 +18565,20 @@
       <c r="G277">
         <v>43.409991662158482</v>
       </c>
+      <c r="H277">
+        <v>33.693820339295783</v>
+      </c>
       <c r="I277" s="14">
         <f t="shared" si="25"/>
-        <v>44.098982775993598</v>
+        <v>42.364789036543961</v>
       </c>
       <c r="J277">
         <f t="shared" si="26"/>
-        <v>4.0985023927300848</v>
+        <v>5.3884358753175734</v>
       </c>
       <c r="K277" s="8">
         <f t="shared" si="27"/>
-        <v>9.2938705945870684E-2</v>
+        <v>0.12719137750619972</v>
       </c>
       <c r="L277" t="s">
         <v>847</v>
@@ -18597,17 +18618,20 @@
       <c r="G278">
         <v>41.499744663472747</v>
       </c>
+      <c r="H278">
+        <v>35.968141844793948</v>
+      </c>
       <c r="I278" s="14">
         <f t="shared" si="25"/>
-        <v>44.741881443167252</v>
+        <v>43.279591510105035</v>
       </c>
       <c r="J278">
         <f t="shared" si="26"/>
-        <v>4.2002568520639034</v>
+        <v>5.0391722793629796</v>
       </c>
       <c r="K278" s="8">
         <f t="shared" si="27"/>
-        <v>9.3877519598705758E-2</v>
+        <v>0.11643299078242039</v>
       </c>
       <c r="L278" t="s">
         <v>847</v>
@@ -18647,17 +18671,20 @@
       <c r="G279">
         <v>49.669876605783408</v>
       </c>
+      <c r="H279">
+        <v>46.896930961167207</v>
+      </c>
       <c r="I279" s="14">
         <f t="shared" si="25"/>
-        <v>51.115735056122666</v>
+        <v>50.412601040296757</v>
       </c>
       <c r="J279">
         <f t="shared" si="26"/>
-        <v>5.0999212963093532</v>
+        <v>4.9138903370800566</v>
       </c>
       <c r="K279" s="8">
         <f t="shared" si="27"/>
-        <v>9.9772042614859793E-2</v>
+        <v>9.7473453773039648E-2</v>
       </c>
       <c r="L279" t="s">
         <v>847</v>
@@ -18697,17 +18724,20 @@
       <c r="G280">
         <v>37.008897601832601</v>
       </c>
+      <c r="H280">
+        <v>30.837897325704759</v>
+      </c>
       <c r="I280" s="14">
         <f t="shared" si="25"/>
-        <v>35.993172466771092</v>
+        <v>35.133959943260038</v>
       </c>
       <c r="J280">
         <f t="shared" si="26"/>
-        <v>5.4290921973070274</v>
+        <v>5.3154271582982204</v>
       </c>
       <c r="K280" s="8">
         <f t="shared" si="27"/>
-        <v>0.15083672333465928</v>
+        <v>0.15129029482820683</v>
       </c>
       <c r="L280" t="s">
         <v>847</v>
@@ -18747,17 +18777,20 @@
       <c r="G281">
         <v>61.987510355910452</v>
       </c>
+      <c r="H281">
+        <v>55.844178242554577</v>
+      </c>
       <c r="I281" s="14">
         <f t="shared" si="25"/>
-        <v>65.269450598772394</v>
+        <v>63.698571872736089</v>
       </c>
       <c r="J281">
         <f t="shared" si="26"/>
-        <v>6.171368794629438</v>
+        <v>6.6390105080255148</v>
       </c>
       <c r="K281" s="8">
         <f t="shared" si="27"/>
-        <v>9.4552179281642529E-2</v>
+        <v>0.10422542158856637</v>
       </c>
       <c r="L281" t="s">
         <v>847</v>
@@ -18797,17 +18830,20 @@
       <c r="G282">
         <v>44.4546095578497</v>
       </c>
+      <c r="H282">
+        <v>36.438443174634202</v>
+      </c>
       <c r="I282" s="14">
         <f t="shared" si="25"/>
-        <v>44.711277423624225</v>
+        <v>43.332471715459228</v>
       </c>
       <c r="J282">
         <f t="shared" si="26"/>
-        <v>5.7299903334212763</v>
+        <v>6.071752925522655</v>
       </c>
       <c r="K282" s="8">
         <f t="shared" si="27"/>
-        <v>0.12815537071624139</v>
+        <v>0.14012016128211088</v>
       </c>
       <c r="L282" t="s">
         <v>847</v>
@@ -18847,17 +18883,20 @@
       <c r="G283">
         <v>68.801988876898747</v>
       </c>
+      <c r="H283">
+        <v>58.408486908579142</v>
+      </c>
       <c r="I283" s="14">
         <f t="shared" si="25"/>
-        <v>76.093003682472698</v>
+        <v>73.145584220157104</v>
       </c>
       <c r="J283">
         <f t="shared" si="26"/>
-        <v>10.776828783738129</v>
+        <v>11.841443027035254</v>
       </c>
       <c r="K283" s="8">
         <f t="shared" si="27"/>
-        <v>0.14162706506775036</v>
+        <v>0.1618886929851337</v>
       </c>
       <c r="L283" t="s">
         <v>847</v>
@@ -18897,17 +18936,20 @@
       <c r="G284">
         <v>63.20468671910109</v>
       </c>
+      <c r="H284">
+        <v>60.348771256362838</v>
+      </c>
       <c r="I284" s="14">
         <f t="shared" si="25"/>
-        <v>66.688083574342002</v>
+        <v>65.63153152134548</v>
       </c>
       <c r="J284">
         <f t="shared" si="26"/>
-        <v>9.3238470651049763</v>
+        <v>8.8332674936671918</v>
       </c>
       <c r="K284" s="8">
         <f t="shared" si="27"/>
-        <v>0.13981279061214907</v>
+        <v>0.13458877598786995</v>
       </c>
       <c r="L284" t="s">
         <v>847</v>
@@ -18947,17 +18989,20 @@
       <c r="G285">
         <v>48.584636038723559</v>
       </c>
+      <c r="H285">
+        <v>41.501702327097647</v>
+      </c>
       <c r="I285" s="14">
         <f t="shared" si="25"/>
-        <v>45.563054216833905</v>
+        <v>44.886162235211195</v>
       </c>
       <c r="J285">
         <f t="shared" si="26"/>
-        <v>2.33754525508692</v>
+        <v>2.6161699658549975</v>
       </c>
       <c r="K285" s="8">
         <f t="shared" si="27"/>
-        <v>5.1303524209825278E-2</v>
+        <v>5.8284554427839426E-2</v>
       </c>
       <c r="L285" t="s">
         <v>847</v>
@@ -18997,17 +19042,20 @@
       <c r="G286">
         <v>63.619010504998151</v>
       </c>
+      <c r="H286">
+        <v>47.494272475261631</v>
+      </c>
       <c r="I286" s="14">
         <f t="shared" si="25"/>
-        <v>63.797972341158314</v>
+        <v>61.080689030175535</v>
       </c>
       <c r="J286">
         <f t="shared" si="26"/>
-        <v>2.473080776787532</v>
+        <v>6.4818914472931306</v>
       </c>
       <c r="K286" s="8">
         <f t="shared" si="27"/>
-        <v>3.8764253565345068E-2</v>
+        <v>0.10612014288330798</v>
       </c>
       <c r="L286" t="s">
         <v>847</v>
@@ -19047,17 +19095,20 @@
       <c r="G287">
         <v>27.38161138335504</v>
       </c>
+      <c r="H287">
+        <v>26.695841761804932</v>
+      </c>
       <c r="I287" s="14">
         <f t="shared" si="25"/>
-        <v>21.152939100856429</v>
+        <v>22.076756211014512</v>
       </c>
       <c r="J287">
         <f t="shared" si="26"/>
-        <v>6.4046564189862929</v>
+        <v>6.200823343408211</v>
       </c>
       <c r="K287" s="8">
         <f t="shared" si="27"/>
-        <v>0.30277855897230777</v>
+        <v>0.28087565420115945</v>
       </c>
       <c r="L287" t="s">
         <v>847</v>
@@ -19097,17 +19148,20 @@
       <c r="G288">
         <v>12.033348440016569</v>
       </c>
+      <c r="H288">
+        <v>17.8648564422258</v>
+      </c>
       <c r="I288" s="14">
         <f t="shared" si="25"/>
-        <v>17.76183084806744</v>
+        <v>17.779001780427169</v>
       </c>
       <c r="J288">
         <f t="shared" si="26"/>
-        <v>6.9299454936401137</v>
+        <v>6.3262622976453917</v>
       </c>
       <c r="K288" s="8">
         <f t="shared" si="27"/>
-        <v>0.39015941278340233</v>
+        <v>0.35582775544856227</v>
       </c>
       <c r="L288" t="s">
         <v>847</v>
@@ -19147,17 +19201,20 @@
       <c r="G289">
         <v>58.756180363329392</v>
       </c>
+      <c r="H289">
+        <v>55.633399291479087</v>
+      </c>
       <c r="I289" s="14">
         <f t="shared" si="25"/>
-        <v>62.251305265889116</v>
+        <v>61.148320936820774</v>
       </c>
       <c r="J289">
         <f t="shared" si="26"/>
-        <v>4.9691418930766096</v>
+        <v>5.1633175490304497</v>
       </c>
       <c r="K289" s="8">
         <f t="shared" si="27"/>
-        <v>7.9823898821917122E-2</v>
+        <v>8.4439236759505723E-2</v>
       </c>
       <c r="L289" t="s">
         <v>847</v>
@@ -19197,17 +19254,20 @@
       <c r="G290">
         <v>35.406952486803128</v>
       </c>
+      <c r="H290">
+        <v>29.008031871426621</v>
+      </c>
       <c r="I290" s="14">
         <f t="shared" si="25"/>
-        <v>29.133234899805792</v>
+        <v>29.112367728409264</v>
       </c>
       <c r="J290">
         <f t="shared" si="26"/>
-        <v>7.1269178977759085</v>
+        <v>6.5061234845010469</v>
       </c>
       <c r="K290" s="8">
         <f t="shared" si="27"/>
-        <v>0.24463187566662628</v>
+        <v>0.22348314452458826</v>
       </c>
       <c r="L290" t="s">
         <v>847</v>
@@ -19247,17 +19307,20 @@
       <c r="G291">
         <v>15.0005568211943</v>
       </c>
+      <c r="H291">
+        <v>12.21423970874962</v>
+      </c>
       <c r="I291" s="14">
         <f t="shared" si="25"/>
-        <v>13.200471002515622</v>
+        <v>13.036099120221287</v>
       </c>
       <c r="J291">
         <f t="shared" si="26"/>
-        <v>9.2065555779260855</v>
+        <v>8.4124300048388623</v>
       </c>
       <c r="K291" s="8">
         <f t="shared" si="27"/>
-        <v>0.69744144554929799</v>
+        <v>0.64531804547187743</v>
       </c>
       <c r="L291" t="s">
         <v>847</v>
@@ -19297,17 +19360,20 @@
       <c r="G292">
         <v>51.419401583181212</v>
       </c>
+      <c r="H292">
+        <v>55.157167085543954</v>
+      </c>
       <c r="I292" s="14">
         <f t="shared" si="25"/>
-        <v>58.94296272736392</v>
+        <v>58.311996787060593</v>
       </c>
       <c r="J292">
         <f t="shared" si="26"/>
-        <v>6.4792935597767807</v>
+        <v>6.0807039847853819</v>
       </c>
       <c r="K292" s="8">
         <f t="shared" si="27"/>
-        <v>0.10992480289371011</v>
+        <v>0.10427878172291791</v>
       </c>
       <c r="L292" t="s">
         <v>847</v>
@@ -19347,17 +19413,20 @@
       <c r="G293">
         <v>8.6542133979630247</v>
       </c>
+      <c r="H293">
+        <v>18.434788152817649</v>
+      </c>
       <c r="I293" s="14">
         <f t="shared" si="25"/>
-        <v>14.780723991796526</v>
+        <v>15.389734685300047</v>
       </c>
       <c r="J293">
         <f t="shared" si="26"/>
-        <v>3.7585090967590995</v>
+        <v>3.6914038408206751</v>
       </c>
       <c r="K293" s="8">
         <f t="shared" si="27"/>
-        <v>0.2542845058770542</v>
+        <v>0.23986143467090612</v>
       </c>
       <c r="L293" t="s">
         <v>847</v>
@@ -19397,17 +19466,20 @@
       <c r="G294">
         <v>19.718559537388231</v>
       </c>
+      <c r="H294">
+        <v>29.01686320758915</v>
+      </c>
       <c r="I294" s="14">
         <f t="shared" si="25"/>
-        <v>24.617370440145351</v>
+        <v>25.350619234719318</v>
       </c>
       <c r="J294">
         <f t="shared" si="26"/>
-        <v>6.5636481582600279</v>
+        <v>6.2120447461561366</v>
       </c>
       <c r="K294" s="8">
         <f t="shared" si="27"/>
-        <v>0.26662669655229326</v>
+        <v>0.24504508898340197</v>
       </c>
       <c r="L294" t="s">
         <v>847</v>
@@ -19447,17 +19519,20 @@
       <c r="G295">
         <v>57.239792403581077</v>
       </c>
+      <c r="H295">
+        <v>39.599286208824857</v>
+      </c>
       <c r="I295" s="14">
         <f t="shared" si="25"/>
-        <v>54.759061445867985</v>
+        <v>52.232432239694134</v>
       </c>
       <c r="J295">
         <f t="shared" si="26"/>
-        <v>7.1891390238584183</v>
+        <v>8.6596213724633184</v>
       </c>
       <c r="K295" s="8">
         <f t="shared" si="27"/>
-        <v>0.13128674659563394</v>
+        <v>0.16579012313124533</v>
       </c>
       <c r="L295" t="s">
         <v>847</v>
@@ -19497,17 +19572,20 @@
       <c r="G296">
         <v>33.063256252230723</v>
       </c>
+      <c r="H296">
+        <v>32.04159955728732</v>
+      </c>
       <c r="I296" s="14">
         <f t="shared" si="25"/>
-        <v>38.387174469086588</v>
+        <v>37.329578650453378</v>
       </c>
       <c r="J296">
         <f t="shared" si="26"/>
-        <v>3.9882174552890755</v>
+        <v>4.3413642214760664</v>
       </c>
       <c r="K296" s="8">
         <f t="shared" si="27"/>
-        <v>0.10389453015097035</v>
+        <v>0.11629823797712058</v>
       </c>
       <c r="L296" t="s">
         <v>847</v>
@@ -19547,17 +19625,20 @@
       <c r="G297">
         <v>25.759370994288268</v>
       </c>
+      <c r="H297">
+        <v>16.080530351905431</v>
+      </c>
       <c r="I297" s="14">
         <f t="shared" si="25"/>
-        <v>22.342179502362391</v>
+        <v>21.298571310619565</v>
       </c>
       <c r="J297">
         <f t="shared" si="26"/>
-        <v>7.3940260956884529</v>
+        <v>7.1417977575069971</v>
       </c>
       <c r="K297" s="8">
         <f t="shared" si="27"/>
-        <v>0.3309447090829537</v>
+        <v>0.33531816070433157</v>
       </c>
       <c r="L297" t="s">
         <v>847</v>
@@ -19597,17 +19678,20 @@
       <c r="G298">
         <v>8.1750443305149911</v>
       </c>
+      <c r="H298">
+        <v>14.787458856868779</v>
+      </c>
       <c r="I298" s="14">
         <f t="shared" si="25"/>
-        <v>16.153213642989741</v>
+        <v>15.925587845302914</v>
       </c>
       <c r="J298">
         <f t="shared" si="26"/>
-        <v>8.2869768660578149</v>
+        <v>7.5820438428133592</v>
       </c>
       <c r="K298" s="8">
         <f t="shared" si="27"/>
-        <v>0.51302341745812552</v>
+        <v>0.47609192931924355</v>
       </c>
       <c r="L298" t="s">
         <v>847</v>
@@ -19647,17 +19731,20 @@
       <c r="G299">
         <v>12.97749504328255</v>
       </c>
+      <c r="H299">
+        <v>9.1599908397488097</v>
+      </c>
       <c r="I299" s="14">
         <f t="shared" si="25"/>
-        <v>15.445455550117501</v>
+        <v>14.397878098389386</v>
       </c>
       <c r="J299">
         <f t="shared" si="26"/>
-        <v>5.729062273753625</v>
+        <v>5.7305224922312572</v>
       </c>
       <c r="K299" s="8">
         <f t="shared" si="27"/>
-        <v>0.37092219489181988</v>
+        <v>0.3980115995614868</v>
       </c>
       <c r="L299" t="s">
         <v>847</v>
@@ -19697,17 +19784,20 @@
       <c r="G300">
         <v>10.76514726676157</v>
       </c>
+      <c r="H300">
+        <v>21.501829993425659</v>
+      </c>
       <c r="I300" s="14">
         <f t="shared" si="25"/>
-        <v>17.075302902402044</v>
+        <v>17.813057417572647</v>
       </c>
       <c r="J300">
         <f t="shared" si="26"/>
-        <v>4.9820592269743598</v>
+        <v>4.8379234947278755</v>
       </c>
       <c r="K300" s="8">
         <f t="shared" si="27"/>
-        <v>0.29176988867784687</v>
+        <v>0.27159422334513145</v>
       </c>
       <c r="L300" t="s">
         <v>847</v>
@@ -19747,17 +19837,20 @@
       <c r="G301">
         <v>4.9856057360732713</v>
       </c>
+      <c r="H301">
+        <v>3.449579851023675</v>
+      </c>
       <c r="I301" s="14">
         <f t="shared" si="25"/>
-        <v>11.142878814970597</v>
+        <v>9.8606623209794453</v>
       </c>
       <c r="J301">
         <f t="shared" si="26"/>
-        <v>5.0807124501250254</v>
+        <v>5.4526838823978263</v>
       </c>
       <c r="K301" s="8">
         <f t="shared" si="27"/>
-        <v>0.45596048691645324</v>
+        <v>0.55297339112776955</v>
       </c>
       <c r="L301" t="s">
         <v>847</v>
@@ -19797,17 +19890,20 @@
       <c r="G302">
         <v>6.8525780369933047</v>
       </c>
+      <c r="H302">
+        <v>2.8288919023975239</v>
+      </c>
       <c r="I302" s="14">
         <f t="shared" si="25"/>
-        <v>8.0868966663547113</v>
+        <v>7.2105625390285129</v>
       </c>
       <c r="J302">
         <f t="shared" si="26"/>
-        <v>6.0920533170826126</v>
+        <v>5.8963889114777057</v>
       </c>
       <c r="K302" s="8">
         <f t="shared" si="27"/>
-        <v>0.7533239966362395</v>
+        <v>0.81774325922040092</v>
       </c>
       <c r="L302" t="s">
         <v>847</v>
@@ -19847,17 +19943,20 @@
       <c r="G303">
         <v>11.36180193368167</v>
       </c>
+      <c r="H303">
+        <v>12.29210564394544</v>
+      </c>
       <c r="I303" s="14">
         <f t="shared" si="25"/>
-        <v>11.998889777112259</v>
+        <v>12.047759088251121</v>
       </c>
       <c r="J303">
         <f t="shared" si="26"/>
-        <v>2.3105281039642849</v>
+        <v>2.1120427269659903</v>
       </c>
       <c r="K303" s="8">
         <f t="shared" si="27"/>
-        <v>0.19256182420906892</v>
+        <v>0.17530585659084413</v>
       </c>
       <c r="L303" t="s">
         <v>847</v>
@@ -19897,17 +19996,20 @@
       <c r="G304">
         <v>3.6272786896211828</v>
       </c>
+      <c r="H304">
+        <v>13.432205900553329</v>
+      </c>
       <c r="I304" s="14">
         <f t="shared" si="25"/>
-        <v>7.1946474955340971</v>
+        <v>8.2342405630373019</v>
       </c>
       <c r="J304">
         <f t="shared" si="26"/>
-        <v>3.9123003237594713</v>
+        <v>4.2613198561099992</v>
       </c>
       <c r="K304" s="8">
         <f t="shared" si="27"/>
-        <v>0.54377929234030398</v>
+        <v>0.51751218870610194</v>
       </c>
       <c r="L304" t="s">
         <v>847</v>
@@ -19947,17 +20049,20 @@
       <c r="G305">
         <v>20.54788599149623</v>
       </c>
+      <c r="H305">
+        <v>31.429414643813129</v>
+      </c>
       <c r="I305" s="14">
         <f t="shared" si="25"/>
-        <v>26.5325221678603</v>
+        <v>27.348670913852434</v>
       </c>
       <c r="J305">
         <f t="shared" si="26"/>
-        <v>6.2950598580646897</v>
+        <v>6.029398205882913</v>
       </c>
       <c r="K305" s="8">
         <f t="shared" si="27"/>
-        <v>0.23725825303144751</v>
+        <v>0.22046403003916909</v>
       </c>
       <c r="L305" t="s">
         <v>847</v>
@@ -19997,17 +20102,20 @@
       <c r="G306">
         <v>36.671088985114309</v>
       </c>
+      <c r="H306">
+        <v>19.12769203849529</v>
+      </c>
       <c r="I306" s="14">
         <f t="shared" si="25"/>
-        <v>29.065058113604255</v>
+        <v>27.408830434419428</v>
       </c>
       <c r="J306">
         <f t="shared" si="26"/>
-        <v>9.063919608560953</v>
+        <v>9.065188884879138</v>
       </c>
       <c r="K306" s="8">
         <f t="shared" si="27"/>
-        <v>0.31184935440808476</v>
+        <v>0.33073971932400537</v>
       </c>
       <c r="L306" t="s">
         <v>847</v>
@@ -20047,17 +20155,20 @@
       <c r="G307">
         <v>72.62372843365209</v>
       </c>
+      <c r="H307">
+        <v>51.230136164592857</v>
+      </c>
       <c r="I307" s="14">
         <f t="shared" si="25"/>
-        <v>74.967274358544984</v>
+        <v>71.011084659552964</v>
       </c>
       <c r="J307">
         <f t="shared" si="26"/>
-        <v>8.3488955037666699</v>
+        <v>11.676638990568598</v>
       </c>
       <c r="K307" s="8">
         <f t="shared" si="27"/>
-        <v>0.11136720089137186</v>
+        <v>0.1644340323281876</v>
       </c>
       <c r="L307" t="s">
         <v>847</v>
@@ -20097,17 +20208,20 @@
       <c r="G308">
         <v>29.53338568652784</v>
       </c>
+      <c r="H308">
+        <v>25.968344582501089</v>
+      </c>
       <c r="I308" s="14">
         <f t="shared" si="25"/>
-        <v>31.911580828343045</v>
+        <v>30.921041454036054</v>
       </c>
       <c r="J308">
         <f t="shared" si="26"/>
-        <v>3.9621391760219153</v>
+        <v>4.241221950735695</v>
       </c>
       <c r="K308" s="8">
         <f t="shared" si="27"/>
-        <v>0.12415991540296385</v>
+        <v>0.13716297224465246</v>
       </c>
       <c r="L308" t="s">
         <v>847</v>
@@ -20147,17 +20261,20 @@
       <c r="G309">
         <v>10.117727392366721</v>
       </c>
+      <c r="H309">
+        <v>16.25198962372918</v>
+      </c>
       <c r="I309" s="14">
         <f t="shared" si="25"/>
-        <v>16.232080285017915</v>
+        <v>16.235398508136459</v>
       </c>
       <c r="J309">
         <f t="shared" si="26"/>
-        <v>9.1251635189550111</v>
+        <v>8.3300998048890644</v>
       </c>
       <c r="K309" s="8">
         <f t="shared" si="27"/>
-        <v>0.56216845645948821</v>
+        <v>0.51308255850414697</v>
       </c>
       <c r="L309" t="s">
         <v>847</v>
@@ -20197,17 +20314,20 @@
       <c r="G310">
         <v>1.176075268817204</v>
       </c>
+      <c r="H310">
+        <v>12.23319995980791</v>
+      </c>
       <c r="I310" s="14">
         <f t="shared" si="25"/>
-        <v>9.0067395056534032</v>
+        <v>9.5444829146791541</v>
       </c>
       <c r="J310">
         <f t="shared" si="26"/>
-        <v>4.5247903471647755</v>
+        <v>4.3020087875219568</v>
       </c>
       <c r="K310" s="8">
         <f t="shared" si="27"/>
-        <v>0.50237828509691307</v>
+        <v>0.4507325148967038</v>
       </c>
       <c r="L310" t="s">
         <v>847</v>
@@ -20247,17 +20367,20 @@
       <c r="G311">
         <v>44.041912458576832</v>
       </c>
+      <c r="H311">
+        <v>41.166238864209298</v>
+      </c>
       <c r="I311" s="14">
         <f t="shared" si="25"/>
-        <v>51.081435381087829</v>
+        <v>49.428902628274734</v>
       </c>
       <c r="J311">
         <f t="shared" si="26"/>
-        <v>5.1613437206155366</v>
+        <v>5.987810952054847</v>
       </c>
       <c r="K311" s="8">
         <f t="shared" si="27"/>
-        <v>0.10104147783064159</v>
+        <v>0.12113987229466934</v>
       </c>
       <c r="L311" t="s">
         <v>847</v>
@@ -20297,17 +20420,20 @@
       <c r="G312">
         <v>31.181522795794571</v>
       </c>
+      <c r="H312">
+        <v>29.564540890551459</v>
+      </c>
       <c r="I312" s="14">
         <f t="shared" si="25"/>
-        <v>36.98670220809214</v>
+        <v>35.749675321835362</v>
       </c>
       <c r="J312">
         <f t="shared" si="26"/>
-        <v>3.9522633443664472</v>
+        <v>4.5462254166832015</v>
       </c>
       <c r="K312" s="8">
         <f t="shared" si="27"/>
-        <v>0.1068563323686033</v>
+        <v>0.12716829945323826</v>
       </c>
       <c r="L312" t="s">
         <v>847</v>
@@ -20347,17 +20473,20 @@
       <c r="G313">
         <v>14.44449554469255</v>
       </c>
+      <c r="H313">
+        <v>7.0092007799817733</v>
+      </c>
       <c r="I313" s="14">
         <f t="shared" si="25"/>
-        <v>10.966520134250338</v>
+        <v>10.306966908538911</v>
       </c>
       <c r="J313">
         <f t="shared" si="26"/>
-        <v>4.1131025382504971</v>
+        <v>4.0339884353082427</v>
       </c>
       <c r="K313" s="8">
         <f t="shared" si="27"/>
-        <v>0.37505995410563892</v>
+        <v>0.39138463052270445</v>
       </c>
       <c r="L313" t="s">
         <v>847</v>
@@ -20397,17 +20526,20 @@
       <c r="G314">
         <v>12.520059692985051</v>
       </c>
+      <c r="H314">
+        <v>26.23306350596933</v>
+      </c>
       <c r="I314" s="14">
         <f t="shared" si="25"/>
-        <v>16.570576841859623</v>
+        <v>18.180991285877905</v>
       </c>
       <c r="J314">
         <f t="shared" si="26"/>
-        <v>5.5053886321543022</v>
+        <v>6.1826310526661574</v>
       </c>
       <c r="K314" s="8">
         <f t="shared" si="27"/>
-        <v>0.33223880403770323</v>
+        <v>0.34006017358737306</v>
       </c>
       <c r="L314" t="s">
         <v>847</v>
@@ -20447,17 +20579,20 @@
       <c r="G315">
         <v>8.3751048545770246</v>
       </c>
+      <c r="H315">
+        <v>6.3681148934718124</v>
+      </c>
       <c r="I315" s="14">
         <f t="shared" si="25"/>
-        <v>12.652149665383913</v>
+        <v>11.604810536731897</v>
       </c>
       <c r="J315">
         <f t="shared" si="26"/>
-        <v>5.5649233468487207</v>
+        <v>5.5938870920806165</v>
       </c>
       <c r="K315" s="8">
         <f t="shared" si="27"/>
-        <v>0.43984014527383164</v>
+        <v>0.48203174660841519</v>
       </c>
       <c r="L315" t="s">
         <v>847</v>
@@ -20497,17 +20632,20 @@
       <c r="G316">
         <v>13.199809591788821</v>
       </c>
+      <c r="H316">
+        <v>17.620856231641699</v>
+      </c>
       <c r="I316" s="14">
         <f t="shared" si="25"/>
-        <v>18.7840600179102</v>
+        <v>18.590192720198782</v>
       </c>
       <c r="J316">
         <f t="shared" si="26"/>
-        <v>6.8732887753040641</v>
+        <v>6.289382969434314</v>
       </c>
       <c r="K316" s="8">
         <f t="shared" si="27"/>
-        <v>0.36591071199466624</v>
+        <v>0.33831725491477649</v>
       </c>
       <c r="L316" t="s">
         <v>847</v>
@@ -20547,17 +20685,20 @@
       <c r="G317">
         <v>4.6673205198926508</v>
       </c>
+      <c r="H317">
+        <v>3.1710654947029862</v>
+      </c>
       <c r="I317" s="14">
         <f t="shared" si="25"/>
-        <v>10.161072250975732</v>
+        <v>8.9960711249302747</v>
       </c>
       <c r="J317">
         <f t="shared" si="26"/>
-        <v>8.6109944662645823</v>
+        <v>8.2811327445868574</v>
       </c>
       <c r="K317" s="8">
         <f t="shared" si="27"/>
-        <v>0.84744938856602448</v>
+        <v>0.92052770921717686</v>
       </c>
       <c r="L317" t="s">
         <v>847</v>
@@ -20597,17 +20738,20 @@
       <c r="G318">
         <v>26.955816960979011</v>
       </c>
+      <c r="H318">
+        <v>17.184336229430471</v>
+      </c>
       <c r="I318" s="14">
         <f t="shared" si="25"/>
-        <v>21.252387284999202</v>
+        <v>20.574378775737745</v>
       </c>
       <c r="J318">
         <f t="shared" si="26"/>
-        <v>5.9058871208456987</v>
+        <v>5.6004222992524406</v>
       </c>
       <c r="K318" s="8">
         <f t="shared" si="27"/>
-        <v>0.27789288053367606</v>
+        <v>0.27220371318606795</v>
       </c>
       <c r="L318" t="s">
         <v>847</v>
@@ -20647,17 +20791,20 @@
       <c r="G319">
         <v>47.294643517110032</v>
       </c>
+      <c r="H319">
+        <v>36.807232093289088</v>
+      </c>
       <c r="I319" s="14">
         <f t="shared" si="25"/>
-        <v>51.867900275020041</v>
+        <v>49.357788911398217</v>
       </c>
       <c r="J319">
         <f t="shared" si="26"/>
-        <v>5.7198904183075596</v>
+        <v>7.6660018232097995</v>
       </c>
       <c r="K319" s="8">
         <f t="shared" si="27"/>
-        <v>0.11027804071456311</v>
+        <v>0.15531493594599588</v>
       </c>
       <c r="L319" t="s">
         <v>847</v>
@@ -20697,17 +20844,20 @@
       <c r="G320">
         <v>43.6190708993825</v>
       </c>
+      <c r="H320">
+        <v>43.4169377434376</v>
+      </c>
       <c r="I320" s="14">
         <f t="shared" si="25"/>
-        <v>48.112586291615322</v>
+        <v>47.329978200252363</v>
       </c>
       <c r="J320">
         <f t="shared" si="26"/>
-        <v>4.5691206951627885</v>
+        <v>4.5232470338395077</v>
       </c>
       <c r="K320" s="8">
         <f t="shared" si="27"/>
-        <v>9.4967264230379947E-2</v>
+        <v>9.5568331231882755E-2</v>
       </c>
       <c r="L320" t="s">
         <v>847</v>
@@ -20747,17 +20897,20 @@
       <c r="G321">
         <v>10.266936047781959</v>
       </c>
+      <c r="H321">
+        <v>11.13180276048519</v>
+      </c>
       <c r="I321" s="14">
         <f t="shared" si="25"/>
-        <v>12.636752113357776</v>
+        <v>12.385927221212343</v>
       </c>
       <c r="J321">
         <f t="shared" si="26"/>
-        <v>5.9373212466121643</v>
+        <v>5.4489496193143259</v>
       </c>
       <c r="K321" s="8">
         <f t="shared" si="27"/>
-        <v>0.46984551040896599</v>
+        <v>0.43993069892921421</v>
       </c>
       <c r="L321" t="s">
         <v>847</v>
@@ -20797,17 +20950,20 @@
       <c r="G322">
         <v>4.3170569944505406</v>
       </c>
+      <c r="H322">
+        <v>9.0355702227108967</v>
+      </c>
       <c r="I322" s="14">
         <f t="shared" si="25"/>
-        <v>12.719973422305875</v>
+        <v>12.105906222373379</v>
       </c>
       <c r="J322">
         <f t="shared" si="26"/>
-        <v>8.0612690670770526</v>
+        <v>7.4859050960238456</v>
       </c>
       <c r="K322" s="8">
         <f t="shared" si="27"/>
-        <v>0.6337488923475838</v>
+        <v>0.61836800636939215</v>
       </c>
       <c r="L322" t="s">
         <v>847</v>
@@ -20847,17 +21003,20 @@
       <c r="G323">
         <v>12.92613908916737</v>
       </c>
+      <c r="H323">
+        <v>10.278761217617021</v>
+      </c>
       <c r="I323" s="14">
         <f t="shared" ref="I323:I363" si="28">AVERAGE(C323:H323)</f>
-        <v>13.907124699218176</v>
+        <v>13.30239745228465</v>
       </c>
       <c r="J323">
         <f t="shared" si="26"/>
-        <v>5.5299745368925111</v>
+        <v>5.2261193886878106</v>
       </c>
       <c r="K323" s="8">
         <f t="shared" si="27"/>
-        <v>0.39763607909573084</v>
+        <v>0.39287048875465974</v>
       </c>
       <c r="L323" t="s">
         <v>847</v>
@@ -20897,17 +21056,20 @@
       <c r="G324">
         <v>41.44899447655061</v>
       </c>
+      <c r="H324">
+        <v>38.751218044784373</v>
+      </c>
       <c r="I324" s="14">
         <f t="shared" si="28"/>
-        <v>44.725945472647638</v>
+        <v>43.730157568003762</v>
       </c>
       <c r="J324">
         <f t="shared" si="26"/>
-        <v>3.1463182875436719</v>
+        <v>3.6341986820506031</v>
       </c>
       <c r="K324" s="8">
         <f t="shared" si="27"/>
-        <v>7.0346602051550092E-2</v>
+        <v>8.3105090037673537E-2</v>
       </c>
       <c r="L324" t="s">
         <v>847</v>
@@ -20947,17 +21109,20 @@
       <c r="G325">
         <v>28.4826715436039</v>
       </c>
+      <c r="H325">
+        <v>22.111362155156151</v>
+      </c>
       <c r="I325" s="14">
         <f t="shared" si="28"/>
-        <v>27.764097593319129</v>
+        <v>26.821975020291962</v>
       </c>
       <c r="J325">
         <f t="shared" si="26"/>
-        <v>4.4912859082773195</v>
+        <v>4.6095208324306309</v>
       </c>
       <c r="K325" s="8">
         <f t="shared" si="27"/>
-        <v>0.16176596027230711</v>
+        <v>0.17185613024183838</v>
       </c>
       <c r="L325" t="s">
         <v>847</v>
@@ -20997,17 +21162,20 @@
       <c r="G326">
         <v>7.148890220045323</v>
       </c>
+      <c r="H326">
+        <v>1.619012707722385</v>
+      </c>
       <c r="I326" s="14">
         <f t="shared" si="28"/>
-        <v>12.490106406833918</v>
+        <v>10.678257456981996</v>
       </c>
       <c r="J326">
         <f t="shared" si="26"/>
-        <v>4.6334125777692998</v>
+        <v>5.8569966577239789</v>
       </c>
       <c r="K326" s="8">
         <f t="shared" si="27"/>
-        <v>0.37096662164816657</v>
+        <v>0.54849741929516527</v>
       </c>
       <c r="L326" t="s">
         <v>847</v>
@@ -21047,17 +21215,20 @@
       <c r="G327">
         <v>9.5249444290180616</v>
       </c>
+      <c r="H327">
+        <v>13.872041360968129</v>
+      </c>
       <c r="I327" s="14">
         <f t="shared" si="28"/>
-        <v>14.315769366470581</v>
+        <v>14.24181469888684</v>
       </c>
       <c r="J327">
         <f t="shared" si="26"/>
-        <v>6.6082153945549633</v>
+        <v>6.0347139160290588</v>
       </c>
       <c r="K327" s="8">
         <f t="shared" si="27"/>
-        <v>0.46160392958217633</v>
+        <v>0.42373209058117717</v>
       </c>
       <c r="L327" t="s">
         <v>847</v>
@@ -21097,17 +21268,20 @@
       <c r="G328">
         <v>7.2122382070877338</v>
       </c>
+      <c r="H328">
+        <v>8.2283719808829598</v>
+      </c>
       <c r="I328" s="14">
         <f t="shared" si="28"/>
-        <v>8.8685286918764508</v>
+        <v>8.7618359067108695</v>
       </c>
       <c r="J328">
         <f t="shared" si="26"/>
-        <v>5.9102605616483501</v>
+        <v>5.4005771303486778</v>
       </c>
       <c r="K328" s="8">
         <f t="shared" si="27"/>
-        <v>0.66643078767531461</v>
+        <v>0.61637505973060569</v>
       </c>
       <c r="L328" t="s">
         <v>847</v>
@@ -21147,17 +21321,20 @@
       <c r="G329">
         <v>29.28087229318427</v>
       </c>
+      <c r="H329">
+        <v>36.114593769184467</v>
+      </c>
       <c r="I329" s="14">
         <f t="shared" si="28"/>
-        <v>33.751673291459504</v>
+        <v>34.145493371080327</v>
       </c>
       <c r="J329">
         <f t="shared" si="26"/>
-        <v>6.9066102171600647</v>
+        <v>6.3660447049466589</v>
       </c>
       <c r="K329" s="8">
         <f t="shared" si="27"/>
-        <v>0.20463015737082604</v>
+        <v>0.18643879693764823</v>
       </c>
       <c r="L329" t="s">
         <v>847</v>
@@ -21197,17 +21374,20 @@
       <c r="G330">
         <v>23.91413085626337</v>
       </c>
+      <c r="H330">
+        <v>34.620074210057929</v>
+      </c>
       <c r="I330" s="14">
         <f t="shared" si="28"/>
-        <v>36.584166975445086</v>
+        <v>36.256818181213895</v>
       </c>
       <c r="J330">
         <f t="shared" si="26"/>
-        <v>7.158729611501081</v>
+        <v>6.5758619871649877</v>
       </c>
       <c r="K330" s="8">
         <f t="shared" si="27"/>
-        <v>0.19567835496448358</v>
+        <v>0.18136897601710136</v>
       </c>
       <c r="L330" t="s">
         <v>847</v>
@@ -21247,17 +21427,20 @@
       <c r="G331">
         <v>36.996261161977579</v>
       </c>
+      <c r="H331">
+        <v>34.519781895535189</v>
+      </c>
       <c r="I331" s="14">
         <f t="shared" si="28"/>
-        <v>49.447086780210569</v>
+        <v>46.959202632764679</v>
       </c>
       <c r="J331">
         <f t="shared" si="26"/>
-        <v>7.2939163119303556</v>
+        <v>8.6765306215541074</v>
       </c>
       <c r="K331" s="8">
         <f t="shared" si="27"/>
-        <v>0.14750952557329394</v>
+        <v>0.18476741799487589</v>
       </c>
       <c r="L331" t="s">
         <v>847</v>
@@ -21297,17 +21480,20 @@
       <c r="G332">
         <v>27.05470396434789</v>
       </c>
+      <c r="H332">
+        <v>27.957599684224981</v>
+      </c>
       <c r="I332" s="14">
         <f t="shared" si="28"/>
-        <v>25.497511872784806</v>
+        <v>25.907526508024834</v>
       </c>
       <c r="J332">
         <f t="shared" si="26"/>
-        <v>9.1454809230220491</v>
+        <v>8.3988339131109111</v>
       </c>
       <c r="K332" s="8">
         <f t="shared" si="27"/>
-        <v>0.35868130853911401</v>
+        <v>0.32418509387646016</v>
       </c>
       <c r="L332" t="s">
         <v>847</v>
@@ -21347,17 +21533,20 @@
       <c r="G333">
         <v>4.9844504856025944</v>
       </c>
+      <c r="H333">
+        <v>15.74218106660852</v>
+      </c>
       <c r="I333" s="14">
         <f t="shared" si="28"/>
-        <v>13.234023817790126</v>
+        <v>13.652050025926526</v>
       </c>
       <c r="J333">
         <f t="shared" si="26"/>
-        <v>6.396050946945131</v>
+        <v>5.9131169995225488</v>
       </c>
       <c r="K333" s="8">
         <f t="shared" si="27"/>
-        <v>0.4833035692702245</v>
+        <v>0.43313033487959568</v>
       </c>
       <c r="L333" t="s">
         <v>847</v>
@@ -21397,17 +21586,20 @@
       <c r="G334">
         <v>4.9381976431985368</v>
       </c>
+      <c r="H334">
+        <v>13.025500914525709</v>
+      </c>
       <c r="I334" s="14">
         <f t="shared" si="28"/>
-        <v>12.894574466127441</v>
+        <v>12.916395540860485</v>
       </c>
       <c r="J334">
         <f t="shared" si="26"/>
-        <v>4.469602231407972</v>
+        <v>4.080461683725483</v>
       </c>
       <c r="K334" s="8">
         <f t="shared" si="27"/>
-        <v>0.34662657873271441</v>
+        <v>0.31591334214077843</v>
       </c>
       <c r="L334" t="s">
         <v>847</v>
@@ -21447,17 +21639,20 @@
       <c r="G335">
         <v>28.71544134235846</v>
       </c>
+      <c r="H335">
+        <v>36.63201974073889</v>
+      </c>
       <c r="I335" s="14">
         <f t="shared" si="28"/>
-        <v>40.192001043105314</v>
+        <v>39.598670826044241</v>
       </c>
       <c r="J335">
         <f t="shared" ref="J335:J363" si="29">_xlfn.STDEV.P(C335:H335)</f>
-        <v>6.6159762361029912</v>
+        <v>6.1835390376079564</v>
       </c>
       <c r="K335" s="8">
         <f t="shared" ref="K335:K363" si="30">J335/I335</f>
-        <v>0.16460927707997064</v>
+        <v>0.15615521704685634</v>
       </c>
       <c r="L335" t="s">
         <v>847</v>
@@ -21497,17 +21692,20 @@
       <c r="G336">
         <v>4.8842494641016909</v>
       </c>
+      <c r="H336">
+        <v>13.768808614745661</v>
+      </c>
       <c r="I336" s="14">
         <f t="shared" si="28"/>
-        <v>7.2287700331646576</v>
+        <v>8.3187764634281578</v>
       </c>
       <c r="J336">
         <f t="shared" si="29"/>
-        <v>5.0635435669229336</v>
+        <v>5.2255906813027151</v>
       </c>
       <c r="K336" s="8">
         <f t="shared" si="30"/>
-        <v>0.70047097136747383</v>
+        <v>0.62816818125549867</v>
       </c>
       <c r="L336" t="s">
         <v>847</v>
@@ -21547,17 +21745,20 @@
       <c r="G337">
         <v>19.622528307945959</v>
       </c>
+      <c r="H337">
+        <v>14.044049840868089</v>
+      </c>
       <c r="I337" s="14">
         <f t="shared" si="28"/>
-        <v>19.604819119770234</v>
+        <v>18.678024239953206</v>
       </c>
       <c r="J337">
         <f t="shared" si="29"/>
-        <v>10.291848042978957</v>
+        <v>9.6209765891730985</v>
       </c>
       <c r="K337" s="8">
         <f t="shared" si="30"/>
-        <v>0.52496521289504128</v>
+        <v>0.51509605435640027</v>
       </c>
       <c r="L337" t="s">
         <v>847</v>
@@ -21597,17 +21798,20 @@
       <c r="G338">
         <v>23.4342149368821</v>
       </c>
+      <c r="H338">
+        <v>28.26618475995955</v>
+      </c>
       <c r="I338" s="14">
         <f t="shared" si="28"/>
-        <v>27.70180330221357</v>
+        <v>27.795866878504565</v>
       </c>
       <c r="J338">
         <f t="shared" si="29"/>
-        <v>7.5467206136342613</v>
+        <v>6.8923919262812294</v>
       </c>
       <c r="K338" s="8">
         <f t="shared" si="30"/>
-        <v>0.2724270521779073</v>
+        <v>0.24796463288616974</v>
       </c>
       <c r="L338" t="s">
         <v>847</v>
@@ -21647,17 +21851,20 @@
       <c r="G339">
         <v>27.269774420089551</v>
       </c>
+      <c r="H339">
+        <v>21.55041799781808</v>
+      </c>
       <c r="I339" s="14">
         <f t="shared" si="28"/>
-        <v>18.094839255650029</v>
+        <v>18.670769046011372</v>
       </c>
       <c r="J339">
         <f t="shared" si="29"/>
-        <v>5.5830996320703772</v>
+        <v>5.2568346180772343</v>
       </c>
       <c r="K339" s="8">
         <f t="shared" si="30"/>
-        <v>0.30854651722463244</v>
+        <v>0.28155426298309066</v>
       </c>
       <c r="L339" t="s">
         <v>847</v>
@@ -21697,17 +21904,20 @@
       <c r="G340">
         <v>13.74667347840335</v>
       </c>
+      <c r="H340">
+        <v>14.913812040568409</v>
+      </c>
       <c r="I340" s="14">
         <f t="shared" si="28"/>
-        <v>17.867873939045261</v>
+        <v>17.375530289299121</v>
       </c>
       <c r="J340">
         <f t="shared" si="29"/>
-        <v>3.8602148549756348</v>
+        <v>3.6918460088017646</v>
       </c>
       <c r="K340" s="8">
         <f t="shared" si="30"/>
-        <v>0.21604220335023802</v>
+        <v>0.21247386107550464</v>
       </c>
       <c r="L340" t="s">
         <v>847</v>
@@ -21747,17 +21957,20 @@
       <c r="G341">
         <v>23.000798974714421</v>
       </c>
+      <c r="H341">
+        <v>29.545217999646312</v>
+      </c>
       <c r="I341" s="14">
         <f t="shared" si="28"/>
-        <v>27.131035699301208</v>
+        <v>27.533399416025389</v>
       </c>
       <c r="J341">
         <f t="shared" si="29"/>
-        <v>7.3342814447314071</v>
+        <v>6.7554338420852185</v>
       </c>
       <c r="K341" s="8">
         <f t="shared" si="30"/>
-        <v>0.27032810416892084</v>
+        <v>0.24535415115335604</v>
       </c>
       <c r="L341" t="s">
         <v>847</v>
@@ -21797,17 +22010,20 @@
       <c r="G342">
         <v>37.833374112356331</v>
       </c>
+      <c r="H342">
+        <v>30.88372040674377</v>
+      </c>
       <c r="I342" s="14">
         <f t="shared" si="28"/>
-        <v>35.757628553785018</v>
+        <v>34.945310529278146</v>
       </c>
       <c r="J342">
         <f t="shared" si="29"/>
-        <v>5.0861129363814612</v>
+        <v>4.9856216796620245</v>
       </c>
       <c r="K342" s="8">
         <f t="shared" si="30"/>
-        <v>0.14223854159486998</v>
+        <v>0.14266926246040748</v>
       </c>
       <c r="L342" t="s">
         <v>847</v>
@@ -21847,17 +22063,20 @@
       <c r="G343">
         <v>38.399983422844819</v>
       </c>
+      <c r="H343">
+        <v>32.615218825373638</v>
+      </c>
       <c r="I343" s="14">
         <f t="shared" si="28"/>
-        <v>48.101205771155989</v>
+        <v>45.520207946858932</v>
       </c>
       <c r="J343">
         <f t="shared" si="29"/>
-        <v>7.5136315387892889</v>
+        <v>8.9640001075991851</v>
       </c>
       <c r="K343" s="8">
         <f t="shared" si="30"/>
-        <v>0.1562046401609096</v>
+        <v>0.19692353158983614</v>
       </c>
       <c r="L343" t="s">
         <v>847</v>
@@ -21897,17 +22116,20 @@
       <c r="G344">
         <v>47.751002824715592</v>
       </c>
+      <c r="H344">
+        <v>35.955594396001167</v>
+      </c>
       <c r="I344" s="14">
         <f t="shared" si="28"/>
-        <v>49.367913984307442</v>
+        <v>47.132527386256392</v>
       </c>
       <c r="J344">
         <f t="shared" si="29"/>
-        <v>5.61797733182211</v>
+        <v>7.1614354216028095</v>
       </c>
       <c r="K344" s="8">
         <f t="shared" si="30"/>
-        <v>0.11379815103404803</v>
+        <v>0.15194252926252047</v>
       </c>
       <c r="L344" t="s">
         <v>847</v>
@@ -21947,17 +22169,20 @@
       <c r="G345">
         <v>19.698264834671871</v>
       </c>
+      <c r="H345">
+        <v>21.771920703870869</v>
+      </c>
       <c r="I345" s="14">
         <f t="shared" si="28"/>
-        <v>21.450935791240354</v>
+        <v>21.504433276678771</v>
       </c>
       <c r="J345">
         <f t="shared" si="29"/>
-        <v>4.3647697662687248</v>
+        <v>3.9862667370008249</v>
       </c>
       <c r="K345" s="8">
         <f t="shared" si="30"/>
-        <v>0.20347689297783969</v>
+        <v>0.18536953221287028</v>
       </c>
       <c r="L345" t="s">
         <v>847</v>
@@ -21997,17 +22222,20 @@
       <c r="G346">
         <v>6.717987040039441</v>
       </c>
+      <c r="H346">
+        <v>13.33831785154373</v>
+      </c>
       <c r="I346" s="14">
         <f t="shared" si="28"/>
-        <v>16.075363619090616</v>
+        <v>15.619189324499468</v>
       </c>
       <c r="J346">
         <f t="shared" si="29"/>
-        <v>6.507698203874563</v>
+        <v>6.0276243133168768</v>
       </c>
       <c r="K346" s="8">
         <f t="shared" si="30"/>
-        <v>0.40482432360946519</v>
+        <v>0.38591147005704396</v>
       </c>
       <c r="L346" t="s">
         <v>847</v>
@@ -22047,17 +22275,20 @@
       <c r="G347">
         <v>25.765612429380031</v>
       </c>
+      <c r="H347">
+        <v>26.248885912629969</v>
+      </c>
       <c r="I347" s="14">
         <f t="shared" si="28"/>
-        <v>26.662333169222599</v>
+        <v>26.593425293123826</v>
       </c>
       <c r="J347">
         <f t="shared" si="29"/>
-        <v>6.5589447005129804</v>
+        <v>5.9894522117857463</v>
       </c>
       <c r="K347" s="8">
         <f t="shared" si="30"/>
-        <v>0.24600040284862368</v>
+        <v>0.22522304463481127</v>
       </c>
       <c r="L347" t="s">
         <v>847</v>
@@ -22097,17 +22328,20 @@
       <c r="G348">
         <v>31.994575253376428</v>
       </c>
+      <c r="H348">
+        <v>31.16822375973932</v>
+      </c>
       <c r="I348" s="14">
         <f t="shared" si="28"/>
-        <v>36.098122993455647</v>
+        <v>35.276473121169595</v>
       </c>
       <c r="J348">
         <f t="shared" si="29"/>
-        <v>5.2853963893932372</v>
+        <v>5.1628533832866301</v>
       </c>
       <c r="K348" s="8">
         <f t="shared" si="30"/>
-        <v>0.14641748520695785</v>
+        <v>0.14635401236265808</v>
       </c>
       <c r="L348" t="s">
         <v>847</v>
@@ -22147,17 +22381,20 @@
       <c r="G349">
         <v>23.1968393881486</v>
       </c>
+      <c r="H349">
+        <v>11.836563721133549</v>
+      </c>
       <c r="I349" s="14">
         <f t="shared" si="28"/>
-        <v>19.191736733641555</v>
+        <v>17.965874564890218</v>
       </c>
       <c r="J349">
         <f t="shared" si="29"/>
-        <v>4.8539276903621342</v>
+        <v>5.2103296731843667</v>
       </c>
       <c r="K349" s="8">
         <f t="shared" si="30"/>
-        <v>0.25291758415243332</v>
+        <v>0.29001258215208991</v>
       </c>
       <c r="L349" t="s">
         <v>847</v>
@@ -22197,17 +22434,20 @@
       <c r="G350">
         <v>11.027437244376349</v>
       </c>
+      <c r="H350">
+        <v>15.003155009247889</v>
+      </c>
       <c r="I350" s="14">
         <f t="shared" si="28"/>
-        <v>18.884113666847089</v>
+        <v>18.237287223913889</v>
       </c>
       <c r="J350">
         <f t="shared" si="29"/>
-        <v>7.7292397756053965</v>
+        <v>7.2025142712149659</v>
       </c>
       <c r="K350" s="8">
         <f t="shared" si="30"/>
-        <v>0.40929852001340333</v>
+        <v>0.39493342308995233</v>
       </c>
       <c r="L350" t="s">
         <v>847</v>
@@ -22247,17 +22487,20 @@
       <c r="G351">
         <v>34.845573379679188</v>
       </c>
+      <c r="H351">
+        <v>29.781825043519731</v>
+      </c>
       <c r="I351" s="14">
         <f t="shared" si="28"/>
-        <v>33.348674976859954</v>
+        <v>32.754199987969912</v>
       </c>
       <c r="J351">
         <f t="shared" si="29"/>
-        <v>3.2428891060229263</v>
+        <v>3.2450902437961346</v>
       </c>
       <c r="K351" s="8">
         <f t="shared" si="30"/>
-        <v>9.7241917655592272E-2</v>
+        <v>9.9074019362036136E-2</v>
       </c>
       <c r="L351" t="s">
         <v>847</v>
@@ -22297,17 +22540,20 @@
       <c r="G352">
         <v>23.34878390197515</v>
       </c>
+      <c r="H352">
+        <v>15.96125883110159</v>
+      </c>
       <c r="I352" s="14">
         <f t="shared" si="28"/>
-        <v>23.807576097976046</v>
+        <v>22.499856553496969</v>
       </c>
       <c r="J352">
         <f t="shared" si="29"/>
-        <v>6.370583795143328</v>
+        <v>6.5092959381832092</v>
       </c>
       <c r="K352" s="8">
         <f t="shared" si="30"/>
-        <v>0.26758640900385111</v>
+        <v>0.28930388612506608</v>
       </c>
       <c r="L352" t="s">
         <v>847</v>
@@ -22347,17 +22593,20 @@
       <c r="G353">
         <v>28.599408807709331</v>
       </c>
+      <c r="H353">
+        <v>19.608143343378469</v>
+      </c>
       <c r="I353" s="14">
         <f t="shared" si="28"/>
-        <v>24.409164247966714</v>
+        <v>23.608994097202004</v>
       </c>
       <c r="J353">
         <f t="shared" si="29"/>
-        <v>6.0905573572802396</v>
+        <v>5.8406993405020611</v>
       </c>
       <c r="K353" s="8">
         <f t="shared" si="30"/>
-        <v>0.24951929100921935</v>
+        <v>0.24739297728886575</v>
       </c>
       <c r="L353" t="s">
         <v>847</v>
@@ -22397,17 +22646,20 @@
       <c r="G354">
         <v>39.206846097128818</v>
       </c>
+      <c r="H354">
+        <v>31.493805222512421</v>
+      </c>
       <c r="I354" s="14">
         <f t="shared" si="28"/>
-        <v>37.913781901121702</v>
+        <v>36.843785788020149</v>
       </c>
       <c r="J354">
         <f t="shared" si="29"/>
-        <v>5.0855718919924398</v>
+        <v>5.2227380718784548</v>
       </c>
       <c r="K354" s="8">
         <f t="shared" si="30"/>
-        <v>0.13413517821185705</v>
+        <v>0.14175356739742639</v>
       </c>
       <c r="L354" t="s">
         <v>847</v>
@@ -22447,17 +22699,20 @@
       <c r="G355">
         <v>59.35340024152439</v>
       </c>
+      <c r="H355">
+        <v>36.948155026893772</v>
+      </c>
       <c r="I355" s="14">
         <f t="shared" si="28"/>
-        <v>61.223397191444498</v>
+        <v>57.177523497352716</v>
       </c>
       <c r="J355">
         <f t="shared" si="29"/>
-        <v>6.6034857938178471</v>
+        <v>10.871238365538121</v>
       </c>
       <c r="K355" s="8">
         <f t="shared" si="30"/>
-        <v>0.10785885946787405</v>
+        <v>0.19013132609777078</v>
       </c>
       <c r="L355" t="s">
         <v>847</v>
@@ -22497,17 +22752,20 @@
       <c r="G356">
         <v>39.351068115616997</v>
       </c>
+      <c r="H356">
+        <v>29.736394265911631</v>
+      </c>
       <c r="I356" s="14">
         <f t="shared" si="28"/>
-        <v>44.556240262649681</v>
+        <v>42.086265929860005</v>
       </c>
       <c r="J356">
         <f t="shared" si="29"/>
-        <v>6.4448593560597454</v>
+        <v>8.0695338231332414</v>
       </c>
       <c r="K356" s="8">
         <f t="shared" si="30"/>
-        <v>0.14464549338249036</v>
+        <v>0.19173793742076667</v>
       </c>
       <c r="L356" t="s">
         <v>847</v>
@@ -22547,17 +22805,20 @@
       <c r="G357">
         <v>80.059424440834917</v>
       </c>
+      <c r="H357">
+        <v>62.315161088050239</v>
+      </c>
       <c r="I357" s="14">
         <f t="shared" si="28"/>
-        <v>75.155970593289851</v>
+        <v>73.015835675749912</v>
       </c>
       <c r="J357">
         <f t="shared" si="29"/>
-        <v>9.7999706785790011</v>
+        <v>10.145626729969679</v>
       </c>
       <c r="K357" s="8">
         <f t="shared" si="30"/>
-        <v>0.13039510502248736</v>
+        <v>0.1389510458392145</v>
       </c>
       <c r="L357" t="s">
         <v>847</v>
@@ -22597,17 +22858,20 @@
       <c r="G358">
         <v>38.438325608352912</v>
       </c>
+      <c r="H358">
+        <v>27.701636479631141</v>
+      </c>
       <c r="I358" s="14">
         <f t="shared" si="28"/>
-        <v>42.259615682854374</v>
+        <v>39.833285815650498</v>
       </c>
       <c r="J358">
         <f t="shared" si="29"/>
-        <v>4.0964307198422487</v>
+        <v>6.5893350947687264</v>
       </c>
       <c r="K358" s="8">
         <f t="shared" si="30"/>
-        <v>9.6934878693283003E-2</v>
+        <v>0.16542283569736987</v>
       </c>
       <c r="L358" t="s">
         <v>847</v>
@@ -22647,17 +22911,20 @@
       <c r="G359">
         <v>54.725995344261463</v>
       </c>
+      <c r="H359">
+        <v>40.821224361760571</v>
+      </c>
       <c r="I359" s="14">
         <f t="shared" si="28"/>
-        <v>53.673356603735627</v>
+        <v>51.531334563406453</v>
       </c>
       <c r="J359">
         <f t="shared" si="29"/>
-        <v>7.9476207267666243</v>
+        <v>8.6935908261999675</v>
       </c>
       <c r="K359" s="8">
         <f t="shared" si="30"/>
-        <v>0.14807385320510169</v>
+        <v>0.16870494233955818</v>
       </c>
       <c r="L359" t="s">
         <v>847</v>
@@ -22697,17 +22964,20 @@
       <c r="G360">
         <v>43.027952158896902</v>
       </c>
+      <c r="H360">
+        <v>29.560367552040471</v>
+      </c>
       <c r="I360" s="14">
         <f t="shared" si="28"/>
-        <v>36.23336060184927</v>
+        <v>35.121195093547804</v>
       </c>
       <c r="J360">
         <f t="shared" si="29"/>
-        <v>8.23379111599011</v>
+        <v>7.9171116812935862</v>
       </c>
       <c r="K360" s="8">
         <f t="shared" si="30"/>
-        <v>0.22724337404049338</v>
+        <v>0.2254226161782307</v>
       </c>
       <c r="L360" t="s">
         <v>847</v>
@@ -22747,17 +23017,20 @@
       <c r="G361">
         <v>83.306284728428352</v>
       </c>
+      <c r="H361">
+        <v>51.757053674874371</v>
+      </c>
       <c r="I361" s="14">
         <f t="shared" si="28"/>
-        <v>76.628368590257182</v>
+        <v>72.483149437693385</v>
       </c>
       <c r="J361">
         <f t="shared" si="29"/>
-        <v>7.1042824828681441</v>
+        <v>11.312525526051342</v>
       </c>
       <c r="K361" s="8">
         <f t="shared" si="30"/>
-        <v>9.2710866922611337E-2</v>
+        <v>0.15607110913103472</v>
       </c>
       <c r="L361" t="s">
         <v>21</v>
@@ -22797,17 +23070,20 @@
       <c r="G362">
         <v>90.268871855835172</v>
       </c>
+      <c r="H362">
+        <v>63.41490320943327</v>
+      </c>
       <c r="I362" s="14">
         <f t="shared" si="28"/>
-        <v>80.102935824574104</v>
+        <v>77.321597055383961</v>
       </c>
       <c r="J362">
         <f t="shared" si="29"/>
-        <v>11.173171013384747</v>
+        <v>11.946227528259822</v>
       </c>
       <c r="K362" s="8">
         <f t="shared" si="30"/>
-        <v>0.13948516241469672</v>
+        <v>0.15450052744905116</v>
       </c>
       <c r="L362" t="s">
         <v>21</v>
@@ -22847,17 +23123,20 @@
       <c r="G363">
         <v>86.138336611046341</v>
       </c>
+      <c r="H363">
+        <v>61.102778362665262</v>
+      </c>
       <c r="I363" s="14">
         <f t="shared" si="28"/>
-        <v>76.566686800809094</v>
+        <v>73.98936872778512</v>
       </c>
       <c r="J363">
         <f t="shared" si="29"/>
-        <v>12.122135436829609</v>
+        <v>12.476697554710276</v>
       </c>
       <c r="K363" s="8">
         <f t="shared" si="30"/>
-        <v>0.15832127447757752</v>
+        <v>0.16862824712849481</v>
       </c>
       <c r="L363" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Added Rep 6 for Plate 5.
</commit_message>
<xml_diff>
--- a/data/Results_Masterfile.xlsx
+++ b/data/Results_Masterfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOL428\Documents\Repos\SynbioML\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F0716A-A898-42AE-8B1E-F245648106CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25035B1-B6FB-4EA4-B2C2-D87A7D7FC61E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Microplate!$L$1:$L$363</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3901,8 +3901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A359" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H368" sqref="H368"/>
+    <sheetView tabSelected="1" topLeftCell="A353" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H364" sqref="H364:H456"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -24000,17 +24000,20 @@
       <c r="G364">
         <v>101.13930397320649</v>
       </c>
+      <c r="H364">
+        <v>120.6918074097939</v>
+      </c>
       <c r="I364" s="1">
         <f t="shared" si="42"/>
-        <v>102.31403650886438</v>
+        <v>105.37699832568596</v>
       </c>
       <c r="J364">
         <f t="shared" si="43"/>
-        <v>3.4026550225473366</v>
+        <v>7.520442792277847</v>
       </c>
       <c r="K364" s="10">
         <f t="shared" si="44"/>
-        <v>3.3256971757267481E-2</v>
+        <v>7.1367024225102799E-2</v>
       </c>
       <c r="L364" t="s">
         <v>755</v>
@@ -24050,17 +24053,20 @@
       <c r="G365">
         <v>63.347086266471273</v>
       </c>
+      <c r="H365">
+        <v>74.069999554422338</v>
+      </c>
       <c r="I365" s="1">
         <f t="shared" si="42"/>
-        <v>61.668532622866522</v>
+        <v>63.73544377812582</v>
       </c>
       <c r="J365">
         <f t="shared" si="43"/>
-        <v>6.3806832695459716</v>
+        <v>7.4356040624750941</v>
       </c>
       <c r="K365" s="10">
         <f t="shared" si="44"/>
-        <v>0.10346740871178167</v>
+        <v>0.11666356459931035</v>
       </c>
       <c r="L365" t="s">
         <v>755</v>
@@ -24100,17 +24106,20 @@
       <c r="G366">
         <v>74.372984689989281</v>
       </c>
+      <c r="H366">
+        <v>78.611326583270284</v>
+      </c>
       <c r="I366" s="1">
         <f t="shared" si="42"/>
-        <v>68.972375834687725</v>
+        <v>70.578867626118154</v>
       </c>
       <c r="J366">
         <f t="shared" si="43"/>
-        <v>3.7561318955623006</v>
+        <v>4.9660029259338652</v>
       </c>
       <c r="K366" s="10">
         <f t="shared" si="44"/>
-        <v>5.4458496609787063E-2</v>
+        <v>7.0361045635367561E-2</v>
       </c>
       <c r="L366" t="s">
         <v>755</v>
@@ -24150,17 +24159,20 @@
       <c r="G367">
         <v>43.262691602174037</v>
       </c>
+      <c r="H367">
+        <v>52.712891335340011</v>
+      </c>
       <c r="I367" s="1">
         <f t="shared" si="42"/>
-        <v>46.253606641947925</v>
+        <v>47.330154090846605</v>
       </c>
       <c r="J367">
         <f t="shared" si="43"/>
-        <v>2.7222000200616119</v>
+        <v>3.4597807502312663</v>
       </c>
       <c r="K367" s="10">
         <f t="shared" si="44"/>
-        <v>5.885378930846049E-2</v>
+        <v>7.3098869350614881E-2</v>
       </c>
       <c r="L367" t="s">
         <v>755</v>
@@ -24200,17 +24212,20 @@
       <c r="G368">
         <v>85.126629119370165</v>
       </c>
+      <c r="H368">
+        <v>98.986595991902675</v>
+      </c>
       <c r="I368" s="1">
         <f t="shared" si="42"/>
-        <v>89.200329266298382</v>
+        <v>90.831373720565765</v>
       </c>
       <c r="J368">
         <f t="shared" si="43"/>
-        <v>4.5352589345748235</v>
+        <v>5.5174276671303897</v>
       </c>
       <c r="K368" s="10">
         <f t="shared" si="44"/>
-        <v>5.0843522348838821E-2</v>
+        <v>6.0743633406935366E-2</v>
       </c>
       <c r="L368" t="s">
         <v>755</v>
@@ -24250,17 +24265,20 @@
       <c r="G369">
         <v>70.270230392106086</v>
       </c>
+      <c r="H369">
+        <v>81.689905126624836</v>
+      </c>
       <c r="I369" s="1">
         <f t="shared" si="42"/>
-        <v>75.792480144881964</v>
+        <v>76.775384308505764</v>
       </c>
       <c r="J369">
         <f t="shared" si="43"/>
-        <v>6.9001128310101905</v>
+        <v>6.6713417347315804</v>
       </c>
       <c r="K369" s="10">
         <f t="shared" si="44"/>
-        <v>9.1039543999882344E-2</v>
+        <v>8.6894279915606734E-2</v>
       </c>
       <c r="L369" t="s">
         <v>755</v>
@@ -24300,17 +24318,20 @@
       <c r="G370">
         <v>42.865791431202901</v>
       </c>
+      <c r="H370">
+        <v>46.891721133213217</v>
+      </c>
       <c r="I370" s="1">
         <f t="shared" si="42"/>
-        <v>45.456109903270217</v>
+        <v>45.695378441594045</v>
       </c>
       <c r="J370">
         <f t="shared" si="43"/>
-        <v>4.6350159248902498</v>
+        <v>4.2648631498732517</v>
       </c>
       <c r="K370" s="10">
         <f t="shared" si="44"/>
-        <v>0.10196684086591395</v>
+        <v>9.3332483400360156E-2</v>
       </c>
       <c r="L370" t="s">
         <v>755</v>
@@ -24350,17 +24371,20 @@
       <c r="G371">
         <v>46.292634353244722</v>
       </c>
+      <c r="H371">
+        <v>53.195031471752053</v>
+      </c>
       <c r="I371" s="1">
         <f t="shared" si="42"/>
-        <v>48.289162539379632</v>
+        <v>49.106807361441703</v>
       </c>
       <c r="J371">
         <f t="shared" si="43"/>
-        <v>4.377130531390554</v>
+        <v>4.394175123492162</v>
       </c>
       <c r="K371" s="10">
         <f t="shared" si="44"/>
-        <v>9.0644159086855566E-2</v>
+        <v>8.9481995666092426E-2</v>
       </c>
       <c r="L371" t="s">
         <v>755</v>
@@ -24400,17 +24424,20 @@
       <c r="G372">
         <v>48.586565787788139</v>
       </c>
+      <c r="H372">
+        <v>50.338237293340079</v>
+      </c>
       <c r="I372" s="1">
         <f t="shared" si="42"/>
-        <v>48.573331195695054</v>
+        <v>48.867482211969225</v>
       </c>
       <c r="J372">
         <f t="shared" si="43"/>
-        <v>2.9919528865687921</v>
+        <v>2.8093491235661228</v>
       </c>
       <c r="K372" s="10">
         <f t="shared" si="44"/>
-        <v>6.159661717485751E-2</v>
+        <v>5.7489131758010285E-2</v>
       </c>
       <c r="L372" t="s">
         <v>755</v>
@@ -24450,17 +24477,20 @@
       <c r="G373">
         <v>61.786596843429173</v>
       </c>
+      <c r="H373">
+        <v>52.832983975273002</v>
+      </c>
       <c r="I373" s="1">
         <f t="shared" si="42"/>
-        <v>58.443378295064647</v>
+        <v>57.508312575099374</v>
       </c>
       <c r="J373">
         <f t="shared" si="43"/>
-        <v>3.3923537196002531</v>
+        <v>3.7365482247223332</v>
       </c>
       <c r="K373" s="10">
         <f t="shared" si="44"/>
-        <v>5.8045133915311777E-2</v>
+        <v>6.49740543133277E-2</v>
       </c>
       <c r="L373" t="s">
         <v>755</v>
@@ -24500,17 +24530,20 @@
       <c r="G374">
         <v>37.658984280693687</v>
       </c>
+      <c r="H374">
+        <v>34.530121678835783</v>
+      </c>
       <c r="I374" s="1">
         <f t="shared" si="42"/>
-        <v>34.032090238161729</v>
+        <v>34.115095478274071</v>
       </c>
       <c r="J374">
         <f t="shared" si="43"/>
-        <v>8.4373491191066421</v>
+        <v>7.7044467342462868</v>
       </c>
       <c r="K374" s="10">
         <f t="shared" si="44"/>
-        <v>0.24792332942410511</v>
+        <v>0.22583688030868337</v>
       </c>
       <c r="L374" t="s">
         <v>755</v>
@@ -24550,17 +24583,20 @@
       <c r="G375">
         <v>57.492888409539987</v>
       </c>
+      <c r="H375">
+        <v>57.121670329996313</v>
+      </c>
       <c r="I375" s="1">
         <f t="shared" si="42"/>
-        <v>61.418309575974945</v>
+        <v>60.70220303497851</v>
       </c>
       <c r="J375">
         <f t="shared" si="43"/>
-        <v>2.8254613940058757</v>
+        <v>3.0359078210321395</v>
       </c>
       <c r="K375" s="10">
         <f t="shared" si="44"/>
-        <v>4.6003568211377702E-2</v>
+        <v>5.0013140697426656E-2</v>
       </c>
       <c r="L375" t="s">
         <v>755</v>
@@ -24600,17 +24636,20 @@
       <c r="G376">
         <v>57.791824067068923</v>
       </c>
+      <c r="H376">
+        <v>60.108527191249053</v>
+      </c>
       <c r="I376" s="1">
         <f t="shared" si="42"/>
-        <v>62.717331321051496</v>
+        <v>62.282530632751083</v>
       </c>
       <c r="J376">
         <f t="shared" si="43"/>
-        <v>5.4770778943640464</v>
+        <v>5.0935164745823638</v>
       </c>
       <c r="K376" s="10">
         <f t="shared" si="44"/>
-        <v>8.7329575079123756E-2</v>
+        <v>8.1780820766842011E-2</v>
       </c>
       <c r="L376" t="s">
         <v>755</v>
@@ -24650,17 +24689,20 @@
       <c r="G377">
         <v>55.188967361899209</v>
       </c>
+      <c r="H377">
+        <v>55.257429179997423</v>
+      </c>
       <c r="I377" s="1">
         <f t="shared" si="42"/>
-        <v>53.65796966431477</v>
+        <v>53.924546250261876</v>
       </c>
       <c r="J377">
         <f t="shared" si="43"/>
-        <v>2.6114243548601657</v>
+        <v>2.4572877355274128</v>
       </c>
       <c r="K377" s="10">
         <f t="shared" si="44"/>
-        <v>4.8667968079994149E-2</v>
+        <v>4.5569001621696158E-2</v>
       </c>
       <c r="L377" t="s">
         <v>755</v>
@@ -24700,17 +24742,20 @@
       <c r="G378">
         <v>60.240716716892408</v>
       </c>
+      <c r="H378">
+        <v>69.73117229520156</v>
+      </c>
       <c r="I378" s="1">
         <f t="shared" si="42"/>
-        <v>60.590221332337009</v>
+        <v>62.113713159481108</v>
       </c>
       <c r="J378">
         <f t="shared" si="43"/>
-        <v>3.2150207977698351</v>
+        <v>4.4965285512216386</v>
       </c>
       <c r="K378" s="10">
         <f t="shared" si="44"/>
-        <v>5.3061710736052023E-2</v>
+        <v>7.2391881317359033E-2</v>
       </c>
       <c r="L378" t="s">
         <v>755</v>
@@ -24750,17 +24795,20 @@
       <c r="G379">
         <v>44.672296260783739</v>
       </c>
+      <c r="H379">
+        <v>37.476025835442357</v>
+      </c>
       <c r="I379" s="1">
         <f t="shared" si="42"/>
-        <v>45.788340032977636</v>
+        <v>44.402954333388415</v>
       </c>
       <c r="J379">
         <f t="shared" si="43"/>
-        <v>1.1637726434699562</v>
+        <v>3.2749208623322494</v>
       </c>
       <c r="K379" s="10">
         <f t="shared" si="44"/>
-        <v>2.5416353653174257E-2</v>
+        <v>7.375457132296491E-2</v>
       </c>
       <c r="L379" t="s">
         <v>755</v>
@@ -24800,17 +24848,20 @@
       <c r="G380">
         <v>60.331177021018767</v>
       </c>
+      <c r="H380">
+        <v>68.364318749681345</v>
+      </c>
       <c r="I380" s="1">
         <f t="shared" si="42"/>
-        <v>63.538449009189229</v>
+        <v>64.34276063260458</v>
       </c>
       <c r="J380">
         <f t="shared" si="43"/>
-        <v>2.62115955829031</v>
+        <v>2.9933232027551626</v>
       </c>
       <c r="K380" s="10">
         <f t="shared" si="44"/>
-        <v>4.1253124669618953E-2</v>
+        <v>4.6521522752916322E-2</v>
       </c>
       <c r="L380" t="s">
         <v>755</v>
@@ -24850,17 +24901,20 @@
       <c r="G381">
         <v>30.836770600840481</v>
       </c>
+      <c r="H381">
+        <v>10.767209344720291</v>
+      </c>
       <c r="I381" s="1">
         <f t="shared" si="42"/>
-        <v>20.127447338283002</v>
+        <v>18.567407672689217</v>
       </c>
       <c r="J381">
         <f t="shared" si="43"/>
-        <v>10.015003132454378</v>
+        <v>9.7853048961366422</v>
       </c>
       <c r="K381" s="10">
         <f t="shared" si="44"/>
-        <v>0.49757939812891949</v>
+        <v>0.5270151368804078</v>
       </c>
       <c r="L381" t="s">
         <v>755</v>
@@ -24900,17 +24954,20 @@
       <c r="G382">
         <v>45.885147859558437</v>
       </c>
+      <c r="H382">
+        <v>49.729308301140591</v>
+      </c>
       <c r="I382" s="1">
         <f t="shared" si="42"/>
-        <v>47.771680906137902</v>
+        <v>48.097952138638355</v>
       </c>
       <c r="J382">
         <f t="shared" si="43"/>
-        <v>2.3148951308941945</v>
+        <v>2.2355940616127477</v>
       </c>
       <c r="K382" s="10">
         <f t="shared" si="44"/>
-        <v>4.8457477044664077E-2</v>
+        <v>4.6480025909810742E-2</v>
       </c>
       <c r="L382" t="s">
         <v>755</v>
@@ -24950,17 +25007,20 @@
       <c r="G383">
         <v>70.338541253403648</v>
       </c>
+      <c r="H383">
+        <v>74.241344574141152</v>
+      </c>
       <c r="I383" s="1">
         <f t="shared" si="42"/>
-        <v>72.382866423339749</v>
+        <v>72.692612781806645</v>
       </c>
       <c r="J383">
         <f t="shared" si="43"/>
-        <v>5.6101798433321957</v>
+        <v>5.1679924143739386</v>
       </c>
       <c r="K383" s="10">
         <f t="shared" si="44"/>
-        <v>7.7507014028988519E-2</v>
+        <v>7.1093777161183189E-2</v>
       </c>
       <c r="L383" t="s">
         <v>755</v>
@@ -25000,17 +25060,20 @@
       <c r="G384">
         <v>40.942247231158618</v>
       </c>
+      <c r="H384">
+        <v>44.702434421807887</v>
+      </c>
       <c r="I384" s="1">
         <f t="shared" si="42"/>
-        <v>42.982518811111348</v>
+        <v>43.269171412894103</v>
       </c>
       <c r="J384">
         <f t="shared" si="43"/>
-        <v>1.6875020186727852</v>
+        <v>1.6685026589924044</v>
       </c>
       <c r="K384" s="10">
         <f t="shared" si="44"/>
-        <v>3.9260193803173568E-2</v>
+        <v>3.856100323879081E-2</v>
       </c>
       <c r="L384" t="s">
         <v>755</v>
@@ -25050,17 +25113,20 @@
       <c r="G385">
         <v>11.371566441044701</v>
       </c>
+      <c r="H385">
+        <v>9.5262334215032247</v>
+      </c>
       <c r="I385" s="1">
         <f t="shared" si="42"/>
-        <v>8.5139294907491294</v>
+        <v>8.6826468125414777</v>
       </c>
       <c r="J385">
         <f t="shared" si="43"/>
-        <v>3.8351575108074321</v>
+        <v>3.5212718276142057</v>
       </c>
       <c r="K385" s="10">
         <f t="shared" si="44"/>
-        <v>0.45045680904153007</v>
+        <v>0.40555281167580998</v>
       </c>
       <c r="L385" t="s">
         <v>755</v>
@@ -25100,17 +25166,20 @@
       <c r="G386">
         <v>42.663705749243071</v>
       </c>
+      <c r="H386">
+        <v>45.580796668487203</v>
+      </c>
       <c r="I386" s="1">
         <f t="shared" si="42"/>
-        <v>43.400381228483155</v>
+        <v>43.763783801817162</v>
       </c>
       <c r="J386">
         <f t="shared" si="43"/>
-        <v>1.799606265909621</v>
+        <v>1.8327918808327743</v>
       </c>
       <c r="K386" s="10">
         <f t="shared" si="44"/>
-        <v>4.1465217930587224E-2</v>
+        <v>4.1879191459598453E-2</v>
       </c>
       <c r="L386" t="s">
         <v>755</v>
@@ -25150,17 +25219,20 @@
       <c r="G387">
         <v>48.345296633384912</v>
       </c>
+      <c r="H387">
+        <v>52.020993709698132</v>
+      </c>
       <c r="I387" s="1">
         <f t="shared" si="42"/>
-        <v>48.854225724814661</v>
+        <v>49.382020388961905</v>
       </c>
       <c r="J387">
         <f t="shared" si="43"/>
-        <v>4.5589548298509532</v>
+        <v>4.3258402252852521</v>
       </c>
       <c r="K387" s="10">
         <f t="shared" si="44"/>
-        <v>9.3317512706691225E-2</v>
+        <v>8.7599498586983363E-2</v>
       </c>
       <c r="L387" t="s">
         <v>755</v>
@@ -25200,17 +25272,20 @@
       <c r="G388">
         <v>50.884382379155042</v>
       </c>
+      <c r="H388">
+        <v>52.681928165303283</v>
+      </c>
       <c r="I388" s="1">
         <f t="shared" si="42"/>
-        <v>52.241640568357219</v>
+        <v>52.315021834514901</v>
       </c>
       <c r="J388">
         <f t="shared" si="43"/>
-        <v>4.5286438947720358</v>
+        <v>4.1373224420101966</v>
       </c>
       <c r="K388" s="10">
         <f t="shared" si="44"/>
-        <v>8.6686479320005061E-2</v>
+        <v>7.9084788592797509E-2</v>
       </c>
       <c r="L388" t="s">
         <v>755</v>
@@ -25250,17 +25325,20 @@
       <c r="G389">
         <v>55.368283655818033</v>
       </c>
+      <c r="H389">
+        <v>61.781376439365637</v>
+      </c>
       <c r="I389" s="1">
         <f t="shared" si="42"/>
-        <v>56.040166155295722</v>
+        <v>56.997034535974045</v>
       </c>
       <c r="J389">
         <f t="shared" si="43"/>
-        <v>3.3142953567412032</v>
+        <v>3.7056416785049957</v>
       </c>
       <c r="K389" s="10">
         <f t="shared" si="44"/>
-        <v>5.9141426304068989E-2</v>
+        <v>6.5014639948788144E-2</v>
       </c>
       <c r="L389" t="s">
         <v>755</v>
@@ -25300,17 +25378,20 @@
       <c r="G390">
         <v>65.719450292938603</v>
       </c>
+      <c r="H390">
+        <v>59.591432273083527</v>
+      </c>
       <c r="I390" s="1">
         <f t="shared" si="42"/>
-        <v>65.609836927970719</v>
+        <v>64.606769485489522</v>
       </c>
       <c r="J390">
         <f t="shared" si="43"/>
-        <v>2.8834088344212212</v>
+        <v>3.4581922386574795</v>
       </c>
       <c r="K390" s="10">
         <f t="shared" si="44"/>
-        <v>4.3947812849874181E-2</v>
+        <v>5.3526778481536343E-2</v>
       </c>
       <c r="L390" t="s">
         <v>755</v>
@@ -25350,17 +25431,20 @@
       <c r="G391">
         <v>11.05057097886449</v>
       </c>
+      <c r="H391">
+        <v>17.078030945155199</v>
+      </c>
       <c r="I391" s="1">
         <f t="shared" si="42"/>
-        <v>11.49550543772399</v>
+        <v>12.425926355629192</v>
       </c>
       <c r="J391">
         <f t="shared" si="43"/>
-        <v>4.3773732048249521</v>
+        <v>4.5051354660702509</v>
       </c>
       <c r="K391" s="10">
         <f t="shared" si="44"/>
-        <v>0.38078997296282729</v>
+        <v>0.36255932452306339</v>
       </c>
       <c r="L391" t="s">
         <v>755</v>
@@ -25400,17 +25484,20 @@
       <c r="G392">
         <v>51.2850048251739</v>
       </c>
+      <c r="H392">
+        <v>54.884699746481978</v>
+      </c>
       <c r="I392" s="1">
         <f t="shared" si="42"/>
-        <v>53.836695742074404</v>
+        <v>54.011363076142338</v>
       </c>
       <c r="J392">
         <f t="shared" si="43"/>
-        <v>2.6295700028599613</v>
+        <v>2.4320242709663558</v>
       </c>
       <c r="K392" s="10">
         <f t="shared" si="44"/>
-        <v>4.8843450858461625E-2</v>
+        <v>4.5028011374899347E-2</v>
       </c>
       <c r="L392" t="s">
         <v>755</v>
@@ -25450,17 +25537,20 @@
       <c r="G393">
         <v>16.2984289005914</v>
       </c>
+      <c r="H393">
+        <v>12.064753148722829</v>
+      </c>
       <c r="I393" s="1">
         <f t="shared" si="42"/>
-        <v>12.153693068170464</v>
+        <v>12.138869748262524</v>
       </c>
       <c r="J393">
         <f t="shared" si="43"/>
-        <v>2.3602974401009718</v>
+        <v>2.154901852100954</v>
       </c>
       <c r="K393" s="10">
         <f t="shared" si="44"/>
-        <v>0.1942041342382094</v>
+        <v>0.17752079862372624</v>
       </c>
       <c r="L393" t="s">
         <v>755</v>
@@ -25500,17 +25590,20 @@
       <c r="G394">
         <v>33.786465171271409</v>
       </c>
+      <c r="H394">
+        <v>40.065938939720851</v>
+      </c>
       <c r="I394" s="1">
         <f t="shared" ref="I394:I425" si="45">AVERAGE(C394:H394)</f>
-        <v>37.405570962160539</v>
+        <v>37.84896562508726</v>
       </c>
       <c r="J394">
         <f t="shared" ref="J394:J425" si="46">_xlfn.STDEV.P(C394:H394)</f>
-        <v>3.4065176732680138</v>
+        <v>3.2639387786536269</v>
       </c>
       <c r="K394" s="10">
         <f t="shared" ref="K394:K425" si="47">J394/I394</f>
-        <v>9.1069794836551102E-2</v>
+        <v>8.6235877909704481E-2</v>
       </c>
       <c r="L394" t="s">
         <v>755</v>
@@ -25550,17 +25643,20 @@
       <c r="G395">
         <v>4.0358196432219744</v>
       </c>
+      <c r="H395">
+        <v>14.40178647962952</v>
+      </c>
       <c r="I395" s="1">
         <f t="shared" si="45"/>
-        <v>5.1825768292838177</v>
+        <v>6.7191117710081016</v>
       </c>
       <c r="J395">
         <f t="shared" si="46"/>
-        <v>2.0547940197124799</v>
+        <v>3.914483387187897</v>
       </c>
       <c r="K395" s="10">
         <f t="shared" si="47"/>
-        <v>0.39648114970568271</v>
+        <v>0.58258941368980799</v>
       </c>
       <c r="L395" t="s">
         <v>755</v>
@@ -25600,17 +25696,20 @@
       <c r="G396">
         <v>10.204995486870001</v>
       </c>
+      <c r="H396">
+        <v>14.552269951839801</v>
+      </c>
       <c r="I396" s="1">
         <f t="shared" si="45"/>
-        <v>9.7888824735395641</v>
+        <v>10.582780386589604</v>
       </c>
       <c r="J396">
         <f t="shared" si="46"/>
-        <v>2.8419489237343769</v>
+        <v>3.143553862428397</v>
       </c>
       <c r="K396" s="10">
         <f t="shared" si="47"/>
-        <v>0.29032414388634048</v>
+        <v>0.29704423106160999</v>
       </c>
       <c r="L396" t="s">
         <v>755</v>
@@ -25650,17 +25749,20 @@
       <c r="G397">
         <v>15.258897660739519</v>
       </c>
+      <c r="H397">
+        <v>19.67689885313218</v>
+      </c>
       <c r="I397" s="1">
         <f t="shared" si="45"/>
-        <v>20.850319556883878</v>
+        <v>20.654749439591928</v>
       </c>
       <c r="J397">
         <f t="shared" si="46"/>
-        <v>7.3412453187680162</v>
+        <v>6.7158623704752669</v>
       </c>
       <c r="K397" s="10">
         <f t="shared" si="47"/>
-        <v>0.35209270048545865</v>
+        <v>0.32514857612370779</v>
       </c>
       <c r="L397" t="s">
         <v>755</v>
@@ -25700,17 +25802,20 @@
       <c r="G398">
         <v>16.579407854771219</v>
       </c>
+      <c r="H398">
+        <v>12.424315041499771</v>
+      </c>
       <c r="I398" s="1">
         <f t="shared" si="45"/>
-        <v>11.791941904888535</v>
+        <v>11.897337427657076</v>
       </c>
       <c r="J398">
         <f t="shared" si="46"/>
-        <v>4.4081894805183675</v>
+        <v>4.0310031623107072</v>
       </c>
       <c r="K398" s="10">
         <f t="shared" si="47"/>
-        <v>0.37383066470933707</v>
+        <v>0.33881557002326074</v>
       </c>
       <c r="L398" t="s">
         <v>755</v>
@@ -25750,17 +25855,20 @@
       <c r="G399">
         <v>39.008302640655103</v>
       </c>
+      <c r="H399">
+        <v>49.241810504658517</v>
+      </c>
       <c r="I399" s="1">
         <f t="shared" si="45"/>
-        <v>45.222716226365165</v>
+        <v>45.89256527274739</v>
       </c>
       <c r="J399">
         <f t="shared" si="46"/>
-        <v>3.7478469764063993</v>
+        <v>3.7348073832744535</v>
       </c>
       <c r="K399" s="10">
         <f t="shared" si="47"/>
-        <v>8.2875317741780793E-2</v>
+        <v>8.1381534483371154E-2</v>
       </c>
       <c r="L399" t="s">
         <v>755</v>
@@ -25800,17 +25908,20 @@
       <c r="G400">
         <v>71.909924408382949</v>
       </c>
+      <c r="H400">
+        <v>79.167920389744722</v>
+      </c>
       <c r="I400" s="1">
         <f t="shared" si="45"/>
-        <v>70.376876666665453</v>
+        <v>71.842050620511998</v>
       </c>
       <c r="J400">
         <f t="shared" si="46"/>
-        <v>5.9492340611454351</v>
+        <v>6.342567448365247</v>
       </c>
       <c r="K400" s="10">
         <f t="shared" si="47"/>
-        <v>8.4533931355372793E-2</v>
+        <v>8.8284888774518747E-2</v>
       </c>
       <c r="L400" t="s">
         <v>755</v>
@@ -25850,17 +25961,20 @@
       <c r="G401">
         <v>37.378409934435567</v>
       </c>
+      <c r="H401">
+        <v>30.660243388375239</v>
+      </c>
       <c r="I401" s="1">
         <f t="shared" si="45"/>
-        <v>33.553497904290666</v>
+        <v>33.071288818304765</v>
       </c>
       <c r="J401">
         <f t="shared" si="46"/>
-        <v>4.0133970725819221</v>
+        <v>3.819086897616256</v>
       </c>
       <c r="K401" s="10">
         <f t="shared" si="47"/>
-        <v>0.11961188320901432</v>
+        <v>0.11548043738478114</v>
       </c>
       <c r="L401" t="s">
         <v>755</v>
@@ -25900,17 +26014,20 @@
       <c r="G402">
         <v>52.243640363036803</v>
       </c>
+      <c r="H402">
+        <v>46.627605259773581</v>
+      </c>
       <c r="I402" s="1">
         <f t="shared" si="45"/>
-        <v>51.31341429528004</v>
+        <v>50.532446122695632</v>
       </c>
       <c r="J402">
         <f t="shared" si="46"/>
-        <v>2.3064275838024795</v>
+        <v>2.7354274374802841</v>
       </c>
       <c r="K402" s="10">
         <f t="shared" si="47"/>
-        <v>4.4947848734646204E-2</v>
+        <v>5.4132100212178763E-2</v>
       </c>
       <c r="L402" t="s">
         <v>755</v>
@@ -25950,17 +26067,20 @@
       <c r="G403">
         <v>38.786465031148559</v>
       </c>
+      <c r="H403">
+        <v>37.397291652262993</v>
+      </c>
       <c r="I403" s="1">
         <f t="shared" si="45"/>
-        <v>37.965149756600397</v>
+        <v>37.870506739210832</v>
       </c>
       <c r="J403">
         <f t="shared" si="46"/>
-        <v>2.0403362686452868</v>
+        <v>1.8745479218540892</v>
       </c>
       <c r="K403" s="10">
         <f t="shared" si="47"/>
-        <v>5.3742347435112275E-2</v>
+        <v>4.9498886686752376E-2</v>
       </c>
       <c r="L403" t="s">
         <v>755</v>
@@ -26000,17 +26120,20 @@
       <c r="G404">
         <v>7.1311622389893516</v>
       </c>
+      <c r="H404">
+        <v>19.265871266327661</v>
+      </c>
       <c r="I404" s="1">
         <f t="shared" si="45"/>
-        <v>25.569752670711157</v>
+        <v>24.519105769980573</v>
       </c>
       <c r="J404">
         <f t="shared" si="46"/>
-        <v>10.278731023442713</v>
+        <v>9.6727910877355807</v>
       </c>
       <c r="K404" s="10">
         <f t="shared" si="47"/>
-        <v>0.40198789389216399</v>
+        <v>0.39450015748854306</v>
       </c>
       <c r="L404" t="s">
         <v>755</v>
@@ -26050,17 +26173,20 @@
       <c r="G405">
         <v>12.878025001608711</v>
       </c>
+      <c r="H405">
+        <v>28.23783785546312</v>
+      </c>
       <c r="I405" s="1">
         <f t="shared" si="45"/>
-        <v>14.212396079376457</v>
+        <v>16.549969708724234</v>
       </c>
       <c r="J405">
         <f t="shared" si="46"/>
-        <v>3.6485797805178719</v>
+        <v>6.1979591567531847</v>
       </c>
       <c r="K405" s="10">
         <f t="shared" si="47"/>
-        <v>0.25671813254714376</v>
+        <v>0.3744997281466903</v>
       </c>
       <c r="L405" t="s">
         <v>755</v>
@@ -26100,17 +26226,20 @@
       <c r="G406">
         <v>10.9547399890725</v>
       </c>
+      <c r="H406">
+        <v>18.269370567657749</v>
+      </c>
       <c r="I406" s="1">
         <f t="shared" si="45"/>
-        <v>14.280251973841104</v>
+        <v>14.945105072810543</v>
       </c>
       <c r="J406">
         <f t="shared" si="46"/>
-        <v>4.2974671259864667</v>
+        <v>4.1952752748568249</v>
       </c>
       <c r="K406" s="10">
         <f t="shared" si="47"/>
-        <v>0.30093776593428928</v>
+        <v>0.28071233052012734</v>
       </c>
       <c r="L406" t="s">
         <v>755</v>
@@ -26150,17 +26279,20 @@
       <c r="G407">
         <v>7.1109106564658786</v>
       </c>
+      <c r="H407">
+        <v>2.8988874774730462</v>
+      </c>
       <c r="I407" s="1">
         <f t="shared" si="45"/>
-        <v>11.974231236894624</v>
+        <v>10.461673943657695</v>
       </c>
       <c r="J407">
         <f t="shared" si="46"/>
-        <v>3.8097365152387712</v>
+        <v>4.8512085871709187</v>
       </c>
       <c r="K407" s="10">
         <f t="shared" si="47"/>
-        <v>0.31816126145120122</v>
+        <v>0.46371246258462534</v>
       </c>
       <c r="L407" t="s">
         <v>755</v>
@@ -26200,17 +26332,20 @@
       <c r="G408">
         <v>57.415773847073822</v>
       </c>
+      <c r="H408">
+        <v>59.638148240511057</v>
+      </c>
       <c r="I408" s="1">
         <f t="shared" si="45"/>
-        <v>58.668219762553619</v>
+        <v>58.829874508879861</v>
       </c>
       <c r="J408">
         <f t="shared" si="46"/>
-        <v>2.2749515854682301</v>
+        <v>2.1079607559367299</v>
       </c>
       <c r="K408" s="10">
         <f t="shared" si="47"/>
-        <v>3.8776557302668858E-2</v>
+        <v>3.583146783049064E-2</v>
       </c>
       <c r="L408" t="s">
         <v>755</v>
@@ -26250,17 +26385,20 @@
       <c r="G409">
         <v>17.43177591482392</v>
       </c>
+      <c r="H409">
+        <v>12.54632059900956</v>
+      </c>
       <c r="I409" s="1">
         <f t="shared" si="45"/>
-        <v>13.716613797134642</v>
+        <v>13.521564930780462</v>
       </c>
       <c r="J409">
         <f t="shared" si="46"/>
-        <v>2.8235099540689479</v>
+        <v>2.6141398875989066</v>
       </c>
       <c r="K409" s="10">
         <f t="shared" si="47"/>
-        <v>0.20584599055043529</v>
+        <v>0.19333116403176706</v>
       </c>
       <c r="L409" t="s">
         <v>755</v>
@@ -26300,17 +26438,20 @@
       <c r="G410">
         <v>6.5771661870789098</v>
       </c>
+      <c r="H410">
+        <v>14.91351924697774</v>
+      </c>
       <c r="I410" s="1">
         <f t="shared" si="45"/>
-        <v>10.000091817756616</v>
+        <v>10.818996389293469</v>
       </c>
       <c r="J410">
         <f t="shared" si="46"/>
-        <v>4.3448618405739845</v>
+        <v>4.3685860219468911</v>
       </c>
       <c r="K410" s="10">
         <f t="shared" si="47"/>
-        <v>0.4344821947393574</v>
+        <v>0.40378847212390834</v>
       </c>
       <c r="L410" t="s">
         <v>755</v>
@@ -26350,17 +26491,20 @@
       <c r="G411">
         <v>22.02650094316903</v>
       </c>
+      <c r="H411">
+        <v>34.443336981783638</v>
+      </c>
       <c r="I411" s="1">
         <f t="shared" si="45"/>
-        <v>26.271310358538294</v>
+        <v>27.63331479574585</v>
       </c>
       <c r="J411">
         <f t="shared" si="46"/>
-        <v>7.1954441183784184</v>
+        <v>7.240209054448683</v>
       </c>
       <c r="K411" s="10">
         <f t="shared" si="47"/>
-        <v>0.27388980679602326</v>
+        <v>0.2620101536122374</v>
       </c>
       <c r="L411" t="s">
         <v>755</v>
@@ -26400,17 +26544,20 @@
       <c r="G412">
         <v>57.595236062111198</v>
       </c>
+      <c r="H412">
+        <v>55.437517787406897</v>
+      </c>
       <c r="I412" s="1">
         <f t="shared" si="45"/>
-        <v>52.45433783996684</v>
+        <v>52.951534497873517</v>
       </c>
       <c r="J412">
         <f t="shared" si="46"/>
-        <v>5.126561405177843</v>
+        <v>4.8101333090380161</v>
       </c>
       <c r="K412" s="10">
         <f t="shared" si="47"/>
-        <v>9.7733793167277996E-2</v>
+        <v>9.0840300562605725E-2</v>
       </c>
       <c r="L412" t="s">
         <v>755</v>
@@ -26450,17 +26597,20 @@
       <c r="G413">
         <v>65.21516648653936</v>
       </c>
+      <c r="H413">
+        <v>64.222916947331498</v>
+      </c>
       <c r="I413" s="1">
         <f t="shared" si="45"/>
-        <v>61.988576921397581</v>
+        <v>62.3609669257199</v>
       </c>
       <c r="J413">
         <f t="shared" si="46"/>
-        <v>5.0585367309455389</v>
+        <v>4.6922666653264224</v>
       </c>
       <c r="K413" s="10">
         <f t="shared" si="47"/>
-        <v>8.1604337156502837E-2</v>
+        <v>7.5243648337196697E-2</v>
       </c>
       <c r="L413" t="s">
         <v>755</v>
@@ -26500,17 +26650,20 @@
       <c r="G414">
         <v>14.348476129754649</v>
       </c>
+      <c r="H414">
+        <v>18.459238607115491</v>
+      </c>
       <c r="I414" s="1">
         <f t="shared" si="45"/>
-        <v>14.029822758085285</v>
+        <v>14.768058732923654</v>
       </c>
       <c r="J414">
         <f t="shared" si="46"/>
-        <v>5.0619461235477408</v>
+        <v>4.9069043775899184</v>
       </c>
       <c r="K414" s="10">
         <f t="shared" si="47"/>
-        <v>0.36079900728828368</v>
+        <v>0.33226468463661718</v>
       </c>
       <c r="L414" t="s">
         <v>755</v>
@@ -26550,17 +26703,20 @@
       <c r="G415">
         <v>9.1097993835229847</v>
       </c>
+      <c r="H415">
+        <v>16.186451589261669</v>
+      </c>
       <c r="I415" s="1">
         <f t="shared" si="45"/>
-        <v>11.875778062911008</v>
+        <v>12.594223650636119</v>
       </c>
       <c r="J415">
         <f t="shared" si="46"/>
-        <v>1.962411973731891</v>
+        <v>2.4062496977967456</v>
       </c>
       <c r="K415" s="10">
         <f t="shared" si="47"/>
-        <v>0.16524491812967257</v>
+        <v>0.19105978776827651</v>
       </c>
       <c r="L415" t="s">
         <v>755</v>
@@ -26600,17 +26756,20 @@
       <c r="G416">
         <v>14.37272158978136</v>
       </c>
+      <c r="H416">
+        <v>9.1822226583546573</v>
+      </c>
       <c r="I416" s="1">
         <f t="shared" si="45"/>
-        <v>10.114803053340051</v>
+        <v>9.9593729875091537</v>
       </c>
       <c r="J416">
         <f t="shared" si="46"/>
-        <v>3.7485721816154176</v>
+        <v>3.4395668856420141</v>
       </c>
       <c r="K416" s="10">
         <f t="shared" si="47"/>
-        <v>0.37060258730174545</v>
+        <v>0.3453597821826585</v>
       </c>
       <c r="L416" t="s">
         <v>755</v>
@@ -26650,17 +26809,20 @@
       <c r="G417">
         <v>17.594089197052721</v>
       </c>
+      <c r="H417">
+        <v>15.868521840111701</v>
+      </c>
       <c r="I417" s="1">
         <f t="shared" si="45"/>
-        <v>17.551477005623845</v>
+        <v>17.270984478038489</v>
       </c>
       <c r="J417">
         <f t="shared" si="46"/>
-        <v>7.3876147251244335</v>
+        <v>6.7730413943234442</v>
       </c>
       <c r="K417" s="10">
         <f t="shared" si="47"/>
-        <v>0.42091128414761297</v>
+        <v>0.39216301786015362</v>
       </c>
       <c r="L417" t="s">
         <v>755</v>
@@ -26700,17 +26862,20 @@
       <c r="G418">
         <v>13.7626075720072</v>
       </c>
+      <c r="H418">
+        <v>9.5384311084947342</v>
+      </c>
       <c r="I418" s="1">
         <f t="shared" si="45"/>
-        <v>9.4550151992005471</v>
+        <v>9.4689178507495786</v>
       </c>
       <c r="J418">
         <f t="shared" si="46"/>
-        <v>3.6421973035942083</v>
+        <v>3.325001365993391</v>
       </c>
       <c r="K418" s="10">
         <f t="shared" si="47"/>
-        <v>0.38521326797043842</v>
+        <v>0.35114903502200912</v>
       </c>
       <c r="L418" t="s">
         <v>755</v>
@@ -26750,17 +26915,20 @@
       <c r="G419">
         <v>14.12607864395633</v>
       </c>
+      <c r="H419">
+        <v>13.60990855159921</v>
+      </c>
       <c r="I419" s="1">
         <f t="shared" si="45"/>
-        <v>21.287664088592923</v>
+        <v>20.008038165760635</v>
       </c>
       <c r="J419">
         <f t="shared" si="46"/>
-        <v>8.4357309769896176</v>
+        <v>8.2151390803021158</v>
       </c>
       <c r="K419" s="10">
         <f t="shared" si="47"/>
-        <v>0.39627320977457253</v>
+        <v>0.4105919337139472</v>
       </c>
       <c r="L419" t="s">
         <v>755</v>
@@ -26800,17 +26968,20 @@
       <c r="G420">
         <v>7.3979494499382641</v>
       </c>
+      <c r="H420">
+        <v>12.96908642165212</v>
+      </c>
       <c r="I420" s="1">
         <f t="shared" si="45"/>
-        <v>8.2600114544494438</v>
+        <v>9.0448572823165563</v>
       </c>
       <c r="J420">
         <f t="shared" si="46"/>
-        <v>1.7624209503352608</v>
+        <v>2.3808306406418898</v>
       </c>
       <c r="K420" s="10">
         <f t="shared" si="47"/>
-        <v>0.21336785790846483</v>
+        <v>0.26322478800153215</v>
       </c>
       <c r="L420" t="s">
         <v>755</v>
@@ -26850,17 +27021,20 @@
       <c r="G421">
         <v>38.080610121813841</v>
       </c>
+      <c r="H421">
+        <v>37.470972959654681</v>
+      </c>
       <c r="I421" s="1">
         <f t="shared" si="45"/>
-        <v>30.183966408807372</v>
+        <v>31.398467500615258</v>
       </c>
       <c r="J421">
         <f t="shared" si="46"/>
-        <v>7.8419508640738034</v>
+        <v>7.6564934732205687</v>
       </c>
       <c r="K421" s="10">
         <f t="shared" si="47"/>
-        <v>0.25980518126291058</v>
+        <v>0.24384927299622311</v>
       </c>
       <c r="L421" t="s">
         <v>755</v>
@@ -26900,17 +27074,20 @@
       <c r="G422">
         <v>6.4686342546618194</v>
       </c>
+      <c r="H422">
+        <v>16.047020431902531</v>
+      </c>
       <c r="I422" s="1">
         <f t="shared" si="45"/>
-        <v>17.041997338196182</v>
+        <v>16.876167853813907</v>
       </c>
       <c r="J422">
         <f t="shared" si="46"/>
-        <v>6.8352023691779928</v>
+        <v>6.2506658268645978</v>
       </c>
       <c r="K422" s="10">
         <f t="shared" si="47"/>
-        <v>0.40107988714786807</v>
+        <v>0.37038419391236305</v>
       </c>
       <c r="L422" t="s">
         <v>755</v>
@@ -26950,17 +27127,20 @@
       <c r="G423">
         <v>37.075570765004258</v>
       </c>
+      <c r="H423">
+        <v>23.51970890209228</v>
+      </c>
       <c r="I423" s="1">
         <f t="shared" si="45"/>
-        <v>23.951019271654324</v>
+        <v>23.879134210060652</v>
       </c>
       <c r="J423">
         <f t="shared" si="46"/>
-        <v>7.4862125163296014</v>
+        <v>6.835835879888907</v>
       </c>
       <c r="K423" s="10">
         <f t="shared" si="47"/>
-        <v>0.31256342084737171</v>
+        <v>0.28626816281340983</v>
       </c>
       <c r="L423" t="s">
         <v>755</v>
@@ -27000,17 +27180,20 @@
       <c r="G424">
         <v>51.168249535159148</v>
       </c>
+      <c r="H424">
+        <v>49.454576897244188</v>
+      </c>
       <c r="I424" s="1">
         <f t="shared" si="45"/>
-        <v>49.187293502140619</v>
+        <v>49.231840734657879</v>
       </c>
       <c r="J424">
         <f t="shared" si="46"/>
-        <v>4.2537223702883997</v>
+        <v>3.8843769061718723</v>
       </c>
       <c r="K424" s="10">
         <f t="shared" si="47"/>
-        <v>8.6480106292152026E-2</v>
+        <v>7.8899688660988385E-2</v>
       </c>
       <c r="L424" t="s">
         <v>755</v>
@@ -27050,17 +27233,20 @@
       <c r="G425">
         <v>43.174721238156643</v>
       </c>
+      <c r="H425">
+        <v>43.16861448315462</v>
+      </c>
       <c r="I425" s="1">
         <f t="shared" si="45"/>
-        <v>41.897089388194999</v>
+        <v>42.10901023735493</v>
       </c>
       <c r="J425">
         <f t="shared" si="46"/>
-        <v>4.1254774280879429</v>
+        <v>3.7957242048910675</v>
       </c>
       <c r="K425" s="10">
         <f t="shared" si="47"/>
-        <v>9.8466921887188308E-2</v>
+        <v>9.0140427986689614E-2</v>
       </c>
       <c r="L425" t="s">
         <v>755</v>
@@ -27100,17 +27286,20 @@
       <c r="G426">
         <v>14.518603903067961</v>
       </c>
+      <c r="H426">
+        <v>26.109849914075841</v>
+      </c>
       <c r="I426" s="1">
         <f t="shared" ref="I426:I456" si="48">AVERAGE(C426:H426)</f>
-        <v>12.897302391301741</v>
+        <v>15.099393645097424</v>
       </c>
       <c r="J426">
         <f t="shared" ref="J426:J456" si="49">_xlfn.STDEV.P(C426:H426)</f>
-        <v>2.4449048084275007</v>
+        <v>5.4062305770389116</v>
       </c>
       <c r="K426" s="10">
         <f t="shared" ref="K426:K456" si="50">J426/I426</f>
-        <v>0.18956714623333984</v>
+        <v>0.35804289258954741</v>
       </c>
       <c r="L426" t="s">
         <v>755</v>
@@ -27150,17 +27339,20 @@
       <c r="G427">
         <v>5.5865050042412259</v>
       </c>
+      <c r="H427">
+        <v>15.23971771962564</v>
+      </c>
       <c r="I427" s="1">
         <f t="shared" si="48"/>
-        <v>9.3334682650322822</v>
+        <v>10.317843174131175</v>
       </c>
       <c r="J427">
         <f t="shared" si="49"/>
-        <v>4.9380215369802052</v>
+        <v>5.0164745646769608</v>
       </c>
       <c r="K427" s="10">
         <f t="shared" si="50"/>
-        <v>0.52906608741366157</v>
+        <v>0.48619410859570256</v>
       </c>
       <c r="L427" t="s">
         <v>755</v>
@@ -27200,17 +27392,20 @@
       <c r="G428">
         <v>15.56905094483459</v>
       </c>
+      <c r="H428">
+        <v>13.49728724122199</v>
+      </c>
       <c r="I428" s="1">
         <f t="shared" si="48"/>
-        <v>14.789547575537835</v>
+        <v>14.574170853151861</v>
       </c>
       <c r="J428">
         <f t="shared" si="49"/>
-        <v>6.2884223936190384</v>
+        <v>5.7606842038543027</v>
       </c>
       <c r="K428" s="10">
         <f t="shared" si="50"/>
-        <v>0.42519369585180528</v>
+        <v>0.39526668528168635</v>
       </c>
       <c r="L428" t="s">
         <v>755</v>
@@ -27250,17 +27445,20 @@
       <c r="G429">
         <v>6.5515684206570874</v>
       </c>
+      <c r="H429">
+        <v>9.5703359053012793</v>
+      </c>
       <c r="I429" s="1">
         <f t="shared" si="48"/>
-        <v>8.6679809170851652</v>
+        <v>8.8183734151211848</v>
       </c>
       <c r="J429">
         <f t="shared" si="49"/>
-        <v>3.6970396564529668</v>
+        <v>3.3916330435080684</v>
       </c>
       <c r="K429" s="10">
         <f t="shared" si="50"/>
-        <v>0.42651681998582353</v>
+        <v>0.38460982358632173</v>
       </c>
       <c r="L429" t="s">
         <v>755</v>
@@ -27300,17 +27498,20 @@
       <c r="G430">
         <v>6.1917267146093984</v>
       </c>
+      <c r="H430">
+        <v>13.150755673673199</v>
+      </c>
       <c r="I430" s="1">
         <f t="shared" si="48"/>
-        <v>3.2808605316965016</v>
+        <v>4.9258430553592847</v>
       </c>
       <c r="J430">
         <f t="shared" si="49"/>
-        <v>2.3935327844153744</v>
+        <v>4.2783178361951917</v>
       </c>
       <c r="K430" s="10">
         <f t="shared" si="50"/>
-        <v>0.72954420381219365</v>
+        <v>0.86854530039084576</v>
       </c>
       <c r="L430" t="s">
         <v>755</v>
@@ -27350,17 +27551,20 @@
       <c r="G431">
         <v>37.487400250486147</v>
       </c>
+      <c r="H431">
+        <v>33.13887813629087</v>
+      </c>
       <c r="I431" s="1">
         <f t="shared" si="48"/>
-        <v>40.335160617163936</v>
+        <v>39.135780203685094</v>
       </c>
       <c r="J431">
         <f t="shared" si="49"/>
-        <v>2.3536173032201715</v>
+        <v>3.4363976617282281</v>
       </c>
       <c r="K431" s="10">
         <f t="shared" si="50"/>
-        <v>5.8351504424619297E-2</v>
+        <v>8.7807056454304463E-2</v>
       </c>
       <c r="L431" t="s">
         <v>755</v>
@@ -27400,17 +27604,20 @@
       <c r="G432">
         <v>10.73172759400577</v>
       </c>
+      <c r="H432">
+        <v>14.59753433716763</v>
+      </c>
       <c r="I432" s="1">
         <f t="shared" si="48"/>
-        <v>10.191951658395427</v>
+        <v>10.926215438190795</v>
       </c>
       <c r="J432">
         <f t="shared" si="49"/>
-        <v>1.6952378147790377</v>
+        <v>2.2562304548688181</v>
       </c>
       <c r="K432" s="10">
         <f t="shared" si="50"/>
-        <v>0.16633102977707098</v>
+        <v>0.20649697671002665</v>
       </c>
       <c r="L432" t="s">
         <v>755</v>
@@ -27450,17 +27657,20 @@
       <c r="G433">
         <v>12.55631425234025</v>
       </c>
+      <c r="H433">
+        <v>34.721740096824753</v>
+      </c>
       <c r="I433" s="1">
         <f t="shared" si="48"/>
-        <v>29.466260906058768</v>
+        <v>30.342174104519767</v>
       </c>
       <c r="J433">
         <f t="shared" si="49"/>
-        <v>9.0895015006825961</v>
+        <v>8.5255684619042604</v>
       </c>
       <c r="K433" s="10">
         <f t="shared" si="50"/>
-        <v>0.30847149319897726</v>
+        <v>0.28098080356853178</v>
       </c>
       <c r="L433" t="s">
         <v>755</v>
@@ -27500,17 +27710,20 @@
       <c r="G434">
         <v>33.285507642614803</v>
       </c>
+      <c r="H434">
+        <v>32.470278164507548</v>
+      </c>
       <c r="I434" s="1">
         <f t="shared" si="48"/>
-        <v>34.816254704484528</v>
+        <v>34.425258614488364</v>
       </c>
       <c r="J434">
         <f t="shared" si="49"/>
-        <v>3.7342786771779832</v>
+        <v>3.5192452899710527</v>
       </c>
       <c r="K434" s="10">
         <f t="shared" si="50"/>
-        <v>0.10725676006434395</v>
+        <v>0.10222857958400138</v>
       </c>
       <c r="L434" t="s">
         <v>755</v>
@@ -27550,17 +27763,20 @@
       <c r="G435">
         <v>37.872038792384991</v>
       </c>
+      <c r="H435">
+        <v>18.01319821538819</v>
+      </c>
       <c r="I435" s="1">
         <f t="shared" si="48"/>
-        <v>34.713037277939534</v>
+        <v>31.929730767514311</v>
       </c>
       <c r="J435">
         <f t="shared" si="49"/>
-        <v>7.334060164958017</v>
+        <v>9.1409886996737875</v>
       </c>
       <c r="K435" s="10">
         <f t="shared" si="50"/>
-        <v>0.21127682104668155</v>
+        <v>0.28628455298388983</v>
       </c>
       <c r="L435" t="s">
         <v>755</v>
@@ -27600,17 +27816,20 @@
       <c r="G436">
         <v>43.175302214105081</v>
       </c>
+      <c r="H436">
+        <v>45.28625246489284</v>
+      </c>
       <c r="I436" s="1">
         <f t="shared" si="48"/>
-        <v>40.861269577956435</v>
+        <v>41.598766725779171</v>
       </c>
       <c r="J436">
         <f t="shared" si="49"/>
-        <v>4.8309936503009068</v>
+        <v>4.7083181628836313</v>
       </c>
       <c r="K436" s="10">
         <f t="shared" si="50"/>
-        <v>0.11822916175142779</v>
+        <v>0.11318408052625847</v>
       </c>
       <c r="L436" t="s">
         <v>755</v>
@@ -27650,17 +27869,20 @@
       <c r="G437">
         <v>34.32390833764709</v>
       </c>
+      <c r="H437">
+        <v>38.082384829610461</v>
+      </c>
       <c r="I437" s="1">
         <f t="shared" si="48"/>
-        <v>26.095151147337397</v>
+        <v>28.093023427716236</v>
       </c>
       <c r="J437">
         <f t="shared" si="49"/>
-        <v>8.1283301376528048</v>
+        <v>8.6611543071594497</v>
       </c>
       <c r="K437" s="10">
         <f t="shared" si="50"/>
-        <v>0.31148814167654953</v>
+        <v>0.30830267626568308</v>
       </c>
       <c r="L437" t="s">
         <v>755</v>
@@ -27700,17 +27922,20 @@
       <c r="G438">
         <v>33.453642178232961</v>
       </c>
+      <c r="H438">
+        <v>36.646374587733902</v>
+      </c>
       <c r="I438" s="1">
         <f t="shared" si="48"/>
-        <v>33.296500397643385</v>
+        <v>33.854812762658469</v>
       </c>
       <c r="J438">
         <f t="shared" si="49"/>
-        <v>4.1979821513059576</v>
+        <v>4.0304394223061975</v>
       </c>
       <c r="K438" s="10">
         <f t="shared" si="50"/>
-        <v>0.12607878008714324</v>
+        <v>0.1190507078140374</v>
       </c>
       <c r="L438" t="s">
         <v>755</v>
@@ -27750,17 +27975,20 @@
       <c r="G439">
         <v>51.585144163729552</v>
       </c>
+      <c r="H439">
+        <v>50.646279081693699</v>
+      </c>
       <c r="I439" s="1">
         <f t="shared" si="48"/>
-        <v>53.01612995309695</v>
+        <v>52.621154807863071</v>
       </c>
       <c r="J439">
         <f t="shared" si="49"/>
-        <v>4.4080670381504925</v>
+        <v>4.119778230777313</v>
       </c>
       <c r="K439" s="10">
         <f t="shared" si="50"/>
-        <v>8.3145771712312508E-2</v>
+        <v>7.8291292652545572E-2</v>
       </c>
       <c r="L439" t="s">
         <v>755</v>
@@ -27800,17 +28028,20 @@
       <c r="G440">
         <v>15.42475337341793</v>
       </c>
+      <c r="H440">
+        <v>13.043129128646539</v>
+      </c>
       <c r="I440" s="1">
         <f t="shared" si="48"/>
-        <v>18.448716125586309</v>
+        <v>17.547784959429681</v>
       </c>
       <c r="J440">
         <f t="shared" si="49"/>
-        <v>5.1962263053178512</v>
+        <v>5.1535448651867526</v>
       </c>
       <c r="K440" s="10">
         <f t="shared" si="50"/>
-        <v>0.28165788177049705</v>
+        <v>0.29368634714305547</v>
       </c>
       <c r="L440" t="s">
         <v>755</v>
@@ -27850,17 +28081,20 @@
       <c r="G441">
         <v>31.218794647709629</v>
       </c>
+      <c r="H441">
+        <v>23.99068523442066</v>
+      </c>
       <c r="I441" s="1">
         <f t="shared" si="48"/>
-        <v>31.555030949905483</v>
+        <v>30.294306663991346</v>
       </c>
       <c r="J441">
         <f t="shared" si="49"/>
-        <v>2.6425308266749239</v>
+        <v>3.7102923874551883</v>
       </c>
       <c r="K441" s="10">
         <f t="shared" si="50"/>
-        <v>8.3743566307065823E-2</v>
+        <v>0.12247490687302459</v>
       </c>
       <c r="L441" t="s">
         <v>755</v>
@@ -27900,17 +28134,20 @@
       <c r="G442">
         <v>13.314998464547079</v>
       </c>
+      <c r="H442">
+        <v>32.402094267657191</v>
+      </c>
       <c r="I442" s="1">
         <f t="shared" si="48"/>
-        <v>18.156357637312937</v>
+        <v>20.530647075703644</v>
       </c>
       <c r="J442">
         <f t="shared" si="49"/>
-        <v>6.8667748557685657</v>
+        <v>8.2146261298236301</v>
       </c>
       <c r="K442" s="10">
         <f t="shared" si="50"/>
-        <v>0.37820222496921574</v>
+        <v>0.40011530564689185</v>
       </c>
       <c r="L442" t="s">
         <v>755</v>
@@ -27950,17 +28187,20 @@
       <c r="G443">
         <v>16.782900365338591</v>
       </c>
+      <c r="H443">
+        <v>31.906154485356961</v>
+      </c>
       <c r="I443" s="1">
         <f t="shared" si="48"/>
-        <v>13.202830270658193</v>
+        <v>16.320050973107989</v>
       </c>
       <c r="J443">
         <f t="shared" si="49"/>
-        <v>2.8300396881613796</v>
+        <v>7.4336797798520857</v>
       </c>
       <c r="K443" s="10">
         <f t="shared" si="50"/>
-        <v>0.21435098612536319</v>
+        <v>0.45549366188262685</v>
       </c>
       <c r="L443" t="s">
         <v>755</v>
@@ -28000,17 +28240,20 @@
       <c r="G444">
         <v>20.511404517985749</v>
       </c>
+      <c r="H444">
+        <v>19.54855879147398</v>
+      </c>
       <c r="I444" s="1">
         <f t="shared" si="48"/>
-        <v>28.386465217082236</v>
+        <v>26.913480812814196</v>
       </c>
       <c r="J444">
         <f t="shared" si="49"/>
-        <v>7.4661483209304613</v>
+        <v>7.569757211068799</v>
       </c>
       <c r="K444" s="10">
         <f t="shared" si="50"/>
-        <v>0.26301789475491044</v>
+        <v>0.28126266028973274</v>
       </c>
       <c r="L444" t="s">
         <v>755</v>
@@ -28050,17 +28293,20 @@
       <c r="G445">
         <v>18.333507510757141</v>
       </c>
+      <c r="H445">
+        <v>16.021034193423549</v>
+      </c>
       <c r="I445" s="1">
         <f t="shared" si="48"/>
-        <v>22.94654957850263</v>
+        <v>21.792297014322784</v>
       </c>
       <c r="J445">
         <f t="shared" si="49"/>
-        <v>8.9167060494212418</v>
+        <v>8.539195935180306</v>
       </c>
       <c r="K445" s="10">
         <f t="shared" si="50"/>
-        <v>0.38858591872020781</v>
+        <v>0.39184469308434988</v>
       </c>
       <c r="L445" t="s">
         <v>755</v>
@@ -28100,17 +28346,20 @@
       <c r="G446">
         <v>21.49036697591287</v>
       </c>
+      <c r="H446">
+        <v>30.76525329184765</v>
+      </c>
       <c r="I446" s="1">
         <f t="shared" si="48"/>
-        <v>22.695470940663153</v>
+        <v>24.04043466586057</v>
       </c>
       <c r="J446">
         <f t="shared" si="49"/>
-        <v>4.6337303213585823</v>
+        <v>5.1901365768525602</v>
       </c>
       <c r="K446" s="10">
         <f t="shared" si="50"/>
-        <v>0.20416982460832719</v>
+        <v>0.21589196073159977</v>
       </c>
       <c r="L446" t="s">
         <v>755</v>
@@ -28150,17 +28399,20 @@
       <c r="G447">
         <v>38.326428546047772</v>
       </c>
+      <c r="H447">
+        <v>43.90536478967676</v>
+      </c>
       <c r="I447" s="1">
         <f t="shared" si="48"/>
-        <v>39.674588982710027</v>
+        <v>40.379718283871149</v>
       </c>
       <c r="J447">
         <f t="shared" si="49"/>
-        <v>5.0660348252902327</v>
+        <v>4.8860304985394656</v>
       </c>
       <c r="K447" s="10">
         <f t="shared" si="50"/>
-        <v>0.12768966119593536</v>
+        <v>0.12100209476922207</v>
       </c>
       <c r="L447" t="s">
         <v>755</v>
@@ -28200,17 +28452,20 @@
       <c r="G448">
         <v>60.649718665570923</v>
       </c>
+      <c r="H448">
+        <v>61.348384000013823</v>
+      </c>
       <c r="I448" s="1">
         <f t="shared" si="48"/>
-        <v>59.24794204264542</v>
+        <v>59.598015702206823</v>
       </c>
       <c r="J448">
         <f t="shared" si="49"/>
-        <v>8.4257481972784145</v>
+        <v>7.7313507922102884</v>
       </c>
       <c r="K448" s="10">
         <f t="shared" si="50"/>
-        <v>0.14221166013181924</v>
+        <v>0.12972496988559987</v>
       </c>
       <c r="L448" t="s">
         <v>755</v>
@@ -28250,17 +28505,20 @@
       <c r="G449">
         <v>43.323497892013457</v>
       </c>
+      <c r="H449">
+        <v>45.094889411882953</v>
+      </c>
       <c r="I449" s="1">
         <f t="shared" si="48"/>
-        <v>42.510824321785499</v>
+        <v>42.941501836801741</v>
       </c>
       <c r="J449">
         <f t="shared" si="49"/>
-        <v>5.7789055541786327</v>
+        <v>5.362574640953687</v>
       </c>
       <c r="K449" s="10">
         <f t="shared" si="50"/>
-        <v>0.1359396258805812</v>
+        <v>0.12488092897481874</v>
       </c>
       <c r="L449" t="s">
         <v>755</v>
@@ -28300,17 +28558,20 @@
       <c r="G450">
         <v>39.618298254574157</v>
       </c>
+      <c r="H450">
+        <v>40.841156983430253</v>
+      </c>
       <c r="I450" s="1">
         <f t="shared" si="48"/>
-        <v>39.431073102354127</v>
+        <v>39.666087082533487</v>
       </c>
       <c r="J450">
         <f t="shared" si="49"/>
-        <v>4.8099631380812538</v>
+        <v>4.4222104969289582</v>
       </c>
       <c r="K450" s="10">
         <f t="shared" si="50"/>
-        <v>0.12198407904333924</v>
+        <v>0.11148592720344802</v>
       </c>
       <c r="L450" t="s">
         <v>755</v>
@@ -28350,17 +28611,20 @@
       <c r="G451">
         <v>41.423976489951208</v>
       </c>
+      <c r="H451">
+        <v>43.986371629607582</v>
+      </c>
       <c r="I451" s="1">
         <f t="shared" si="48"/>
-        <v>42.508314198269929</v>
+        <v>42.754657103492868</v>
       </c>
       <c r="J451">
         <f t="shared" si="49"/>
-        <v>4.0081657375952391</v>
+        <v>3.700169088676271</v>
       </c>
       <c r="K451" s="10">
         <f t="shared" si="50"/>
-        <v>9.4291336017234245E-2</v>
+        <v>8.6544234929064212E-2</v>
       </c>
       <c r="L451" t="s">
         <v>755</v>
@@ -28400,17 +28664,20 @@
       <c r="G452">
         <v>38.082260073484832</v>
       </c>
+      <c r="H452">
+        <v>46.790299484658227</v>
+      </c>
       <c r="I452" s="1">
         <f t="shared" si="48"/>
-        <v>40.528955944485816</v>
+        <v>41.572513201181216</v>
       </c>
       <c r="J452">
         <f t="shared" si="49"/>
-        <v>3.241697367028912</v>
+        <v>3.7685842066807145</v>
       </c>
       <c r="K452" s="10">
         <f t="shared" si="50"/>
-        <v>7.9984724291175882E-2</v>
+        <v>9.0650863190384082E-2</v>
       </c>
       <c r="L452" t="s">
         <v>755</v>
@@ -28450,17 +28717,20 @@
       <c r="G453">
         <v>38.594423165847687</v>
       </c>
+      <c r="H453">
+        <v>37.144043995045777</v>
+      </c>
       <c r="I453" s="1">
         <f t="shared" si="48"/>
-        <v>41.318952292560517</v>
+        <v>40.623134242974722</v>
       </c>
       <c r="J453">
         <f t="shared" si="49"/>
-        <v>4.082850936779348</v>
+        <v>4.0388373245213591</v>
       </c>
       <c r="K453" s="10">
         <f t="shared" si="50"/>
-        <v>9.881303155681577E-2</v>
+        <v>9.9422100233928334E-2</v>
       </c>
       <c r="L453" t="s">
         <v>755</v>
@@ -28500,17 +28770,20 @@
       <c r="G454">
         <v>78.935463673017551</v>
       </c>
+      <c r="H454">
+        <v>85.62811786783692</v>
+      </c>
       <c r="I454" s="1">
         <f t="shared" si="48"/>
-        <v>76.595963643114061</v>
+        <v>78.101322680567861</v>
       </c>
       <c r="J454">
         <f t="shared" si="49"/>
-        <v>2.4510212723956579</v>
+        <v>4.0418787161829446</v>
       </c>
       <c r="K454" s="10">
         <f t="shared" si="50"/>
-        <v>3.1999352913892137E-2</v>
+        <v>5.1751731948434611E-2</v>
       </c>
       <c r="L454" s="11" t="s">
         <v>21</v>
@@ -28550,17 +28823,20 @@
       <c r="G455">
         <v>77.583976478112632</v>
       </c>
+      <c r="H455">
+        <v>89.121264819789815</v>
+      </c>
       <c r="I455" s="1">
         <f t="shared" si="48"/>
-        <v>80.223534513332964</v>
+        <v>81.706489564409111</v>
       </c>
       <c r="J455">
         <f t="shared" si="49"/>
-        <v>4.592347228466295</v>
+        <v>5.3451369773433219</v>
       </c>
       <c r="K455" s="10">
         <f t="shared" si="50"/>
-        <v>5.7244389147464672E-2</v>
+        <v>6.5418756892373378E-2</v>
       </c>
       <c r="L455" s="11" t="s">
         <v>21</v>
@@ -28600,17 +28876,20 @@
       <c r="G456">
         <v>73.623656942667907</v>
       </c>
+      <c r="H456">
+        <v>77.931814187103072</v>
+      </c>
       <c r="I456" s="1">
         <f t="shared" si="48"/>
-        <v>75.894565301610399</v>
+        <v>76.234106782525842</v>
       </c>
       <c r="J456">
         <f t="shared" si="49"/>
-        <v>5.5206711293045156</v>
+        <v>5.0965298832890475</v>
       </c>
       <c r="K456" s="10">
         <f t="shared" si="50"/>
-        <v>7.2741323537001315E-2</v>
+        <v>6.6853670861888537E-2</v>
       </c>
       <c r="L456" s="11" t="s">
         <v>21</v>

</xml_diff>